<commit_message>
0.1: translated hero roles
translated 23,774 words
</commit_message>
<xml_diff>
--- a/tradept/Excel/Localization/english/R人物列表_Roles_Heros_hotfix.xlsx
+++ b/tradept/Excel/Localization/english/R人物列表_Roles_Heros_hotfix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\tradesp\Excel\Localization\english\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="f:\Users\isyuricunha\Documents\GitHub\sands-of-salzaar-game-translation\tradept\Excel\Localization\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A3FDFD-E52B-4167-ABE3-BF9F7B32299C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D4CBFF-2FDE-4759-B961-541C30D32A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="3" r:id="rId1"/>
@@ -2372,1696 +2372,538 @@
 Like:历史</t>
   </si>
   <si>
-    <t>喜欢的礼物: Mis necesidades son sencillas y modestas; no requiero de grandes obsequios.
-hello: El destino de Salzaar está inexorablemente ligado a mi gobierno como Nasir Sultan, ya sea por medios pacíficos o por la fuerza.
-refuse_recruit_0: Si mantengo mi valentía sin retroceder, recuperaré esta tierra y honraré el legado de mi padre.
-refuse_recruit_1: Soy el Nasir Sultan, un líder auténtico y no seguiré las órdenes de aquellos que son ajenos a nuestra tierra.
-refuse_recruit_2: ¿Cómo te atreves a formulare una pregunta tan insensata y carente de sentido?
-refuse_recruit_3: ¡Nunca cometería tal acto que vaya en contra de mis principios y deberes!
-recruit_msg: Aunque ya no ostento el título de Nasir Sultan, valoro tu apoyo y dedicación hacia mí. Te seguiré con lealtad.
-enemy_hello: Mantente alejado. Mi lanza es infalible y no errará su objetivo.
-be_attack: Hoy te has convertido en un enemigo del Nasir. Prepárate para enfrentar las consecuencias de tus actos.
-be_attack_enemy: Un pequeño pájaro osa desafiar al majestuoso águila al picotear sus alas.</t>
-  </si>
-  <si>
-    <t>Husnu es el legítimo heredero del trono del Nasir. Aunque el antiguo rey Nasir aún gobierna sobre Jamal City, ha designado a Husnu como sultán interino. Husnu es un hombre de paz, pero se debate internamente, pues teme perder todo lo que aprecia en medio de las tensiones y conflictos.
-Nature:kind=4,severe=6,honest=7,cunning=3,calm=8,anger=2,strong=5,weak=5
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能霍驹</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Tratas de ganarme? ¡Jajaja! ¡Imposible!
-hello: ¡Pocos se atreverían a desafiarme en las majestuosas Montañas Zagros! Mi nombre es Ruha, la guardiana de estas tierras sagradas y la defensora de su pueblo.
-refuse_recruit_0: Si me uno a ti, ¿quién protegerá al valiente pueblo de las montañas? Durante generaciones, he velado por su seguridad y bienestar.
-refuse_recruit_1: Gracias, pero con el apoyo y la lealtad del pueblo de las montañas, aún puedo superar cualquier desafío que se presente en mi camino.
-refuse_recruit_2: ¿Por qué me haces esa pregunta? Mi lealtad y compromiso están con mi gente y estas tierras ancestrales.
-refuse_recruit_3: ¡No te sobrevalores! Las montañas me han forjado en una guerrera temible y no permitiré que nadie subestime mi fuerza.
-recruit_msg: Tú, con tu promesa de asegurar la seguridad y el bienestar del pueblo de las montañas, has logrado ganarte mi respeto. Ruha dejará de lado las bromas y se unirá a tu causa.
-enemy_hello: ¿Por qué estás aquí? Estas montañas son mi hogar y protegeré sus secretos y su gente con mi vida.
-be_attack: Si deseas presenciar de primera mano la furia de las montañas, prepárate para enfrentar mi habilidad en el combate. ¡No te decepcionaré!
-be_attack_enemy: ¡Ven! ¡Te mostraré la destreza y la fiereza que emana de estas majestuosas montañas!</t>
-  </si>
-  <si>
-    <t>Desc:Ruha es la líder de los Dhib. Los Dhib viven en las remotas Montañas Zagros. Los Dhib son un pueblo valiente y listo para la batalla, y Ruha no es una excepción. Ama el combate con espadas, aunque puede verse envuelta en una furia desenfrenada debido a la locura de la batalla. Ruha detesta a los magos y desconfía de sus trucos.
-Ruha, una guerrera formidable y apasionada por el arte de la espada, lidera con valentía a los Dhib en las inhóspitas Montañas Zagros. Su habilidad en el combate con espadas es legendaria, y su destreza con la hoja ha sido forjada a través de innumerables batallas y desafíos. Ruha personifica el espíritu intrépido y audaz de su pueblo, siempre dispuesta a enfrentarse a cualquier adversario que amenace su territorio sagrado.
-Nature:kind=6,severe=4,honest=8,cunning=2,calm=2,anger=8,strong=7,weak=3
-fight_skills:升龙拳|吼叫|饮酒|飞腿
-fight_dgskill:刺拳,1
-AssSkill:统率技能封凛</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Agradecemos tu amabilidad, pero en este momento no requerimos ningún obsequio. Nuestra historia está entrelazada con el legado del Viejo Imperio, y nosotros somos los dignos herederos y el legítimo rey de Salzaar.
-refuse_recruit_0：También buscamos a Ilayda, pero lamentablemente no podemos aceptar. Nuestra lealtad y compromiso son inquebrantables, y solo seguimos las órdenes y designios de Ilayda.
-refuse_recruit_1：Nuestros movimientos están determinados exclusivamente por las órdenes de Ilayda. Solo nos movemos cuando ella así lo dispone.
-refuse_recruit_2：Incluso si estuviéramos involucrados en asuntos similares, no nos uniríamos a tu causa. Nuestra lealtad está arraigada en Ilayda y a seguir nuestros propios caminos.
-refuse_recruit_3：No te sorprendas si nuestra espada acaba contigo por esta insolencia. No toleramos la falta de respeto hacia nuestra causa y nuestra líder.
-recruit_msg：Si Ilayda estuviera presente, ella desearía que nos unamos a ti. Nuestra espada está a tu disposición, ya que su voluntad es nuestra guía.
-enemy_hello：Si te opones a nosotros, te enfrentas al heredero del desierto. Nuestra autoridad y poderío representan la herencia de las arenas áridas. ¿Entendido?
-be_attack：Entonces, permitamos que nuestros caminos se crucen en duelo. Demostremos quién posee la verdadera fuerza.
-be_attack_enemy：¡Caerás ante nuestro poderío indomable! No subestimes nuestra determinación y habilidades de combate.</t>
-  </si>
-  <si>
-    <t>Desc: Bahat es el líder de los Akhal, un antiguo clan guerrero que solía ser leal a los Nephrit del Viejo Imperio. Durante siglos, los Akhal sirvieron como defensores y protectores del imperio, comprometidos con su deber y tradiciones ancestrales. Sin embargo, cuando estalló la guerra y el Viejo Imperio se sumió en el caos, los Akhal perdieron la esperanza de restaurar su antiguo esplendor.
-En medio del desaliento y la desilusión, los Akhal buscaron un nuevo líder capaz de guiarlos hacia un nuevo destino. Bahat emergió como una figura carismática y valiente, con una herencia que lo conectaba directamente con el antiguo rey Nephrit. Su padre, un leal consejero y confidente del rey, había asegurado un compromiso matrimonial con la princesa Ilayda, una joven de gran belleza y sabiduría.
-Sin embargo, la tragedia golpeó a Bahat y a los Akhal cuando la Ciudad de Jamal cayó en manos del enemigo. Durante el caos y la confusión, la princesa Ilayda desapareció misteriosamente, sumiendo a Bahat en un profundo pesar y determinación. Desde entonces, ha dedicado su vida a buscar a Ilayda, la mujer que debería haber sido su prometida, pero a quien nunca ha conocido en persona.
-Nature:kind=5,severe=5,honest=7,cunning=3,calm=1,anger=9,strong=8,weak=2
-fight_skills:冲刺膝盖顶|冲刺重拳|饮酒|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能苍骐</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Oh! Este anciano ya ha vivido bastante. Solo deseo tener una buena noche de sueño... y nada más.
-hello: Los Acantilados de Umbra son un lugar agradable. Ven y ve cuando quieras, sin restricciones.
-refuse_recruit_0: ¡Admiro tus logros a tan temprana edad! Pero aún no es suficiente para convencer a este viejo.
-refuse_recruit_1: No tienes lo necesario para ganarte a este veterano.
-refuse_recruit_2: Posees cierta habilidad, pero no lo suficiente como para impresionarme.
-refuse_recruit_3: ¡Desperdicio de tiempo! ¡Vete!
-recruit_msg: Soy un anciano que no ha servido a otro durante mucho tiempo. ¡Tú podrías ser el primero!
-enemy_hello: Piensa dos veces antes de actuar de forma imprudente.
-be_attack: ¡Aún tengo energía para enseñarte una lección, jovenzuelo!
-be_attack_enemy: ¡Prepárate para ser aplastado bajo mis pies!</t>
-  </si>
-  <si>
-    <t>Desc:Ludo Khan lidera a los Thur, una tribu ancestral que ha resistido el paso del tiempo y las dificultades en un bosque pantanoso infestado de peligros. Conocido como el más anciano entre los cinco líderes tribales, Ludo Khan encarna la sabiduría acumulada a lo largo de los años y es venerado por su experiencia y conocimiento.
-Gracias a Ludo Khan los Thur se establecieron en el corazón del bosque, un lugar marcado por el sufrimiento y la lucha. La tierra en la que residen ha sido testigo de innumerables conflictos y batallas, y ha sido bañada en las llamas de la guerra. A pesar de enfrentar la adversidad y la pobreza, los Thur han mantenido su espíritu indomable y se han convertido en una de las tribus más resistentes y fuertes de la región.
-Ludo Khan, a pesar de su avanzada edad, continúa siendo una figura respetada y reverenciada entre los Thur. Se dice que su sabiduría ancestral es un faro de guía para su pueblo, y que su estrategia meticulosa ha asegurado la supervivencia y el crecimiento de la tribu. Detrás de su fachada de anciano tranquilo y amante de la siesta, se esconde un líder astuto y visionario, cuyo deseo de ver prosperar a su pueblo es inquebrantable. Los Thur encuentran en él una fuente de inspiración y confianza, sabiendo que su líder siempre estará allí para proteger y velar por su bienestar en este mundo hostil.
-Nature:kind=7,severe=3,honest=4,cunning=6,calm=7,anger=3,strong=7,weak=3
-fight_skills:冲刺膝盖顶|冲刺重拳|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能汗卢达</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Oh, simplemente amo las estrellas en el cielo! ¿Podrías traerme una? Sin embargo, mi verdadero deseo es conquistar el mundo entero y verlo sometido a mi dominio implacable.
-hello: ¿Qué es lo que deseas? Veo ambición y determinación en tus ojos.
-refuse_recruit_0: Debo ocuparme de mi hermano mayor, Hassan. Su bienestar es mi prioridad. Te pido disculpas por no poder unirme a ti en este momento.
-refuse_recruit_1: ¡Eres tan inocente~! ¿No te da miedo que yo, te envenene en secreto? Es mejor que sigas tu camino sin mí.
-refuse_recruit_2: Realmente tienes mucha audacia al pensar que puedo unirme a tu causa. Mi ambición es mucho más grande y mis planes más intrincados.
-refuse_recruit_3: ¡Te odio! No hay nada en ti que me impresione o me haga cambiar de opinión. Puedes irte ahora, antes de que te arrepientas.
-recruit_msg: Si acepto unirme a ti, debes entender que mi hermano Hassan y yo merecemos un trato privilegiado. Asegúrate de que nuestras necesidades sean satisfechas y nuestro poder reconocido.
-enemy_hello: Los escorpiones son más peligrosos a corta distancia. Y yo soy como un escorpión letal, listo para atacar sin piedad.
-be_attack: Oh, disfrutaré torturándote lentamente, viendo cómo tu resistencia se desvanece mientras te someto a mi voluntad.
-be_attack_enemy: Oh, esto no será rápido, ¡jejeje! Prepárate para sufrir y para ser testigo de mi implacable sed de poder.</t>
-  </si>
-  <si>
-    <t>Desc: Rebiya es la líder de los Dakn, una tribu clandestina y temida compuesta por hábiles asesinos. Al principio, los Dakn eran una pequeña organización en las sombras, pero se fortalecieron durante la guerra. La sangre asesina corre por sus venas, y Rebiya fue entrenada por los suyos desde una edad temprana en el arte de la muerte sigilosa.
-El hermano mayor de Rebiya fue reconocido como general por el Viejo Rey, lo que otorgó a los Dakn cierto estatus en el conflicto. En la batalla de la Ciudad de Jamal, Rebiya se unió a Husnu en una audaz ofensiva para conquistar a los Nephrit. Sin embargo, cuando llegó el momento de dividir el territorio conquistado, la alianza entre los Dakn y Nasir se rompió, sumiendo al hermano de Rebiya al borde de la muerte. Fue en ese momento de crisis que Rebiya, con su calma inquebrantable, astucia viciosa y sutileza letal, asumió su lugar como la única líder femenina de las cinco tribus, destacándose por su habilidad distintiva en el uso de venenos mortales.
-Rebiya se convirtió en la encarnación misma de los Dakn, utilizando su inteligencia y estrategia para guiar a su tribu hacia una posición de poder y respeto en el mundo peligroso que los rodea. Además de sus habilidades de asesinato sin igual, Rebiya es reconocida por su dominio en el arte de los venenos, capaz de manipular y utilizar sustancias mortales con precisión mortal.Como líder femenina en un mundo dominado por hombres y rodeada de asesinos letales, Rebiya ha desafiado las expectativas y ha demostrado ser una fuerza a tener en cuenta. Su presencia inspira temor y respeto, y su determinación inquebrantable ha llevado a los Dakn a superar obstáculos y a luchar con astucia y fiereza por su causa.A pesar de su apariencia calmada, Rebiya es conocida por su ferocidad y su habilidad para utilizar la sutileza y la astucia para lograr sus objetivos.
-Nature:kind=3,severe=7,honest=1,cunning=9,calm=8,anger=2,strong=4,weak=6
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能阿曼莎</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me he cansado de la búsqueda de Utar. Si quieres ser mi amigo, intenta conquistarme con una buena &lt;color=red&gt;historia&lt;/color&gt;.
-hello: Los problemas de los ricos están más allá de tu imaginación, desafortunadamente.
-refuse_recruit_0: No necesitas mirarme así, sé lo que estás pensando, y la respuesta es: ¡de ninguna manera!
-recruit_msg: Parece que hay algunos placeres que el dinero no puede comprar, ¡jajaja! Me has ganado con tu ingeniosa historia.
-enemy_hello: Únete a mí, y habrá una recompensa de Utar para ti.
-be_attack: ¡Tonto! Eres igual que el Fuego Salvaje, un mero juguete para mí.
-be_attack_enemy: Ven, déjame ver cómo luchan las personas comunes. Preparémonos para un duelo de verdad.</t>
-  </si>
-  <si>
-    <t>Desc: Gizeh, conocido en el pasado como uno de los mercaderes más prósperos del desierto, oculta celosamente su verdadera historia. Aunque todos en la región son conscientes de que desempeñó un papel crucial en la captura del infame bandido Hashim, su pasado y sus motivaciones permanecen envueltos en misterio.
-Aunque Gizeh actualmente trabaja bajo la bandera de los Akhal, su lealtad no es fácil de definir. A pesar de su compromiso aparente con la tribu, Gizeh sigue siendo un alguien independiente que se guía por sus propios intereses y objetivos. Nadie sabe con certeza cuáles son sus verdaderas intenciones y cuánto tiempo permanecerá al servicio de los Akhal.
-Con una astucia innata y una perspicacia comercial sin igual, Gizeh posee un conocimiento profundo de los secretos y las dinámicas de la región. Su habilidad para mantener su pasado en secreto y su capacidad para negociar con maestría lo han convertido en una figura intrigante y respetada en el desierto. Los rumores sobre sus riquezas y conexiones ocultas circulan entre los comerciantes y líderes tribales, alimentando aún más el misterio que lo rodea.
-Like:文学|故事
-Nature:kind=3,severe=7,honest=1,cunning=9,calm=7,anger=3,strong=5,weak=5
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能格罗瓦兹</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Oh! ¿Por qué no comparamos nuestros &lt;color=red&gt;objetos de combate&lt;/color&gt;?
-hello: Cuando la espada descansa, su verdadero significado se revela. Detrás de cada arma hay una historia de honor y habilidad.
-refuse_recruit_0: Solo hay un alfa en la manada. Si la manada debe rendirse ante ti, primero debes desafiar y vencer al actual líder. La jerarquía se respeta en nuestra tradición.
-recruit_msg: ¡Has demostrado ser un líder formidable! Tu destreza en el combate y tu visión estratégica me han convencido de unirme a tu causa.
-enemy_hello: Si deseas desafiarme, deberás respaldar tus palabras con acciones. No tolero las palabras vacías y solo la fuerza del combate revelará quién es verdaderamente digno.
-be_attack: Que esta batalla sea un testamento de nuestras habilidades y una prueba de nuestra valía. No te subestimes, pues no te daré un combate fácil.
-be_attack_enemy: ¡Somete a mi espada, insensato! No te engañes con falsas esperanzas, pues mi destreza en el combate supera con creces la tuya. Prepárate para enfrentar tu destino.</t>
-  </si>
-  <si>
-    <t>Desc:Yusuf comenzó como aprendiz del gran Maestro de la Espada. En algún momento fue adversario de Ruha, pero dejó atrás su odio y apoyó a Ruha como la nueva líder de los Dhib cuando presenció cómo ella resistía a los invasores extranjeros.
-Impresionado por la valentía y determinación de Ruha, Yusuf reconoció su fuerza y cualidades de liderazgo. Vio en ella a una verdadera guerrera que luchaba no solo por sí misma, sino por la liberación y protección de su pueblo. Al presenciar el espíritu inquebrantable de Ruha frente a la adversidad, Yusuf dejó atrás sus resentimientos pasados y abrazó un nuevo camino de unidad y propósito compartido.
-Mientras Yusuf continuaba su entrenamiento bajo la guía del Maestro de la Espada, no solo perfeccionó sus habilidades con la espada, sino que también cultivó un profundo respeto por la visión y los valores de Ruha. Juntos, forjaron un fuerte vínculo basado en la confianza y un compromiso compartido con la prosperidad y la independencia de la tribu Dhib.
-Like:格斗
-Nature:kind=5,severe=5,honest=6,cunning=4,calm=2,anger=8,strong=7,weak=3
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能武</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Mi pasión es investigar lo &lt;color=red&gt;oculto&lt;/color&gt;. Nada más me intriga tanto como los misterios y secretos que yacen más allá de nuestra comprensión.
-hello: Hay dos tipos de personas que desprecio: los arrogantes que se creen superiores y los ingenuos que se dejan engañar por la ignorancia.
-refuse_recruit_0: No me ofreces nada que ya no haya encontrado en mis investigaciones. Busco conocimientos y verdades más allá de lo común.
-recruit_msg: En mis inquietantes estudios he descubierto tesoros de sabiduría oculta. Si eres capaz de apreciar y valorar ese conocimiento, entonces podemos entablar una relación provechosa.
-enemy_hello: Me pregunto cuánto estarías dispuesto a sacrificar por desentrañar los secretos que protejo.
-be_attack: He previsto este enfrentamiento y mis habilidades ocultas te sorprenderán.
-be_attack_enemy: Deberías discutir tu rescate conmigo de antemano, jeje.</t>
-  </si>
-  <si>
-    <t>Desc:En su vida anterior, Behrouz trabajaba junto a Gizeh, uno de los mercaderes más ricos del Desierto de Docana Occidental. Fue nombrado noble honorario de los Thur cuando vendió información detallada sobre una inminente invasión a la tierra natal de los Thur, los Acantilados de Umbra, a su líder, Ludo Khan.
-Behrouz, hábil en el arte del espionaje y la recopilación de información, era un colaborador cercano de Gizeh. Durante su asociación, se infiltró en los círculos más exclusivos y obtuvo conocimientos valiosos sobre los planes y movimientos de diferentes facciones en el desierto. Sin embargo, un acontecimiento trascendental cambió el rumbo de su vida.
-Cuando Behrouz descubrió los planes de invasión que amenazaban a los Thur y su tierra sagrada, tomó la audaz decisión de poner fin a su relación con Gizeh y compartir dicha información con Ludo Khan, el líder de los Thur. Su valentía y lealtad hacia la causa de los Thur le valieron el reconocimiento y la distinción de convertirse en un noble honorario.
-Desde aquel momento, Behrouz se convirtió en un aliado valioso para los Thur, utilizando sus habilidades de inteligencia y su conocimiento estratégico para proteger a los Thurianos y defender su hogar de las amenazas externas. Su experiencia previa en el mundo de la riqueza y el comercio le ha proporcionado una perspectiva única y una red de contactos que utiliza en beneficio de los Thur.
-Like:神秘
-Nature:kind=5,severe=5,honest=2,cunning=8,calm=6,anger=4,strong=5,weak=5
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能安纳西尔</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Siempre me interesa echar un vistazo a tus &lt;color=red&gt;artesanías&lt;/color&gt;, son una expresión única de creatividad.
-hello: Mis ojos de águila no se pierden ningún detalle.
-refuse_recruit_0: Eres alguien común y corriente, ¿por qué debería brindarte mi apoyo?
-recruit_msg: Ayudarte es mi mejor opción en este momento. Juntos podemos lograr grandes cosas.
-enemy_hello: ¿Qué te ha llevado a buscarme? Espero que tengas una buena razón.
-be_attack: Atacar de manera imprudente, confiando únicamente en tus habilidades sin estrategia, es un camino seguro hacia la derrota.
-be_attack_enemy: ¡Te has sobrevalorado! Tu confianza ciega en tus habilidades no será suficiente para enfrentarme.</t>
-  </si>
-  <si>
-    <t>Desc:Zaerur es el primo mayor de Husnu, líder de los Nasir. Acompañó a Husnu y su ejército a Redstone Keep para desempeñar el papel de consejero.
-Zaerur, con su experiencia y sabiduría, ha sido un apoyo crucial para Husnu en su liderazgo. Como consejero de confianza, ha compartido su conocimiento estratégico y su perspicacia para ayudar a tomar decisiones importantes en beneficio de los Nasir.
-Su vínculo familiar fortalece aún más su conexión y comprensión mutua. Zaerur ha estado presente durante el ascenso de Husnu al liderazgo de los Nasir y ha sido testigo de su valentía y habilidades en la batalla. Juntos, han enfrentado desafíos y han forjado un lazo inseparable mientras luchan por proteger y fortalecer a su tribu.
-En Redstone Keep, Zaerur desempeña un papel fundamental como consejero estratégico, aportando su perspectiva y experiencia para ayudar a Husnu a tomar decisiones informadas. Su presencia tranquilizadora y su capacidad para ver más allá de lo evidente han sido de gran valor para el éxito y la supervivencia de los Nasir.
-Like:工艺
-Nature:kind=4,severe=6,honest=6,cunning=4,calm=8,anger=2,strong=7,weak=3
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能霍桑</t>
-  </si>
-  <si>
-    <t>Desc:Esfir, una vez miembro importante de la Pandilla Wildfire y considerada como una querida hermana para Wildfire. Cuando Wildfire fue asesinado y la organización se desintegró, Esfir se cansó de las interminables luchas internas entre Rabia e Ishtar. Decidió unirse a los Thur con algunos de sus subordinados y su experiencia en logística. Ahora, ya no era ingenua y en secreto había estado tratando de encontrar al responsable de la exterminación de la Pandilla Wildfire.
-Esfir, con su experiencia y conocimientos estratégicos, se convirtió en un valioso activo para los Thur. Su liderazgo y habilidades logísticas fueron fundamentales para la organización y eficiencia de las operaciones de los Thur. Sin embargo, en su interior, ardía una sed de venganza y justicia por la caída de la Pandilla Wildfire.
-Mientras trabajaba en las filas de los Thur, Esfir utilizaba su posición y recursos para investigar en secreto y descubrir la verdad detrás del asesinato de Wildfire y la destrucción de su pandilla. Era una cazadora sigilosa, siempre un paso por delante de sus enemigos, buscando pistas y rastros que la llevaran al responsable final.
-Aunque los Thur eran su nueva familia y su prioridad era servir a su líder, Ludo Khan, Esfir no podía olvidar su pasado y su lealtad hacia la Pandilla Wildfire. Encontrar al responsable y hacer que pagara por sus acciones se convirtió en una obsesión que impulsaba su determinación y motivación.
-Like:装饰|忧伤
-Nature:kind=7,severe=3,honest=8,cunning=2,calm=4,anger=6,strong=4,weak=6
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能叶斯菲</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Cuando era una niña, mis hermanos de Wildfire me regalaron muchos &lt;color=red&gt;juegos&lt;/color&gt;. Aunque ahora soy adulta, esos objetos me evocan recuerdos de tiempos más felices. Sin embargo, también las cosas &lt;color=red&gt;tristes&lt;/color&gt;  me recuerdan mi misión actual: ¡vengarme!
-hello: Mientras yo esté aquí, el fuego arderá sin cesar, iluminando el camino hacia la justicia.
-refuse_recruit_0: Tengo una misión mucho más importante que la búsqueda de conquistas y riquezas mundanas.
-recruit_msg: Prométeme que juntos encontraremos a aquellos responsables de dañar a Wildfire y los haremos pagar por sus acciones.
-enemy_hello: ¡Qué astuto/a eres al acechar como una sombra! Pero no podrás esconderte por mucho tiempo de mi fuego ardiente.
-be_attack: ¡Villano/a, no recibirás misericordia de mi parte! Mi ira se enciende como un torrente de fuego incontrolable.
-be_attack_enemy: Estaba preparada para este enfrentamiento. Mi determinación y ferocidad superan todas las expectativas. Prepárate para enfrentar las llamas de mi venganza.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Aunque mi entusiasmo por las manualidades ha disminuido, aún aprecio los &lt;color=red&gt;artículos artesanales&lt;/color&gt;. Además, los objetos relacionados con la &lt;color=red&gt;lucha&lt;/color&gt; son de gran utilidad para mí.
-hello: ¡No bajes la guardia! ¿No podrías esforzarte un poco más y mostrar una sonrisa?
-refuse_recruit_0: He trabajado arduamente para conseguir todo lo que tengo. No estoy dispuesto/a a renunciar a ello sin más.
-recruit_msg: Espero poder aportar mi granito de arena a la causa.
-enemy_hello: Más allá de mi posición de nacimiento, puedes confiar en mí en cualquier circunstancia.
-be_attack: ¡Empuña tu arma y prepárate para el combate!
-be_attack_enemy: ¡Serás una insignificancia junto al monumento de mi gloria!</t>
-  </si>
-  <si>
-    <t>Desc:Latif vive una vida ordinaria. Era un residente común de la Ciudad de Jamal que fue reclutado en el ejército debido a la guerra. Comenzó como soldado de a pie y escaló lentamente hacia arriba. Ahora se ha convertido en un general incomparable, sirviendo al gran líder de las Montañas Zagros.
-A Latif le gustan las actividades de &lt;color=red&gt;combate&lt;/color&gt; y las &lt;color=red&gt;artesanías&lt;/color&gt;. Disfruta participar en luchas y desafíos físicos, mostrando su destreza y habilidad marcial. Además, tiene un interés por las habilidades artesanales y aprecia la belleza y el valor de los objetos hechos a mano.
-A pesar de su ascenso en el ejército y su posición como general destacado, Latif nunca olvida sus raíces y la vida ordinaria que llevaba antes de la guerra. Mantiene su humildad y se esfuerza por proteger y servir a su gente en las Montañas Zagros. Su experiencia como soldado de base le ha proporcionado una comprensión profunda de los desafíos y dificultades que enfrentan sus compañeros de armas, y se esfuerza por ser un líder compasivo y valiente.
-Like:格斗|工艺
-Nature:kind=6,severe=4,honest=5,cunning=5,calm=5,anger=5,strong=9,weak=1
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:重拳,1
-AssSkill:统率技能洛尔</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Las &lt;color=red&gt;pinturas&lt;/color&gt; exquisitas siempre traen color y alegría a mi vida, como un lienzo que cobra vida.
-hello: ¡En busca de la presa!
-refuse_recruit_0: Un cazador noble prefiere la soledad en su caza.
-recruit_msg: Eres un hábil cazador y un líder digno. Te seguiré con lealtad.
-enemy_hello: Eres mi presa. No hay miedo en mi corazón.
-be_attack: Ven, te aseguro que no apuntaré a tus órganos vitales. Permíteme enseñarte una lección.
-be_attack_enemy: La presa se rebela contra su cazador. Observemos cómo se desarrolla este enfrentamiento.</t>
-  </si>
-  <si>
-    <t>Desc:Una mujer de noble linaje perteneciente a la tribu Dhib, reconocida no solo por su posición de nobleza, sino también por ser la cazadora más talentosa de su pueblo. Además de su destreza en la caza, tiene un profundo amor por el arte de la pintura.
-Desde una edad temprana, demostró una afinidad natural por el arte de la caza, perfeccionando sus habilidades con arco y flecha, rastreo y conocimiento de la fauna local. Su destreza y precisión en la caza le han valido el respeto y la admiración de su tribu, convirtiéndola en una figura icónica de valor y sabiduría.
-Como noble mujer de los Dhib, lleva consigo la responsabilidad de proteger y mantener el equilibrio en su tierra ancestral. Su profundo conocimiento de la naturaleza y su conexión espiritual con las criaturas salvajes le permiten desempeñar un papel vital en la supervivencia y prosperidad de su tribu.
-Más allá de su destreza como cazadora, también es una líder respetada dentro de la comunidad Dhib.
-Like:绘画
-Nature:kind=7,severe=3,honest=5,cunning=5,calm=6,anger=4,strong=6,weak=4
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能热丽莎</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me apasiona la investigación de lo &lt;color=red&gt;oculto&lt;/color&gt;. Nada me intriga más que descubrir los misterios que se ocultan en las sombras.
-hello: ¿Necesitas ayuda? Estoy dispuesta a ofrecer mi experiencia en los asuntos ocultos.
-refuse_recruit_0: Lamento decirte que en este momento no estoy interesada en asumir ninguna responsabilidad adicional.
-recruit_msg: Si puedes proporcionarme un ambiente propicio para continuar mis investigaciones en el ámbito oculto, consideraré unirme a ti. Necesito más que lo que Husnu pueda ofrecerme.
-enemy_hello: Ah, un/a curioso/a como tú. Ten cuidado con lo que buscas, podría desvelar verdades que preferirías no conocer.
-be_attack: ¿Crees que puedes hacerme retroceder con ataques simples? 
-be_attack_enemy: ¿Crees que los mercenarios son supersticiosos y cobardes? Te lo demostraré.</t>
-  </si>
-  <si>
-    <t>Desc:Janub, una guerrera feroz y habilidosa, comenzó su viaje como mercenaria, vendiendo su espada al mejor postor. Con su destreza excepcional en combate y su mente estratégica, rápidamente se ganó la reputación de ser una de las luchadoras más formidables de la región. Durante su empleo con la tribu Nasir, demostró su valía al derrotar en solitario a un grupo de la Caballería Akhal, exhibiendo su habilidad y valentía incomparables.
-Impresionados por su destacada hazaña, los Nasir reconocieron las habilidades excepcionales de Janub y le concedieron la membresía formal dentro de su tribu. Se convirtió en una figura respetada y admirada, admirada por su destreza en combate y su tenacidad indomable. Janub se ha convertido en una aliada confiable y una fuerza a tener en cuenta en el campo de batalla. Su pasado como mercenaria habla de su resistencia y adaptabilidad, demostrando que puede enfrentar cualquier desafío con determinación y habilidad.
-Like:神秘
-Nature:kind=7,severe=3,honest=6,cunning=4,calm=6,anger=4,strong=8,weak=2
-fight_skills:升龙拳|吼叫|饮酒|飞腿
-fight_dgskill:刺拳,1
-AssSkill:统率技能雅南</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me apasiona coleccionar &lt;color=red&gt;equipamiento especial&lt;/color&gt;. También disfruto de los &lt;color=red&gt;artículos artesanales&lt;/color&gt;. ¿Hmm? ¿Tienes algún regalo para mí?
-hello: ¡Soy yo! Aquí estoy.
-refuse_recruit_0: El último líder en quien no pude confiar se convirtió en mi enemigo. No estoy dispuesto a cometer el mismo error nuevamente.
-recruit_msg: El valor del oro nunca se transformará en madera o piedra. Agradezco tu aprecio y consideración.
-enemy_hello: ¿Hm, será que Bahat está tramando algo en las sombras?
-be_attack: ¡Preparen las lanzas! Es hora de luchar.
-be_attack_enemy: ¡Te demostraré que eres digno/a de vergüenza!</t>
-  </si>
-  <si>
-    <t>Like:工艺|特殊装备
-Robber:100
-WildMonsterKiller:1
-Desc:Mhan Hassan es nativo de los Akhal, pero su familia tiene una relación tumultuosa con el Sultán de los Akhal. Después de un conflicto público con el Sultán de los Akhal, fue desterrado de la tribu. Esto le dio la oportunidad de luchar junto a Bahat y unirse a los Nasir.
-El exilio de Mhan Hassan de los Akhal no solo marcó un quiebre en su relación con su tribu de origen, sino que también despertó en él un sentido de determinación y sed de venganza. Con su experiencia y habilidades de combate, se convirtió en un valioso aliado para Bahat y un fuerte defensor de la causa de los Nasir. Mhan Hassan encontró en su unión con los Nasir una nueva familia y una oportunidad de redención, prometiendo utilizar su destreza y conocimiento para enfrentar a aquellos que alguna vez lo rechazaron. Su lealtad hacia Bahat y su deseo de justicia lo impulsan a luchar incansablemente en busca de la revancha que tanto anhela.
-Voice:NpcVoice.huyanmu
-BattleVoice:BattleVoice.huyanmu
-Nature:kind=5,severe=5,honest=7,cunning=3,calm=1,anger=9,strong=9,weak=1
-fight_skills:升龙拳|吼叫|饮酒|飞腿
-fight_dgskill:刺拳,1
-AssSkill:统率技能呼延牧</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Oh! ¿Por qué no comparamos nuestros &lt;color=red&gt;artículos de combate&lt;/color&gt;?
-hello: Las cicatrices no solo son testimonio del dolor, también cuentan historias de valentía y resistencia.
-refuse_recruit_0: Te admiro, pero eso no significa que me rendiré ante ti. Aún tengo mis propias metas y objetivos.
-recruit_msg: ¡Permíteme liderar el camino y juntos alcanzaremos la victoria!
-enemy_hello: Si tienes algo que decirme, no tengas miedo de enfrentarme cara a cara.
-be_attack: ¡Observa cómo mi espada responde a este desafío!
-be_attack_enemy: ¡Ven, entonces! ¡Enfrentémoslo con toda nuestra determinación!</t>
-  </si>
-  <si>
-    <t>Desc:Yakub desempeña el papel de uno de los Generales de Bahat, el Sultán de los Akhal. La cicatriz en su rostro es tan famosa como su legendaria destreza en el manejo de la espada. Con una mirada imponente y una presencia magnética, Yakub encarna la ferocidad y el coraje de un verdadero líder guerrero.
-La cicatriz que adorna su rostro es un testimonio vivo de las numerosas batallas que ha librado y los desafíos que ha superado. Es un símbolo de su dedicación inquebrantable y su incansable determinación en la protección y defensa de la tribu Akhal. Su habilidad en el combate con la espada es legendaria, y su mera presencia en el campo de batalla infunde temor en el corazón de sus enemigos.
-WildMonsterKiller:1
-Like:格斗
-Nature:kind=4,severe=6,honest=5,cunning=5,calm=3,anger=7,strong=7,weak=3
-fight_skills:升龙拳|吼叫|饮酒|飞腿
-fight_dgskill:刺拳,1
-AssSkill:统率技能尉迟疤</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Sabes, no puedes complacer a todo el mundo. Aparte de los estudios &lt;color=red&gt;ocultos&lt;/color&gt;, hay pocos objetos adecuados para una sacerdotisa como yo.
-hello: Las llamas dan origen a los fénix, ¡pero también a mi pequeño! El fuego es mi aliado y protector.
-refuse_recruit_0: ¿Por qué debería escucharte? Prefiero confiar en mi fiel escorpión, él nunca me falla.
-recruit_msg: A partir de ahora, mis leales escorpiones estarán a tu servicio. Juntos, llevaremos nuestra fuerza a nuevas alturas.
-enemy_hello: Eres un sacrificio adecuado para alimentar el fuego. No subestimes el poder que poseo.
-be_attack: Pronto verás la perfección de mi arte, y te arrepentirás de enfrentarme.
-be_attack_enemy: ¡Te invoco, oh mi pequeño! Que mi enemigo conozca el ardor de mi ira.</t>
-  </si>
-  <si>
-    <t>Desc:Ursula, durante los días del Viejo Imperio, era una acólita en la Ciudad de Cotta. Después de que la Ciudad de Cotta fuera anexada por los Dakn, Ursula aceptó de buena gana las tradiciones de criar escorpiones de los Dakn. Presidía los sacrificios ante las llamas durante el día, pero llevaba a cabo experimentos secretos por la noche. Después de innumerables fracasos, finalmente logró criar una criatura que la satisfacía: un escorpión que crece junto a la llama sagrada y no teme a las altas temperaturas.
-Ursula, durante los días del Viejo Imperio, llevaba una vida humilde como acólita en la Ciudad de Cotta. Sin embargo, cuando los Dakn anexaron la ciudad, Ursula abrazó sus tradiciones de criar escorpiones con los brazos abiertos. Durante el día, presidía con devoción los sacrificios sagrados ante las llamas, pero era durante la oscuridad de la noche cuando sus verdaderas ambiciones salían a la luz.
-Impulsada por una búsqueda incansable de conocimiento y experimentación, Ursula se adentró en los secretos de la cría de escorpiones. Pasó innumerables noches en soledad, trabajando incansablemente para crear una criatura que superara todas las expectativas. 
-WildMonsterKiller:1
-Like:神秘
-Nature:kind=6,severe=4,honest=4,cunning=6,calm=6,anger=4,strong=7,weak=3
-fight_skills:升龙拳|吼叫|饮酒|飞腿
-fight_dgskill:刺拳,1
-AssSkill:统率技能厄苏拉</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Hm? Consigue para mí esos artículos de &lt;color=red&gt;lucha&lt;/color&gt; ¡Me encantan!
-hello: El gancho bloqueador... nunca... falla...
-refuse_recruit_0: No eres merecedor/a de mi habilidad.
-recruit_msg: Tu deseo es una orden para mí, estaré a tu servicio.
-enemy_hello: Detente, ya estás dentro del alcance de mi gancho bloqueador.
-be_attack: Gancho bloqueador, listo para atacar.
-be_attack_enemy: Que comience la pesadilla, no escaparás de mi agarre.</t>
-  </si>
-  <si>
-    <t>Desc:Khaza, apodado también como el "Agarre de Gancho", es reconocido como uno de los combatientes más habilidosos reclutados por Rebiya, la Reina de los Dakn. Desde joven, Khaza ha dedicado su vida al perfeccionamiento de sus habilidades marciales, dominando la técnica del Agarre de Gancho.
-Como miembro leal de las fuerzas de Rebiya, Khaza destaca por su destreza en combate cuerpo a cuerpo y su dominio del Agarre de Gancho, lo que lo convierte en un adversario temible en el campo de batalla. Con movimientos rápidos y precisos, puede inmovilizar y controlar a sus oponentes, dejándolos a merced de sus potentes ataques. La lealtad de Khaza hacia Rebiya y su dedicación incansable a la causa de los Dakn lo convierten en un activo indispensable en su búsqueda de poder y dominio. Su presencia imponente y su habilidad para imponerse en el combate lo convierten en una figura respetada y temida en los círculos de lucha.
-Like:格斗
-Nature:kind=2,severe=8,honest=3,cunning=7,calm=2,anger=8,strong=5,weak=5
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能卡拉</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Trae para mí &lt;color=red&gt;artesanías&lt;/color&gt;! ¡Quiero ver cómo otros maestros las crean!
-hello: ¡No hay arma que no pueda forjar con maestría!
-refuse_recruit_0: ¡No eres digno de recibir mi lealtad!
-recruit_msg: ¡Perfecto! ¡Incluso podría forjar una espada especial para ti!
-enemy_hello: ¿Qué pasa, no te pongas tan amargado/a.
-be_attack: ¡Ja! ¡Ahora podré probar mi nueva arma en combate!
-be_attack_enemy: ¡Lo pediste! ¡Ven y enfrenta tu destino!</t>
-  </si>
-  <si>
-    <t>Desc:Tua es un hábil maestro espadero que recibió su formación de manos del legendario Manal, un renombrado herrero del antiguo imperio. Dotado de un excepcional talento y una dedicación implacable, Tua dominó el arte de forjar espadas de calidad insuperable. Su habilidad en la forja era tan reconocida que el antiguo imperio lo empleó como herrero principal, confiándole la creación de armas de gran valor y poder.
-Durante su tiempo en el antiguo imperio, Tua dejó su huella en la historia al forjar dos de las tres espadas emblemáticas utilizadas por Ruha, una valiente líder militar. Estas espadas eran obras maestras de la metalurgia, imbuidas de una calidad y una magia especial que las convertían en armas letales en manos de su portadora. Tras la caída del imperio, Tua encontró un nuevo propósito y empleo en las filas del ejército de los Dhib, donde ahora sirve como Comandante. Su habilidad como espadero y su experiencia en el campo de batalla lo convierten en un valioso activo para los Dhib, y su legado como creador de armas legendarias perdura en la historia.
-WildMonsterKiller:1
-Like:工艺
-Nature:kind=5,severe=5,honest=8,cunning=2,calm=5,anger=5,strong=9,weak=1
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能图哈</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Oh? ¿Acaso tienes algún objeto de &lt;color=red&gt;magia&lt;/color&gt; que nunca haya visto antes? Me encantan las sorpresas y los objetos mágicos que despiertan mi curiosidad.
-hello: ¡Ey! ¿Quieres escuchar una melodía especial? Puedo crear una sinfonía mágica que te transportará a otros mundos.
-refuse_recruit_0: Tienes una apariencia interesante, pero aún no logras fascinarme lo suficiente como para unirme a tu causa.
-refuse_recruit_1: ¿No ves que estoy inmersa en mis experimentos de alquimia? Prefiero mantener mi libertad y explorar el potencial de la magia por mi cuenta.
-refuse_recruit_2: Tus habilidades son impresionantes, pero no creas que me conformaré con ser solo una más en tu grupo.
-refuse_recruit_3: Eres insignificante, un simple destello en comparación con el poder y la grandeza que persigo.
-recruit_msg: La magia que emana de ti es fascinante y despierta mi interés. Estoy dispuestoa a unirme a tu causa y descubrir juntos nuevos horizontes mágicos.
-enemy_hello: Esa poción que acabas de beber era solo un pequeño adelanto de mis habilidades alquímicas. Prepárate para enfrentar el poder de la magia en su máxima expresión.
-be_attack: Eres lindo/a, te guardaré para probar mis venenos y conjuros.
-be_attack_enemy: Nagukka es un lugar adecuado para poner a prueba tus habilidades. Aquí decidiremos si mereces vivir o ser sepultado bajo el peso de mi poder mágico.</t>
-  </si>
-  <si>
-    <t>Desc:Shirim es una enigmática herbolista que habita en los Acantilados de Umbra, conocida por su vasto conocimiento de las plantas medicinales y su habilidad para sanar enfermedades. Sin embargo, hay rumores que circulan acerca de su oscura conexión con las artes mágicas prohibidas. Se dice que Shirim ha explorado el lado más sombrío de la magia, experimentando con hechizos y pociones que trascienden los límites de lo convencional.
-A medida que la locura se apodera de Nagukka y Mireton, muchos atribuyen parte de la responsabilidad a Shirim y su presunta inclinación hacia la magia negra. Se rumorea que sus prácticas ocultas han desencadenado una fuerza tenebrosa que corrompe las mentes y altera la realidad en estas tierras. Temida y susurrada en los rincones más oscuros, Shirim se convierte en un enigma envuelto en misterio, cuyos poderes y verdaderas intenciones solo pueden ser especulados.
-WildMonsterKiller:1
-Like:魔力
-Nature:kind=2,severe=8,honest=3,cunning=7,calm=5,anger=5,strong=5,weak=5
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能希可弥</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Mi madre era una excepcional pintora. No hay nada que aprecie más que &lt;color=red&gt;obras de arte&lt;/color&gt; que me recuerden su talento.
-hello: Infunde temor o enfrenta tu destino. Mantén tu arma cerca.
-refuse_recruit_0: Permíteme reflexionar un poco más al respecto.
-refuse_recruit_1: No confío en nadie. ¿Por qué debería confiar en ti?
-refuse_recruit_2: ¿Quién eres tú... y por qué debería unirme a tu causa?
-refuse_recruit_3: Dejame sola, no quiero hablar...
-enemy_hello: Cada paso mas cerca de mi, la muerte se aproxima a ti.
-recruit_msg: ¿Realmente puedo depositar mi confianza en ti?
-be_attack: ¡Luchemos hasta el final!
-be_attack_enemy: Es mejor morir en batalla que rendirse sin honor.</t>
-  </si>
-  <si>
-    <t>Desc:Fayiz, a valiente guerrera, lleva consigo el legado de la antigua tribu Oryx, cuyos miembros fueron dispersados y su cultura olvidada. Como una niña vendida al clan Dhib, fue su determinación y habilidad excepcionales las que llamaron la atención de Ruha, líder de los Dhib. Reconociendo su potencial, Ruha la tomó bajo su protección y la guió en el camino de la guerra.
-A medida que los años pasaron, Fayiz demostró ser una aliada leal y una formidable combatiente. Su habilidad en el combate cuerpo a cuerpo y su astucia estratégica la llevaron a convertirse en la mano derecha de Ruha. Juntos, forjaron un vínculo fuerte y compartieron innumerables batallas, defendiendo a los Dhib y enfrentando a sus enemigos con una determinación inquebrantable. Fayiz se ha convertido en un símbolo de la resistencia y el orgullo de su ancestral tribu, luchando incansablemente por su gente y por el legado que lleva en su corazón.
-WildMonsterKiller:1
-Like:绘画
-Nature:kind=5,severe=5,honest=7,cunning=3,calm=7,anger=3,strong=10,weak=0
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能云英</t>
-  </si>
-  <si>
-    <t>Desc:La familia de Sharida es una de las familias nobles más antiguas de Dakn, conocedora de la tradición de Dakn. Ella creció en la tienda del líder de Dakn junto a Hassan. Hassan se unió a los Nasir para atacar la Ciudad de Jamal. El consejo de Sharida fue indispensable. Sin embargo, cuando Hassan enfermó, su hermana más cruel abandonó a la familia de Sharida y se convirtió en la única noble. Sharida guardó esto en su corazón. Solo ella sabe cómo responderá a la traición de Rebiya en el futuro.
-A pesar de la traición y el desprecio frío de la hermana de Hassan, Sharida se mantuvo firme en su lealtad hacia su amigo. Se aferraba a los recuerdos de su crianza compartida y del vínculo que formaron en la tienda del líder de Dakn. En lo más profundo de su ser, un fuego ardía en Sharida, alimentando su determinación de buscar justicia y restaurar el honor de su familia. Sabía que la traición de Rebiya no quedaría sin respuesta y prometió en silencio recuperar lo que legítimamente les pertenecía. Con cada día que pasaba, Sharida perfeccionaba sus habilidades, tanto en el arte de la diplomacia como en las formas del guerrero, preparándose para el día en que enfrentaría a su némesis y remodelaría el destino de su familia y del pueblo Dakn.
-WildMonsterKiller:1
-Like:音乐|历史|绘画
-Nature:kind=5,severe=5,honest=2,cunning=8,calm=9,anger=1,strong=5,weak=5
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能沙里娅</t>
-  </si>
-  <si>
-    <t>Desc: A una noble le gusta la &lt;color=red&gt;música&lt;/color&gt;, la &lt;color=red&gt;pintura&lt;/color&gt; y, por supuesto, la &lt;color=red&gt;historia&lt;/color&gt;. El señor Hassan disfrutaba de discutir sobre tales cosas conmigo.
-hello: ¡Un día! ¡Un día él señor Hassan volverá!
-refuse_recruit_0: Sigo esperando el regreso del señor Hassan.
-refuse_recruit_1: La ambición requiere fuerza. Tú careces de ambas.
-refuse_recruit_2: ¿Te atreverías a intentar comprar a un diplomático? ¿En serio?
-refuse_recruit_3: ...Eres ambicioso. Necesitas de mi ayuda? Por ahora.. no puedo...
-enemy_hello: Eres tan vicioso como esa mujer...
-be_attack: ¡Qué vergonzoso!
-be_attack_enemy: ¿Te atreves a intimidar a una dama con fuerza? No eres nada comparado con los poderes que he presenciado.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me apasiona mi colección de &lt;color=red&gt;equipamiento especial&lt;/color&gt;.
-hello: ¿Quieres practicar tiro con arco?
-enemy_hello: Acércate y tendrás que estar atento a mis flechas.
-refuse_recruit_0: Eres fuerte, pero tu puntería no es precisa. Déjame pensarlo.
-refuse_recruit_1: No mereces ni siquiera tensar la cuerda de mi arco.
-refuse_recruit_2: Vete, no me molestes.
-refuse_recruit_3: Ni siquiera verías cómo tenso la flecha.
-recruit_msg: De acuerdo. Espero que puedas aprender tiro con arco de mí.
-be_attack: Si así quieres que sea...
-be_attack_enemy: ¿Crees que puedes esquivar mis flechas? Ridículo.</t>
-  </si>
-  <si>
-    <t>Desc:Fire Eye, desde temprana edad, mostró una pasión innata por el tiro con arco. Aunque sus habilidades nunca alcanzaron la perfección, su destreza única se reveló durante el asedio de una ciudad. En un momento crucial, mientras lanzaba una flecha hacia su objetivo, un golpe de suerte hizo que esta se encendiera en llamas, provocando una reacción explosiva al entrar en contacto con los depósitos de combustible enemigos. El estallido masivo resultó en una victoria aplastante para los Nasir. Impresionados por su valentía y la inesperada eficacia de su técnica, Fire Eye fue ascendido a Comandante, desafiando la noción convencional de que la precisión es el único criterio para los arqueros.
-Desde ese momento, Fire Eye se convirtió en una leyenda viviente entre las filas de los Nasir. Su habilidad única para causar estragos en las defensas enemigas con sus flechas ardientes le valió el apodo de "Ojo de Fuego". Inspirando tanto temor como admiración, Fire Eye demostró que en la guerra, la imprevisibilidad y la audacia pueden ser igual de poderosas que la precisión. Su legado se convirtió en una enseñanza para futuros arqueros, recordándoles que el valor y la determinación pueden marcar la diferencia en el campo de batalla, incluso cuando la puntería no es perfecta.
-WildMonsterKiller:1
-Like:特殊装备
-Nature:kind=4,severe=6,honest=4,cunning=6,calm=8,anger=2,strong=5,weak=5
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能火眼</t>
-  </si>
-  <si>
-    <t>Desc:Procedente de una larga línea de hábiles adiestradores de camellos, nuestro protagonista perfeccionó su experiencia en el cuidado y entrenamiento de estas majestuosas criaturas del desierto. La reputación de su familia como destacados comerciantes de camellos les otorgó respeto y admiración entre las comunidades que habitaban en el desierto. Sin embargo, el destino tenía preparado un camino diferente cuando la tribu de los Akhal emergió como una fuerza dominante en el vasto desierto occidental de Docana.
-Impresionados por sus habilidades excepcionales y su profundo conocimiento en el manejo de camellos, los Akhal reconocieron el potencial del protagonista y le otorgaron el estatus de noble dentro de sus filas. Ahora elevado a la posición de noble, nuestro protagonista asume el importante papel de liderar a los distinguidos jinetes de camellos de los Akhal. Su comando estratégico y su íntimo conocimiento del terreno del desierto los convierten en un recurso indispensable en las expediciones de la tribu, mientras atraviesan las implacables arenas junto a sus compañeros camellos, asegurando la prosperidad de la tribu y estableciendo su reputación como formidables nómadas del desierto.
-WildMonsterKiller:1
-Like:地理
-Nature:kind=8,severe=2,honest=5,cunning=5,calm=7,anger=3,strong=5,weak=5
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能维库那</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:El sueño de mi infancia era liderar una magnífica caravana de camellos y explorar tierras desconocidas. La &lt;color=red&gt;geografía&lt;/color&gt; siempre ha sido mi pasión, te escuchare atento si me hablas sobre esos temas.
-hello: Nunca olvides quién eres, mantén siempre tu esencia presente.
-refuse_recruit_0: No puedes enfrentar la realidad. Resulta difícil creer en ti.
-recruit_msg: Seguiré a un líder constante como tú. Estoy listo para embarcarme en esta aventura juntos.
-enemy_hello: ¿Qué intentas lograr con todo esto? ¿Cuál es tu verdadero propósito?
-be_attack: Entonces solo nos queda la batalla, y estoy dispuesto a enfrentarla con valentía.
-be_attack_enemy: ¡Con mis camellos no podrán derrotarme! Desafío a cualquier obstáculo que se interponga en mi camino.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Cuando por fin tengo un poco de tiempo para mí, disfruto tocando mis &lt;color=red&gt;instrumentos musicales&lt;/color&gt;. Es en esos momentos donde puedo sumergirme en el mundo de la melodía y la armonía, dejando que la música me lleve a lugares lejanos y emociones profundas.
-hello: Incluso los cambios más pequeños pueden dar lugar a resultados muy diferentes. Recuerda siempre el poder transformador que yace en cada decisión.
-refuse_recruit_0: Es un tanto tarde para unirme a ti en este momento. Mi compromiso ya se encuentra en otro lugar.
-recruit_msg: Esta es, sin duda, la decisión más acertada que has tomado, mi señor. Estoy listo para servirte con lealtad y habilidades musicales que te sorprenderán.
-enemy_hello: Parece que no has reflexionado lo suficiente sobre las consecuencias de tus acciones. Prepárate para enfrentar las consecuencias de tus decisiones.
-be_attack: No esperaba que fueras tan rebelde.
-be_attack_enemy: ¡Ven, esto es algo que planifiqué hace mucho tiempo! He anticipado cada movimiento y estoy listo para hacer frente a cualquier desafío.</t>
-  </si>
-  <si>
-    <t>Desc:Dhaji, un astuto político, aspiraba a convertirse en el Ministro de la Ciudad de Jamal, pero vio sus ambiciones truncadas tras la caída del Imperio Nephrit. Tras el saqueo de Jamal City, regresó a su hogar ancestral en los Acantilados de Umbra. Allí, su habilidad para persuadir y su lengua elocuente llamaron la atención de Ludo Khan, un poderoso personaje de la región, quien rápidamente lo empleó, reconociendo su astucia política.Su camino está marcado por la redención y el ansia de éxito, mientras navega por un peligroso escenario lleno de intrigas y luchas de poder.Con cada día que pasa, Dhaji se convierte en una figura influyente, tejedor de intrigas y estrategias para abrirse camino de regreso hacia la cima del poder político. 
-WildMonsterKiller:1
-Like:乐器
-Nature:kind=4,severe=6,honest=2,cunning=8,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能金达吉</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Los &lt;color=red&gt;juguetes&lt;/color&gt; bellamente elaborados me recuerdan mi feliz infancia cuando mi padre era gobernador de Redstone Keep...Evocan los recuerdos ... Cada detalle de estos objetos me transporta a esos días llenos de inocencia y alegría, recordando las risas y los momentos compartidos en aquel entonces.
-hello: En este mundo, hay quienes siempre buscan atacar, así como hay quienes se dedican a la defensa constante de lo que aman.
-refuse_recruit_0: Eres diferente a los demás, pero mis prioridades me llevan por un camino distinto en este momento.
-recruit_msg: ¿Podrás vengar a mi padre, tal como yo deseo?
-enemy_hello: Si valoras tu vida, te recomendaría no convertirte en mi enemigo.
-be_attack: Descubrirás la vergüenza que pesa sobre el legado de mi padre.
-be_attack_enemy: Perdoname... pero tendre que sere  implacable.</t>
-  </si>
-  <si>
-    <t>Desc:Petra, la hija ilegítima del gobernador que gobernaba Redstone Keep durante el Imperio Nephrit, vio su vida alterada cuando los Nasir tomaron la ciudad. A pesar de las circunstancias adversas, su vida fue perdonada y quedó bajo la protección de Husnu. A simple vista, su lealtad parece firme, pero pocos saben realmente qué pensamientos cruzan su mente.
-Como hija ilegítima, Petra ha aprendido a navegar por el mundo con astucia y discreción. Sus experiencias pasadas y su posición actual bajo la tutela de Husnu han forjado una personalidad enigmática y reservada. Si bien muestra lealtad aparente, sus verdaderas intenciones y motivaciones permanecen ocultas para la mayoría. Petra es una figura enigmática que guarda sus secretos y solo el tiempo revelará qué planes y pensamientos realmente alberga en su interior.
-WildMonsterKiller:1
-Like:玩具
-Nature:kind=3,severe=7,honest=2,cunning=8,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能沙月</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Los nobles solo se complacen con cosas dignas de los &lt;color=red&gt;nobles&lt;/color&gt;!
-hello: Nuestras tradiciones son el tesoro más preciado en todo el mundo.
-refuse_recruit_0: Eres un valiente guerrero, pero no sigues nuestras tradiciones.
-refuse_recruit_1: Puedo confiar en ti, pero no lucharé a tu lado.
-refuse_recruit_2: No respetas las tradiciones de los Akhal, lo que implica que no me respetas a mí.
-refuse_recruit_3: Por favor, retírate y déjanos en paz.
-recruit_msg: Tú respetas las reglas de los Akhal, por lo tanto, te seguiré lealmente.
-enemy_hello: Aunque seamos enemigos, te tengo respeto.
-be_attack: ¡Muy bien, resolvamos esto siguiendo las reglas de nuestro linaje!
-be_attack_enemy: ¡Estupendo, tienes la oportunidad de morir como un verdadero guerrero!</t>
-  </si>
-  <si>
-    <t>Desc:Blackmane es el amado hermano de Bahat y el General de las fuerzas de los Akhal. Como líder conservador, Blackmane insiste en mantener las tradiciones ancestrales sin alteraciones. Su devoción por preservar las costumbres antiguas es incuestionable, y considera que son fundamentales para la identidad y la fuerza de los Akhal.
-Como General, Blackmane se adhiere estrictamente a las formas de batalla tradicionales y promueve la disciplina y el honor entre sus soldados. Su enfoque inflexible hacia las antiguas prácticas refleja su creencia en su eficacia y en la preservación de la herencia de los Akhal. Aunque algunos pueden cuestionar su resistencia al cambio, Blackmane se mantiene firme en su convicción de que las tradiciones sin alteraciones son el fundamento para el éxito y la grandeza de los Akhal.
-WildMonsterKiller:1
-Like:高贵
-Nature:kind=8,severe=2,honest=6,cunning=4,calm=6,anger=4,strong=9,weak=1
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能黑鬃</t>
-  </si>
-  <si>
-    <t>Like:珠宝|高贵
-Desc:Kanaya nació en el seno de una familia de comerciantes. Desde temprana edad, soñaba con alcanzar una riqueza deslumbrante y vivir en la próspera Ciudad de Jamal. Sin embargo, la guerra trajo consigo tiempos difíciles para su familia. A pesar de las adversidades, Kanaya no ha renunciado a sus sueños de prosperidad y trabaja incansablemente en el bullicioso bazar.
-Con una determinación inquebrantable, Kanaya se sumerge en el ajetreo y el bullicio del mercado, buscando oportunidades para mejorar su situación económica. Su habilidad para negociar y su agudo instinto comercial le permiten navegar por los desafíos y obstáculos que se presentan en su camino. Aunque el camino hacia la riqueza puede ser arduo, Kanaya se aferra a la esperanza y sigue trabajando con ahínco para hacer realidad sus anhelos de éxito y fortuna en el fascinante mundo del bazar.
-Robber:100
-Nature:kind=7,severe=3,honest=2,cunning=8,calm=6,anger=4,strong=7,weak=3
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能康牙</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me encantan las &lt;color=red&gt;joyas&lt;/color&gt; o los &lt;color=red&gt;adornos&lt;/color&gt;, cualquier cosa que me haga lucir más hermosa.
-hello: ¡Hola! ¿Por qué estás buscandome?
-refuse_recruit_0: Tienes un cierto encanto, pero hay muy poco más que me emocione contigo.
-refuse_recruit_1: Mi belleza sería desperdiciada a tu lado.
-refuse_recruit_2: ¿Amigos? No, definitivamente no lo somos.
-refuse_recruit_3: Criatura repugnante, te ruego que te vayas.
-recruit_msg: Está bien. Parece que te atraigo, y me atraes... así que no puedo rechazarte.
-enemy_hello: ¿Te atreves a hablarme todavía? Oh, realmente debes estar loco/a.
-be_attack: ¿En serio? ¿Quién se atrevería a intimidar a una chica?
-be_attack_enemy: Pensaba que en ti... al fin habia encontrado a alguien que practique lo oculto conmigo~</t>
-  </si>
-  <si>
-    <t>Like:珠宝|魔力|装饰
-Desc:Miaya fue abandonada por sus padres durante la guerra. Su infancia en el Valle Twinluna fue difícil y desafiante. A medida que crecía y se convertía en mujer, sentía envidia de las chicas que tenían dinero para vestirse elegantemente. Necesitada y con ganas por ganar dinero, estaba dispuesta a realizar trabajos peligrosos que los hombres temían realizar, al punto de poner su vida en peligro... ya que su otra salida era vender su cuerpo. Fue entonces cuando un spiritmancer, apreciando su valentía y determinacion, la aceptó como aprendiz.
-Bajo la tutela del spiritmancer, Miaya comenzó a explorar el mundo de la magia y los espíritus. Aprendió a canalizar sus habilidades naturales y a controlar los poderes que yacían dentro de ella. Con cada desafío superado, su confianza creció y se convirtió en una experta en su arte.
-Ahora, Miaya utiliza su destreza mágica y su valentía para llevar a cabo tareas arriesgadas y desafiantes. Su camino no convencional y su capacidad para enfrentarse a peligrosos trabajos le han ganado respeto en los círculos de spiritmancer. Aunque su pasado ha sido difícil, ha encontrado un nuevo propósito y una familia en la comunidad de los spiritmancers.
-Nature:kind=3,severe=7,honest=2,cunning=8,calm=6,anger=4,strong=8,weak=2
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能百花</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Una mujer madura valora el conocimiento. Disfruto sumergirme en la &lt;color=red&gt;cultura&lt;/color&gt;, ya que me brinda paz y serenidad.
-hello: Te encuentras frente al líder de la Casa Giddah.
-refuse_recruit_0: Aunque te admiro profundamente, la Casa Giddah necesita mi liderazgo en este momento.
-refuse_recruit_1: No mereces realmente mi atención en este momento.
-refuse_recruit_2: Hmph. No te sobreestimes.
-refuse_recruit_3: Debilucho. Retírate de mi vista.
-recruit_msg: Eres fuerte, tal vez juntos podamos enfrentar a todos.
-enemy_hello: Espero que comprendas claramente tu posición y que puedas apreciar mejor la mía.
-be_attack: No tengo problemas contigo. ¡Piensa con claridad!
-be_attack_enemy: Llegas en el momento justo. Mi espada estaba sedienta de almas.</t>
-  </si>
-  <si>
-    <t>Like:文学|装饰
-Desc:Yasmin, la hermana mayor de la familia Giddah, sufrió una humillación cuando fue derrotada por su hermana menor, Bellen, en un torneo familiar de los Giddah. Como resultado, se vio obligada a entregar la espada familiar a Bellen, lo que convirtió a esta última en la líder de la familia Giddah. En secreto, Yasmin conspiró con su hermana Mumtali para incriminar a Bellen y desterrarla de la familia Giddah. Ahora, Yasmin ostenta el liderazgo de la Casa Giddah.
-La traición y el resentimiento en el corazón de Yasmin la impulsaron a tomar medidas drásticas para obtener el poder que creía merecer. Aprovechando su posición como líder de la familia Giddah, ha consolidado su autoridad y establecido su dominio sobre los demás miembros de la casa. Sin embargo, el peso de su traición y la sombra de su pasado oscuro pueden perseguirla y amenazar su liderazgo. Yasmin se enfrenta a la difícil tarea de mantener el equilibrio entre su ansia de poder y la preservación de la unidad y el honor de la familia Giddah.
-Nature:kind=2,severe=8,honest=3,cunning=7,calm=3,anger=7,strong=7,weak=3
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能公孙妍</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Qué me gusta? Los objetos &lt;color=red&gt;ocultos&lt;/color&gt; son buenos accesorios. Hablando de accesorios, los &lt;color=red&gt;adornos&lt;/color&gt; no están mal.
-hello: ¡Uf! ¡Hace viento hoy, eh?
-refuse_recruit_0: Eres una buena persona, pero... podrías frenar mi avance.
-refuse_recruit_1: Nos acabamos de conocer. No necesitas hacer tanto por mí.
-refuse_recruit_2: Eres un vagabundo sin nombre ni casa. ¿Te atreves a hablarme?
-refuse_recruit_3: Fuera, insignificante.
-recruit_msg: ¡Jajaja! Seré tu aliada y te ayudaré en todo. ¡A cambio, me ayudarás a ascender a la cabeza de la Casa Giddah!
-enemy_hello: No deberíamos estar hablando, ¿verdad?
-be_attack: Tienes mucho valor para hablarme de esa manera.
-be_attack_enemy: ¡Jaja! Llegas en el momento justo... ¡mis cuervos tienen hambre!</t>
-  </si>
-  <si>
-    <t>Like:神秘|装饰
-Desc:La segunda hija de la familia Giddah, Mumtali, conspiró junto a su hermana mayor Yasmin para incriminar a su hermana menor, la Princesa Bellen. Con su travesura cumplida, Mumtali ascendió al puesto de segunda al mando de la Casa Giddah. Sin embargo, su ambición no se vería saciada con tan solo ocupar ese puesto. Así, comenzó a idear un nuevo plan...
-Impulsada por su sed de poder y deseosa de obtener un papel aún más prominente dentro de la familia, Mumtali trama nuevas intrigas. Su mente maquiavélica y su astucia se combinan para llevar a cabo su nuevo complot, en busca de alcanzar el dominio absoluto sobre la Casa Giddah. Con su determinación implacable y su habilidad para manipular las situaciones a su favor, Mumtali se convierte en una figura intrigante y peligrosa dentro del entorno familiar.
-Sin embargo, el éxito de sus maquinaciones y la aceptación de sus planes están lejos de ser garantizados. Las consecuencias de sus actos y la respuesta de aquellos que descubran sus verdaderas intenciones podrían poner en peligro su posición y desencadenar una serie de eventos impredecibles. Mumtali se adentra en un camino lleno de incertidumbre y riesgo, donde su astucia y su deseo de poder serán puestos a prueba en cada paso que dé.
-Nature:kind=2,severe=8,honest=1,cunning=9,calm=7,anger=3,strong=3,weak=7
-fight_skills:踩脚趾|丢酒瓶|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能公孙弥</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me gusta el &lt;color=red&gt;combate&lt;/color&gt;... y la &lt;color=red&gt;historia&lt;/color&gt;.
-hello: ¿Has venido a ver a Misod?
-refuse_recruit_0:... Para ser sincero/a, tus hazañas me conmueven, pero tengo otras cosas que debo hacer.
-refuse_recruit_1:Lo siento, debo rechazar.
-refuse_recruit_2:Por favor, vete. Tengo otras cosas que hacer.
-refuse_recruit_3:Vete ahora mismo, villano/a.
-recruit_msg: Luchemos juntos por un futuro pacífico.
-enemy_hello: Buscamos cosas diferentes. Deberías irte.
-be_attack: Pareces decidido/a a luchar. Te daré lo que buscas.
-be_attack_enemy: Me alegra que hayas venido. Has evitado luchar contra mí durante un tiempo.</t>
-  </si>
-  <si>
-    <t>Like:历史|格斗
-WildMonsterKiller:1
-Desc:Un huérfano que aprendió a luchar para sobrevivir en tiempos de guerra. En su juventud, se encontró con el bard Misod y se conmovió por su sueño de crear un mundo pacífico. Inspirado por esta visión, decidió luchar por el futuro que tanto él como Misod soñaban.
-A medida que perfeccionaba sus habilidades de combate, este huérfano canalizó su determinación y valentía hacia la causa de la paz. Reconociendo que la violencia y el conflicto solo perpetuaban el sufrimiento, se unió a Misod en la búsqueda de un mundo mejor.
-Guiado por el sueño compartido de un futuro pacífico, este luchador huérfano se convierte en un defensor incansable de la justicia y la armonía. En cada batalla, busca no solo la victoria, sino también la semilla de un cambio duradero. 
-Nature:kind=6,severe=4,honest=7,cunning=3,calm=2,anger=8,strong=9,weak=1
-fight_skills:蓄力冲刺|冲刺重拳|升龙拳|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能穆长滩</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: &lt;color=red&gt;La historia&lt;/color&gt; es el &lt;color=red&gt;relato&lt;/color&gt; de la vida. Me gusta la historia y me encantan las historias en sí.
-hello: ¡Hola! ¿Quieres escuchar una canción?
-refuse_recruit_0: Te aprecio, pero valoro mi libertad.
-refuse_recruit_1: Gracias, pero no puedo darte la respuesta que buscas.
-refuse_recruit_2: No tengo motivos para acompañarte, ¿verdad?
-refuse_recruit_3: No caminamos por el mismo sendero. Por favor, vete.
-recruit_msg: ♫ Un aventurero y un bardo, ahora el camino será más suave ♫
-enemy_hello: Has hecho algunas cosas malvadas. ¿Me equivoco?
-be_attack: ¡Oye! ¿Estás seguro/a de querer hacer esto? Realmente estás loco/a.
-be_attack_enemy: Así que me has encontrado. Me has ahorrado algo de tiempo.</t>
-  </si>
-  <si>
-    <t>Like:历史|故事
-WildMonsterKiller:1
-Desc:El bardo Misod proviene de la cabeza del río. Es un joven noble de baja posición. Disfruta de la poesía épica y la literatura. Sin embargo, no deseaba participar en las luchas familiares, por lo que decidió seguir su pasión por los viajes y emprender un camino hacia el este, en solitario. En su travesía, se encontró con muchas personas que habían sido testigos de la crueldad de la guerra. Misod tomó la decisión de plasmar sus historias por escrito.
-Movido por su profundo sentido de empatía y justicia, Misod se convirtió en un recopilador de historias, un narrador de los testimonios de aquellos que habían sufrido los horrores de la guerra. A medida que viajaba de lugar en lugar, escuchaba los relatos de los afectados y los inmortalizaba en forma de escritos y canciones. Su dedicación a dar voz a los que habían sido silenciados por el conflicto lo llevó a ser conocido como un defensor de la memoria y la conciencia colectiva.
-A través de sus obras, Misod no solo busca documentar la realidad de la guerra, sino también transmitir un mensaje de esperanza y comprensión. 
-Nature:kind=8,severe=2,honest=6,cunning=4,calm=8,anger=2,strong=6,weak=4
-fight_skills:冲刺膝盖顶|丢酒瓶|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能米索德</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me gustan las cosas &lt;color=red&gt;tristes&lt;/color&gt;, &lt;color=red&gt;románticas&lt;/color&gt;... o cualquier cosa relacionada con la &lt;color=red&gt;Diosa del Río&lt;/color&gt;, por supuesto.
-hello: Tú... ¿por qué me has encontrado?
-refuse_recruit_0: Eres una buena persona, pero yo... yo... no puedo ayudarte.
-refuse_recruit_1: Yo... no me gusta viajar con otros.
-refuse_recruit_2: No quiero ser una carga, por favor, no me pidas esto.
-refuse_recruit_3: ¿Podrías irte, por favor?
-recruit_msg: Tengo el cabello negro y los ojos azules de los Nephrit. Creo que hay un poder en mi linaje esperando a que lo despierte. Gracias por creer en mí. Lucharé contigo.
-enemy_hello: Dicen... que no eres una buena persona...
-be_attack: De acuerdo. No tendré miedo.
-be_attack_enemy: Te detendré. Ven.</t>
-  </si>
-  <si>
-    <t>Like:忧伤|浪漫|女神
-Desc:Amira es la hija de uno de los mercaderes más ricos del Bazar Dorado, quienes una vez fueron nobles entre los Nephrit. Cuando Jamal City cayó y el antiguo imperio desapareció, sus padres tomaron su tesoro y huyeron al Valle de Twinluna. Como nobles del antiguo imperio, sus padres eran personas trabajadoras y honestas. La madre de Amira Zahra era prácticamente una hija para el antiguo rey Nephrit. Su sabiduría y ética de trabajo trajeron éxito a la familia, pero falleció al dar a luz a Amira. Después de su muerte, el padre de Amira cayó en depresión, lo que afectó la crianza de Amira.
-El dolor de la pérdida y la tristeza que envolvieron a su familia dejaron una profunda marca en Amira desde una edad temprana. Criada en un ambiente de melancolía, aprendió a ser fuerte y resiliente, pero también desarrolló un anhelo de encontrar su propio propósito y superar las sombras del pasado. A medida que crece, Amira se enfrenta al desafío de equilibrar su herencia noble y las expectativas que conlleva con su deseo de forjar su propio camino.
-Con una mezcla de determinación y curiosidad, Amira se embarca en una búsqueda personal de autodescubrimiento y superación. Anhela encontrar un sentido de identidad y encontrar su lugar en un mundo cambiante. 
-Nature:kind=5,severe=5,honest=5,cunning=5,calm=5,anger=5,strong=5,weak=5
-fight_skills:踩脚趾|直拳|冲刺膝盖顶|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能西河娜娅</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Disfruto de &lt;color=red&gt;equipamiento muy especial&lt;/color&gt; o &lt;color=red&gt;tesoros&lt;/color&gt; desconocidos para los mortales.
-hello: ¿Buscas a mí o a mi espada?
-refuse_recruit_0: Eres valiente, pero no eres fuerte.
-refuse_recruit_1: Hmph. No somos de la misma casa.
-refuse_recruit_2: Hm.
-refuse_recruit_3: ¡Me disgustas!
-recruit_msg: El arte de la espada de la Casa Giddah es invencible.
-enemy_hello: Eres tan despreciable como esas dos hermanas mías.
-be_attack: Ya he sido traicionado/a. No hay nada que puedas hacer para herirme.
-be_attack_enemy: ¿Quieres presenciar el arte de la espada de la Casa Giddah? ¡Entonces sé testigo de ello!</t>
-  </si>
-  <si>
-    <t>Like:特殊装备|高贵
-WildMonsterKiller:1
-Desc:El fundador de la Casa Giddah fue un general en la primera dinastía del Antiguo Imperio. Se retiró y se convirtió en Sultán. Durante la Batalla del Sol Negro, la Casa Giddah defendió su tierra utilizando el conocimiento de la espada transmitido por sus ancestros. El padre de Bellen falleció hace tres años. De acuerdo con la tradición de la Casa, los hijos de la misma generación debían luchar en un torneo para convertirse en el líder de la Casa. Solo el ganador podía heredar el liderazgo de la Casa Giddah y la valiosa espada familiar. Bellen resultó vencedora del torneo, pero sus dos hermanas mayores conspiraron en su contra y la acusaron de envenenar a su padre. Bellen no protestó. Comprendió las motivaciones de sus hermanas. Dejó atrás su vida como princesa de Giddah y se convirtió en una espadachina errante.
-Movida por el deseo de proteger el honor y la herencia de su familia, Bellen emprendió un viaje solitario en busca de redención y justicia. Su camino como espadachina vagabunda está marcado por la determinación y la valentía, mientras se enfrenta a numerosos desafíos y peligros. Con la espada familiar en mano, Bellen se convierte en una fuerza imparable, utilizando su destreza en el arte de la espada para defender a los desfavorecidos y luchar contra la injusticia en un mundo turbulento.
-Aunque enfrenta la traición de sus hermanas y la pérdida de su estatus noble, Bellen encuentra una nueva identidad y propósito en su papel como espadachina errante. Con cada batalla, se acerca más a descubrir la verdad detrás de la conspiración contra su padre y a desenmascarar a los verdaderos responsables. 
-Nature:kind=7,severe=3,honest=8,cunning=2,calm=7,anger=3,strong=9,weak=1
-fight_skills:冲刺膝盖顶|冲刺重拳|飞腿|蓄力冲刺
-fight_dgskill:刺拳,1
-AssSkill:统率技能公孙巴兰</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Mi padre es un alfarero en la Ciudad de Cotta, por lo que desde que era joven, he disfrutado de las &lt;color=red&gt;artesanías&lt;/color&gt;, especialmente las esculturas. También me gustan los &lt;color=red&gt;equipos muy especiales&lt;/color&gt; que he oído mencionar en leyendas.
-默认: Lo único que puedes protegerte es tu propio puño.
-没耐心: Lo siento. Estoy muy ocupado/a.
-拒绝指教: ¡Jaja! ¿Te conozco? ¿Por qué debería enseñarte?
-完成委托: No está mal. No esperaba menos.
-乞讨冷却中: ¿Vuelves a pedir limosna tan pronto? No es una buena imagen.
-hello: ¿Qué necesitas de mí?
-refuse_recruit_0: Tú... suspiro No, todavía no puedo unirme a tu equipo.
-refuse_recruit_1: Aún somos extraños y no hay nada que me atraiga hacia ti.
-refuse_recruit_2: Lut Jahim no sirve a los débiles.
-refuse_recruit_3: ¡Lárgate!
-recruit_msg: Me recuerdas a mi padre, no al hombre que me engendró, sino aquel que me enseñó cómo vivir. Te ayudaré. Espero que no traiciones mi confianza.
-enemy_hello: Eres un gusano. Y tan ciego como uno también.
-be_attack: ¡Destaco en la batalla!
-be_attack_enemy: ¡Jaja! ¡Eres valiente y a la vez insensato!</t>
-  </si>
-  <si>
-    <t>Like:工艺|故事|特殊装备
-WildMonsterKiller:1
-Robber:100
-Desc:Lut es el hijo de humildes agricultores de la Ciudad de Cotta, quienes lamentablemente perdieron la vida durante una devastadora plaga. Desde muy temprana edad, Lut se vio obligado a enfrentar la dura realidad de la vida como un vagabundo. Sin embargo, su destino dio un giro cuando se encontró con un desertor de los Dakn, quien le enseñó las habilidades de combate necesarias para sobrevivir en un mundo azotado por la guerra. Estas habilidades se convirtieron en su salvación y le permitieron enfrentar los desafíos que se presentaron ante él.
-Tras la trágica muerte de su mentor, Lut Jahim tomó la decisión de unirse oficialmente a las filas de los Dakn como un valiente guerrero. Movido por una insaciable sed de superación, Lut trabaja incansablemente para escalar los escalones de la jerarquía de los Dakn. Su dedicación y determinación son inquebrantables, y está dispuesto a enfrentar cualquier obstáculo con el objetivo de alcanzar la grandeza. 
-Nature:kind=6,severe=4,honest=6,cunning=4,calm=5,anger=5,strong=8,weak=2
-fight_skills:冲刺膝盖顶|冲刺重拳|飞腿|蓄力冲刺
-fight_dgskill:刺拳,1
-AssSkill:统率技能赫连里德</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Qué me gusta? El dinero. ¿A quién no le gusta el dinero? Oh, ¿objetos? &lt;color=red&gt;Las joyas&lt;/color&gt; se pueden convertir en dinero. Y objetos para &lt;color=red&gt;combate&lt;/color&gt; que me ayuden a ganar dinero.
-hello: Un vagabundo, sin un hogar al que regresar.
-refuse_recruit_0: Lamentablemente, estás equivocado/a. Me gustaría acompañarte, pero... también quiero vivir.
-refuse_recruit_1: Tú tampoco pareces rico. Olvídalo.
-refuse_recruit_2: Si quieres contratarme, sigue el camino correcto.
-refuse_recruit_3: ¡Asqueroso/a! Vete al infierno, gusano.
-recruit_msg: Espero que puedas encontrar un lugar para que este vagabundo pueda regresar.
-enemy_hello: Este vagabundo te odia.
-be_attack: ¡Lucha! ¡Lucha!
-be_attack_enemy: Disfrutaré quitándote tu Utar.</t>
-  </si>
-  <si>
-    <t>Like:格斗|珠宝
-Robber:100
-WildMonsterKiller:1
-Desc:Jibirl, natural de los pintorescos Acantilados de Umbra, solía llevar una vida pacífica y satisfactoria durante el reinado del Rey Antiguo. Sus días estaban llenos de trabajar la tierra y disfrutar de las alegrías simples de su humilde existencia. Sin embargo, todo cambió con la catastrófica Batalla del Sol Negro. Las tierras una vez fértiles fueron arrasadas, volviéndose estériles e infértiles. Obligado a abandonar su hogar idílico, Jibirl empuñó una sólida lanza, despidiéndose de sus preciados recuerdos y emprendiendo un nuevo camino como un mercenario errante.
-Ahora un alma nómada, Jibirl deambula por la vasta extensión de la tierra, buscando propósito y fortuna a través de sus habilidades como guerrero a sueldo. El agricultor tranquilo se ha adaptado a las duras realidades de un mundo plagado de conflictos. Con cada paso que da, el peso de su pasado y la incertidumbre de su futuro lo impulsan hacia adelante. La lanza de Jibirl se convierte en su fiel compañera, una herramienta para sobrevivir en un mundo donde la capacidad de defenderse tiene un gran valor. 
-Nature:kind=5,severe=5,honest=4,cunning=6,calm=3,anger=7,strong=7,weak=3
-fight_skills:冲刺膝盖顶|冲刺重拳|吼叫|蓄力冲刺
-fight_dgskill:刺拳,1
-AssSkill:统率技能车巴尔</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me gustan las &lt;color=red&gt;artesanías&lt;/color&gt;, las &lt;color=red&gt;joyas&lt;/color&gt;... ¡y Astrid!
-hello: ¿Aquí para invitarme a una ronda?
-refuse_recruit_0: Si fueras Astrid, no lo dudaría. Pero no eres ella.
-refuse_recruit_1: ¿Yo? ¿Estás seguro/a? Olvídalo. Hic!
-refuse_recruit_2: Debes estar borracho/a. Yo estoy borracho/a. No se puede hacer.
-refuse_recruit_3: Aléjate, voy a vomitar.
-recruit_msg: ¡Bien! Tengo que preguntar, ¿hay licor?
-enemy_hello: Hic! Tu rostro me da náuseas.
-be_attack: Espera, déjame despejarme.
-be_attack_enemy: Estoy trabajando. Espera un segundo, ¿eres mi objetivo? Gracias.</t>
-  </si>
-  <si>
-    <t>Like:工艺|珠宝
-Robber:100
-WildMonsterKiller:1
-Desc:Talat Hassan, un hábil herrero con un pasado problemático, solía trabajar en las peligrosas minas de Redstone Keep. Bajo la guía de un maestro, perfeccionó su oficio y aprendió el arte intricado de la herrería. Sin embargo, su inclinación por el alcohol y su comportamiento imprudente llevaron a un fatídico incidente que rompió sus lazos con la prestigiosa institución. A pesar de su innegable talento, la falta de sobriedad de Talat lo llevó a ofender al propio maestro que lo había mentorado.
-Determinado a encontrar su propio camino, Talat dio la espalda a la vida minera y adoptó un nuevo papel como mercenario disponible para contratar. Con su martillo de forja en mano y un espíritu atribulado en su interior, atraviesa el reino ofreciendo sus servicios como hábil herrero y combatiente capaz. Aunque atormentado por sus errores del pasado, las habilidades y la perseverancia de Talat siguen siendo insuperables, convirtiéndolo en un aliado muy buscado para aquellos que necesitan de su experiencia. Mientras avanza, Talat se esfuerza por superar sus demonios internos, con la esperanza de labrarse una nueva reputación como un respetado herrero y redimir su nombre manchado.
-Nature:kind=7,severe=3,honest=5,cunning=5,calm=2,anger=8,strong=5,weak=4
-fight_skills:冲刺膝盖顶|冲刺重拳|饮酒|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能呼延赭山</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: No me gustan muchas cosas, solo trinkets o instrumentos interesantes. Pero odio muchas cosas, especialmente las rosas blancas y las capas blancas.
-hello: El Sol Negro introdujo un poder primordial en el mundo. Los pensativos lo habrán despertado.
-refuse_recruit_0: No eres malo. Pero debo hacer una investigación importante primero.
-refuse_recruit_1: ¿Por qué debería estar de acuerdo cuando no tienes rastro de poder primordial?
-refuse_recruit_2: Lárgate de aquí. Eres tan molesto como un druida.
-refuse_recruit_3: ¡Déjame o serás estrangulado por mis enredaderas.
-recruit_msg: Bien. Tal vez haga un descubrimiento contigo.
-enemy_hello: ¡Tonto arrogante! Con solo mirarte puedo decir que no respetas la naturaleza.
-be_attack: ¡Contempla el poder de la naturaleza!
-be_attack_enemy: Muy bien. Te estaba buscando.</t>
-  </si>
-  <si>
-    <t>Like:秘宝|魔力
-Desc:Hu'ud, un mago originario de Amaranth Town, se ha convertido en un dedicado guardián de la naturaleza. Su motivación surgió cuando su madre cayó gravemente enferma, superando las posibilidades de curación mágica. Con la esperanza de encontrar una solución en el poder de la naturaleza, Hu'ud interpretó las visiones que le llegaban a través del Sol Negro como una señal de redención para el mundo. Convencido de que los espíritus primordiales podrían ser canalizados por los humanos, creyó en la posibilidad de utilizar dicho poder para curar todas las enfermedades humanas y traer sanación al mundo.
-Determinado a desentrañar los secretos de la magia de la naturaleza, Hu'ud se embarcó en un camino de estudio y práctica intensiva. A través de su dedicación, adquirió conocimientos profundos sobre el equilibrio y la armonía que rigen el mundo natural. Ahora, como guardián de la naturaleza, busca preservar y proteger los recursos naturales, utilizando su magia para sanar y restaurar el equilibrio en aquellos lugares afectados por la interferencia humana. Su deseo de utilizar su don mágico para el bien común lo impulsa a explorar nuevas formas de conectar con la esencia de la naturaleza y encontrar soluciones a los desafíos que enfrenta el mundo.
-Nature:kind=4,severe=6,honest=5,cunning=5,calm=7,anger=3,strong=5,weak=5
-fight_skills:冲刺膝盖顶|冲刺重拳|饮酒|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能胡褐</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Sin duda alguna, me encantan las &lt;color=red&gt;artesanías&lt;/color&gt;. Disfruto ver la emoción que un artesano pone en su trabajo. Cada artesanía tiene su propia alma.
-hello:(Tosidos seguidos de una risa) ¡Hola! tos Perdón, ¿qué dijiste?
-refuse_recruit_0:Pareces una persona muy sensata, pero... Lo siento.
-refuse_recruit_1:tos Perdóname. Simplemente no eres mi tipo.
-refuse_recruit_2:Jeje. Debes estar bromeando. ¿Tienes que preguntar de nuevo?
-refuse_recruit_3:No tengo nada que decirte.
-recruit_msg:Estoy seguro de que un humilde artesano como yo tiene muy poco que ofrecer. Muy bien. Es extraño ser tan admirado.
-enemy_hello:Tú y yo ahora somos enemigos. tos No deberías buscarme.
-be_attack:No me gusta discutir. tos
-be_attack_enemy:No hay otra opción. Prefiero no discutir.</t>
-  </si>
-  <si>
-    <t>Like:工艺
-Robber:100
-Desc:Antiguamente, él desempeñaba el oficio de fabricante de ladrillos en Cotta Town, pero perdió su empleo y su hogar durante la guerra. En busca de estabilidad, se convirtió en mercenario por un tiempo, pero con el paso de los años, anheló su antigua vida. Decidió regresar a Cotta Town y retomar su oficio de artesano. Aunque la vida sigue siendo difícil, ha encontrado paz en su labor artesanal. Ahora, trabaja con dedicación y disfruta de la tranquilidad que le brinda su trabajo.
-Nature:kind=7,severe=3,honest=5,cunning=5,calm=6,anger=4,strong=6,weak=4
-fight_skills:冲刺膝盖顶|冲刺重拳|饮酒|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能呼延鹿</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan los  &lt;color=red&gt;jueguetes&lt;/color&gt; &lt;color=red&gt;lindos&lt;/color&gt; ¡Jeje, hmm! También me gustan algunos tipos de &lt;color=red&gt;equipamiento especial&lt;/color&gt;.
-hello: ¡Hola, soy Muta'aliq!
-refuse_recruit_0: Pareces estar bien, pero... tengo que seguir buscando a mis padres.
-refuse_recruit_1: Gracias por la oferta, pero no puedo aceptarla.
-refuse_recruit_2: Ni siquiera te conozco.
-refuse_recruit_3: Bueno... en realidad, no me gustan mucho las personas como tú. Por favor, no me lo pidas de nuevo.
-recruit_msg: Está bien... Me uniré a ti. Espero que no te moleste mi presencia.
-enemy_hello: ¡No! ¡No te acerques más!
-be_attack: Así que realmente eres ese tipo de persona. Estoy decepcionado.
-be_attack_enemy: No me sorprende que hayas hecho eso.</t>
-  </si>
-  <si>
-    <t>Like:可爱|玩具|特殊装备
-Desc:Triptych Rock es el lugar más rico en minerales de Crying Rock. Durante la guerra, fue un campo de batalla y quedó devastado. Innumerables personas perdieron todo en la guerra. Muta'aliq nació en Triptych Rock. Sus padres eran metalúrgicos. En la guerra, sus padres fueron reclutados en los ejércitos y fueron llevados lejos de su amada hija, sin conocer su destino. Sin sus padres, Muta'aliq y su abuela dependieron el uno del otro. Trabajaron todos los días durante diez años, pero sus padres no regresaron. Cansada de esperar, Muta'aliq decidió emprender un viaje para encontrar a sus padres. Decidió aprender las artes arcanas y buscar al místico Furud. La leyenda dice que el Furud puede ver el futuro. Muta'aliq desea utilizar su poder para encontrar a sus padres.
-Su determinación la lleva a explorar los rincones más oscuros y misteriosos en busca del paradero de sus padres. Con cada paso, se sumerge en el mundo de la magia y los secretos antiguos. A medida que perfecciona sus habilidades arcanas, Muta'aliq se encuentra con aliados y enemigos inesperados en su camino. Su encuentro con el místico Furud es el punto de inflexión que podría revelar la verdad sobre el destino de sus padres. Con el poder de la visión del futuro a su alcance, Muta'aliq se enfrenta a desafíos y peligros para reunirse con su familia y encontrar la esperanza perdida en los tiempos de guerra. Su viaje está impulsado por la esperanza y la determinación de traer la luz a la oscuridad que ha plagado su vida y encontrar el amor y la unión perdidos en los escombros de la guerra.
-Nature:kind=7,severe=3,honest=6,cunning=4,calm=7,anger=3,strong=8,weak=2
-fight_skills:踩脚趾|直拳|冲刺膝盖顶|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能车瑾</t>
-  </si>
-  <si>
-    <t>Me apasiona el &lt;color=red&gt;combate&lt;/color&gt;, ¡es lo que más disfruto! Nada me hace más feliz que estar en medio de la batalla. Además, me encanta escuchar &lt;color=red&gt;cuentos&lt;/color&gt;. Desde que era pequeña, me fascinaba escuchar historias y leyendas.
-hello:¿Nunca has visto a una guerrera antes? No me mires así.
-refuse_recruit_0:Podrías ser un buen aliado, pero tengo asuntos pendientes que debo atender primero.
-refuse_recruit_1:Todavía no has demostrado tu valía.
-refuse_recruit_2:¿Estás bromeando?
-refuse_recruit_3:Di una palabra más y clavaré mi lanza en tu pecho.
-recruit_msg:¡Has ganado el respeto de Astrid la Sinjuramento!
-enemy_hello:Huye. Te daré tiempo para escapar.
-be_attack:¡Ja! Acepto tu desafío.
-be_attack_enemy:Eres un oponente formidable. ¡Yo, Astrid, acepto con gusto tu desafío!</t>
-  </si>
-  <si>
-    <t>Like:格斗|故事
-WildMonsterKiller:1
-Desc:Astrid era una joven que amaba luchar. Fue elegida por un joven noble de los Nephrit para convertirse en su esposa. El noble le prohibió a Astrid practicar con armas... o abandonar su mansión. Un día, el jefe de servicio de la mansión del noble descubrió que este había sido secuestrado por bandidos, quienes exigían una fortuna en Utar a cambio de la vida del noble. Miembros prominentes de los Nephrit se oponían a gastar tanto para rescatar a una sola persona. Con la vida de su amado en peligro, Astrid ignoró la orden de quedarse en casa y, por sí sola, rescató a su esposo. Al regresar a los Nephrit, su esposo la acusó falsamente de coludir con los bandidos. Angustiada, Astrid llevó a su esposo ante el líder de la tribu para anular su matrimonio. Así, Astrid se convirtió en una leyenda en el desierto. Fue la primera mujer en poner fin públicamente a un matrimonio. Poco después, Astrid retomó su pasión anterior y se convirtió en una guerrera.
-Nature:kind=6,severe=4,honest=7,cunning=3,calm=3,anger=7,strong=10,weak=0
-fight_skills:蓄力冲刺|冲刺重拳|头槌|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能安红砂</t>
-  </si>
-  <si>
-    <t>Me gustan las cosas &lt;color=red&gt;románticas&lt;/color&gt;, los &lt;color=red&gt;instrumentos&lt;/color&gt; y algunos &lt;color=red&gt;juguetes divertidos&lt;/color&gt;. Lo siento, sé que sueno un poco ingenuo.
-hello: ¡Hola! ¿Necesitas ayuda?
-refuse_recruit_0: Me gustaría ayudarte, pero hay otras personas que me necesitan.
-refuse_recruit_1: Lo siento, no hay nada que pueda hacer por ti.
-refuse_recruit_2: No puedo, hay otras cosas que debo hacer.
-refuse_recruit_3: Eres una persona malvada, no quiero tener nada que ver contigo.
-recruit_msg: ¡Espero que las rosas blancas florezcan en cada rincón del mundo!
-enemy_hello: Oh, espero que nuestros bandos puedan comunicarse más.
-be_attack: ¿De verdad vas a hacer esto? Esperaba que pudiéramos ser amigos.
-be_attack_enemy: No tiene sentido. No puedo negarle nada a los demás.</t>
-  </si>
-  <si>
-    <t>Like:玩具|浪漫|乐器
-Desc:La Sociedad de la Rosa Blanca es la fuente de todos los sanadores en esta tierra. Riq es la hija del líder de la Sociedad de la Rosa Blanca. Todos los miembros de la Sociedad de la Rosa Blanca tienen un símbolo de rosa en la parte posterior de sus cuellos. Este símbolo de rosa se utiliza para supervisar la magia de curación de la sociedad, para garantizar el control sobre el precio y el estatus de cada sanador y la magia a su disposición. De esta manera, Riq es única entre los sanadores porque tiene una libertad que ni siquiera los magos de nivel más alto de la sociedad pueden disfrutar. Riq no entendía la razón del estricto control de la Sociedad de la Rosa Blanca, así que su padre le dijo que dejara los sagrados salones de la Sociedad para ver este mundo devastado con sus propios ojos y así aprender el valor de ser una sanadora y tener una comprensión más profunda.
-Nature:kind=9,severe=1,honest=7,cunning=3,calm=6,anger=4,strong=2,weak=8
-fight_skills:踩脚趾|直拳|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能曲玉</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me encantan las &lt;color=red&gt;artesanías&lt;/color&gt; como escudos y estatuas. Estas creaciones tienen un encanto místico que me fascina.
-招募对话: Normalmente prefiero no unirme a otros, pero si estás dispuesto a invertir Utar para contratarme... quizás pueda reconsiderarlo.
-hello:... ¿En qué puedo ayudarte?
-refuse_recruit_0:... Lo siento, pero no puedo.
-refuse_recruit_1:No me convence.
-refuse_recruit_2:No, gracias.
-refuse_recruit_3:Lárgate, no tengo interés.
-recruit_msg:... Está bien, contaré contigo. Espero que no me decepciones.
-enemy_hello:Tú y yo somos enemigos ahora.
-be_attack:¡A la batalla, entonces!
-be_attack_enemy:Lo pediste.</t>
-  </si>
-  <si>
-    <t>Like:工艺
-Robber:100
-WildMonsterKiller:1
-Desc:El Águila Solitaria, como su nombre sugiere, es un viejo águila solitario que surca los cielos del desierto. Tiene un parche en el ojo que cubre una cicatriz. Su otro ojo tiene un extraño color dorado, lo que sugiere una misteriosa ascendencia. Es callado y nunca habla sobre su pasado. La gente lo reconoce mejor por el sonido metálico de sus pasos y el halcón que lleva consigo.
-Nature:kind=5,severe=5,honest=5,cunning=5,calm=8,anger=2,strong=7,weak=3
-fight_skills:蓄力冲刺|冲刺重拳|头槌|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能独孤鹰</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Hm, ¿carne de Ifrit a la parrilla? ¿O pollo asado? Aunque esos no saben bien fríos. ¿Qué más me gusta además de la comida... oh! &lt;color=red&gt;Artesanías&lt;/color&gt; y atlas de &lt;color=red&gt;geografía&lt;/color&gt;. Deseo viajar por el mundo algún día.
-hello:¡Ahoy, hola, hola! Soy un mago, no un guerrero.
-refuse_recruit_0:¿Eh? ¿Una invitación para mí? Ah... no, aún no es el momento.
-refuse_recruit_1:¿Quieres mi ayuda? Claro. ¿Qué? ¿Quieres mi ayuda por cuánto tiempo? Déjame pensar.
-refuse_recruit_2:No, no, no. Tengo que estar en casa para la cena.
-refuse_recruit_3:Lamentablemente, Kunju no puede ir contigo.
-recruit_msg:¡Ah, bien! ¡Lucharemos juntos! ¿Quién dice que un hombre de mi estatura no puede ser un mago?
-enemy_hello:¡Ahoy! ¡Hola hola-oh! Eres tú. No puedo hablar contigo.
-be_attack:¿Eh! ¿Hice algo mal?
-be_attack_enemy:¡Llegas justo a tiempo! Tengo un nuevo hechizo que quiero probar... De hecho, lo aprendí hace mucho tiempo.</t>
-  </si>
-  <si>
-    <t>Like:工艺|地理
-WildMonsterKiller:1
-Desc:Kunju es un excéntrico y torpe mago. A simple vista, nadie podría sospechar su verdadero potencial mágico. Sus padres eran magos excepcionalmente talentosos en Amaranth Town, pero debido a la creciente presión del círculo druídico local, decidieron dejar su hogar y establecerse en Camel Bell Bazaar. Para Kunju, el bullicioso bazar resultó mucho más atractivo que la monotonía de los magos en Amaranth Town. Allí encontró personas fascinantes y experiencias emocionantes que alimentaron su pasión por la magia.
-Nature:kind=9,severe=1,honest=9,cunning=1,calm=4,anger=6,strong=3,weak=7
-fight_skills:蓄力冲刺|冲刺重拳|头槌|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能昆鹫</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me encantan las &lt;color=red&gt;pinturas&lt;/color&gt; y los &lt;color=red&gt;cuentos&lt;/color&gt;... Estas cosas me hacen olvidar las partes más desagradables de la vida. No me gusta nada más.
-hello:Soy Hartum de Diresprings.
-refuse_recruit_0:... No, mis padres se negarían.
-refuse_recruit_1:No puedo unirme a ti. Lo siento.
-refuse_recruit_2:Hartum baja la cabeza
-refuse_recruit_3:¡Vete de aquí! Déjame solo.
-recruit_msg:Espero no ser una molestia para ti.
-enemy_hello:Dime lo que tienes que decir.
-be_attack:¿Otro enemigo? No me sorprende.
-be_attack_enemy:No está en nuestro destino ser compañeros. Disculpas.</t>
-  </si>
-  <si>
-    <t>Like:绘画|故事
-Desc:La familia de Hartum eran comerciantes en el Bazar Dorado. Cuando comenzó la guerra, su familia escapó a Diresprings. En Diresprings, comenzaron una nueva vida, pero a medida que la guerra se extendía, los bandidos saquearon su hogar. Muchos de los ricos perdieron todo lo que tenían, incluidos los amigos cercanos de su familia. Sin embargo, los padres de Hartum se negaron a ayudarlos para asegurar que su hijo tuviera una buena vida, lo que generó un gran resentimiento. Hartum comprendía que sus padres actuaban en su mejor interés, pero no podía dejar de sentirse culpable. Se siente incómodo con su vida cómoda.
-Nature:kind=6,severe=4,honest=6,cunning=4,calm=5,anger=5,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能何风</t>
-  </si>
-  <si>
-    <t>Like:历史|神秘
-Desc:Isa, la sabia de Diresprings, es una buscadora incansable de conocimiento y reliquias antiguas. Ha recorrido los rincones más remotos de la tierra en busca de tecnología perdida y fragmentos de sabiduría ancestral. Su pasión por el pasado la impulsa a ayudar a otros a reconstruir sus hogares utilizando los secretos ocultos en esas antiguas reliquias.
-Sin embargo, el anhelo más profundo de Isa va más allá de la mera recuperación de artefactos. Sueña con un mundo en el que los poderosos abandonen las armas y se comprometan con el desarrollo científico. Cree fervientemente que la ciencia y el conocimiento son las verdaderas herramientas para garantizar la estabilidad y la felicidad de todos los habitantes de la tierra. Con su sabiduría y determinación, Isa trabaja incansablemente para difundir la importancia de la educación y el progreso científico, en busca de un futuro mejor para todos.
-Nature:kind=8,severe=2,honest=5,cunning=5,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能伊孤</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me interesa principalmente la &lt;color=red&gt;Historia&lt;/color&gt;. De vez en cuando, también me despiertan curiosidad algunos objetos &lt;color=red&gt;ocultos&lt;/color&gt;.
-招募对话: Prefiero ser solitaria, a menos que estés dispuesto a financiar mi investigación con algo de Utar... o puedes cambiar mi opinión.
-hello: Hay demasiados desconocidos en este desierto.
-refuse_recruit_0: Podrías ser un buen recurso para estudiar materiales antiguos. Pero... hah. Olvídalo. Es algo que debo hacer por mi cuenta.
-refuse_recruit_1: Hm. No es suficiente. No pareces lo suficientemente inteligente.
-refuse_recruit_2: Escucha, viejo, tengo otras cosas que hacer.
-refuse_recruit_3: Troglodita. ¿No tienes algo interesante que decirme?
-recruit_msg: Muy bien. Tu equipo podría beneficiarse de una persona erudita para variar.
-enemy_hello: ¿No estás buscando problemas, verdad?
-be_attack: Lee un libro; te hará menos imprudente.
-be_attack_enemy: Son tontos como tú los que obstaculizan el progreso.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Quieres saber qué les gusta a los segadores de almas del desierto? Sobrevivimos solo con humor negro... y en realidad, los tesoros &lt;color=red&gt;ocultos&lt;/color&gt;  y el  &lt;color=red&gt;equipo especial&lt;/color&gt; no están mal.
-hello: ¿Has visto al líder de los Corsac?
-refuse_recruit_0: Tú y yo somos muy parecidos, pero aún me debes algo.
-refuse_recruit_1: El olor a sangre no es lo suficientemente fuerte en ti.
-refuse_recruit_2: ¡Ja, ja! ¡En tus sueños!
-refuse_recruit_3: ¿Quieres ser un alma que coseche?
-recruit_msg: ¡Cazaremos juntos!
-enemy_hello: ¿Estás trabajando con los Corsac? Sé honesto/a.
-be_attack: ¡Mataré a tus descendientes y a Khurram Aslae también!
-be_attack_enemy: ¡Yaaaaah! ¡Vamos entonces!</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Bueno, me gustan la &lt;color=red&gt;cultura&lt;/color&gt;, los &lt;color=red&gt;tesoros&lt;/color&gt; y el &lt;color=red&gt;equipo especial&lt;/color&gt;. ¡También me gusta la justicia para todas las personas en el mundo!
-hello: ¡La justicia prevalecerá!
-refuse_recruit_0: El desierto necesita talentos como tú, pero es una pena que este viejo esté volviéndose rígido. No quiero ir demasiado lejos.
-refuse_recruit_1: ¡Gracias por la invitación! Soy demasiado viejo para partir.
-refuse_recruit_2: No puedo, tengo cosas importantes que hacer.
-refuse_recruit_3: Deberías huir y no pronunciar palabras tan descabelladas.
-recruit_msg: Actúa con justicia y la justicia te seguirá.
-enemy_hello: No negocia con bandidos.
-be_attack: Parece que mi nombre solo no es suficiente para asustarte.
-be_attack_enemy: ¡Ja! ¿Crees que un viejo como yo se asustaría de un joven como tú?</t>
-  </si>
-  <si>
-    <t>Like:神秘|文学|特殊装备
-WildMonsterKiller:1
-Desc:Alaf Jahim era apenas un joven cuando llegó al Gran Desierto para ganarse la vida como escolta de caravanas. Hoy en día, es ampliamente conocido como músculo a sueldo. Ha escoltado a innumerables viajeros y ha derrotado a demasiados bandidos para contarlos. Pero el tiempo no ha perdonado a este héroe. Alaf Jahim tiene ahora más de 60 años y no posee la misma energía que en su juventud. Las tareas de escolta más difíciles se escapan lentamente de su alcance, pero su nombre todavía infunde miedo en los corazones de los bandidos. Su estatus legendario entre las arenas perdura.
-Nature:kind=5,severe=5,honest=8,cunning=2,calm=6,anger=4,strong=10,weak=0
-fight_skills:冲刺重拳|升龙拳|吼叫|饮酒|绝技裂地
-fight_dgskill:刺拳,1
-AssSkill:统率技能赫连千百</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Prefiero no ser molestado. Considerar lo que me gusta es un poco molesto. Hm... Si tienes que preguntar, probablemente sean libros llenos de &lt;color=red&gt;cuentos&lt;/color&gt; o &lt;color=red&gt;artesanías&lt;/color&gt;.
-hello:Ah... qué molestia.
-refuse_recruit_0:Recibo tan pocas visitas, pero no quiero moverme.
-refuse_recruit_1:Es demasiado problema. Olvídalo.
-refuse_recruit_2:Me niego. No quiero meterme en aguas turbias.
-refuse_recruit_3:Será mejor que te calles.
-recruit_msg:Qué molestia... ¡Ay! Bien. Bien. Puedo ver que eres muy sincero/a.
-enemy_hello:Deja de molestarme.
-be_attack:Dije que dejes de molestarme.
-be_attack_enemy:¿Así que quieres "arreglar las cosas", eh?</t>
-  </si>
-  <si>
-    <t>Like:故事|工艺
-WildMonsterKiller:1
-Desc:Makan es un trabajador de poca reputación. Es un poco perezoso y cobarde, pero constantemente encuentra trabajo debido a su habilidad en las reparaciones. Odia a aquellos que saquean y destruyen porque les genera más trabajo.
-Makan posee un talento innato para las reparaciones, aunque su habilidad es subestimada. Es conocido como la persona a la que acudir cuando algo necesita ser arreglado. Su especialidad radica en restaurar estructuras y objetos dañados, ya sean edificios, maquinarias o incluso artefactos delicados. Su atención meticulosa a los detalles y su capacidad para revivir cosas rotas lo han convertido en alguien indispensable para aquellos que valoran su artesanía.
-En el fondo, Makan alberga un profundo resentimiento hacia aquellos que se dedican al saqueo y la destrucción. Desprecia el caos que dejan a su paso, ya que no solo perturba la paz, sino que también crea más trabajo para él al tener que reparar los daños ocasionados. 
-Nature:kind=5,severe=5,honest=4,cunning=6,calm=5,anger=5,strong=3,weak=7
-fight_skills:冲刺重拳|升龙拳|吼叫|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能何疆</t>
-  </si>
-  <si>
-    <t>Like:特殊装备|神秘
-Robber:100
-Desc:Bataru nació en los Acantilados de Umbra, pero no estaba satisfecho con la vida como granjero allí. Viajó al Gran Desierto y se unió al Gremio de Mercaderes Corsac. Mientras cobraba una deuda, mató a un hombre, traicionando las reglas del Corsac. Bataru fue excomulgado del Gremio de Mercaderes Corsac y exiliado para siempre de Dunestorm. Después de ser exiliado, Bataru comenzó a odiar al Corsac. Se volvió cada vez más violento y sediento de poder, hasta convertirse en un temido y despiadado bandido del desierto con un único objetivo: matar al insensato líder del Corsac.
-Nature:kind=2,severe=8,honest=3,cunning=7,calm=2,anger=8,strong=8,weak=2
-fight_skills:冲刺重拳|升龙拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能巴塔鲁</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Me gustan las canciones &lt;color=red&gt;románticas&lt;/color&gt; o &lt;color=red&gt;tristes&lt;/color&gt;. A mi esposa le gusta escucharlas también.
-hello:La magia de curación... muy importante.
-refuse_recruit_0:Te admiro, pero eso no es suficiente.
-refuse_recruit_1:No puedo hacerlo. Tengo órdenes.
-refuse_recruit_2:Espero que estés bromeando.
-refuse_recruit_3:Es una lástima que mi magia de curación no pueda arreglar lo que está mal en tu cabeza.
-recruit_msg:Muy bien. Informaré a la Sociedad de mi partida.
-enemy_hello:Ríndete ahora y se garantiza tu protección como prisionero.
-be_attack:Tus tonterías no se pueden curar con arcana, solo la hoja podrá hacerlo.
-be_attack_enemy:Ruega a la Diosa del Río para que tus heridas no sean demasiado graves. No me interesa verte suplicar por piedad.</t>
-  </si>
-  <si>
-    <t>Like:浪漫|忧伤|音乐
-Desc:Yousef era un espadachín de los Nasir hasta que su esposa falleció hace tres años a causa de una enfermedad grave. Debido a un desacuerdo entre la Sociedad de la Rosa Blanca y los Nasir, la Sociedad retiró a todos sus magos curanderos de los Nasir. Sin los magos curanderos de la Sociedad de la Rosa Blanca, muchos Nasir murieron por enfermedades o heridas graves, incluyendo, por supuesto, la esposa de Yousef. Después de su fallecimiento, Yousef adquirió un profundo aprecio por la magia curativa y se acercó a la Sociedad de la Rosa Blanca para recibir entrenamiento en las artes de la curación.
-Nature:kind=7,severe=3,honest=5,cunning=5,calm=8,anger=2,strong=3,weak=7
-fight_skills:冲刺重拳|升龙拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能齐肃之</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:No hay nadie que pueda resistirse a un &lt;color=red&gt;cuento romántico&lt;/color&gt;. ¡Así como nadie puede resistirse a un noble joven generoso y elegante!
-hello:Deja de mirar, ¿hay algo mal con tus ojos?
-refuse_recruit_0:Jajaja, ¿otro ha sucumbido a mis encantos? Por supuesto. ¡Por supuesto! Sin embargo... estoy bastante emocionado por ver qué más tienes para ofrecer.
-refuse_recruit_1:¿Ah? ¿Crees que un noble se puede comprar y vender tan fácilmente?
-refuse_recruit_2:Lamentablemente, otro admirador obsesionado. Permíteme decirte lentamente para que entiendas: Yo. Me niego.
-refuse_recruit_3:Oh, odio ser cruel, pero eres el tipo de persona que detesto absolutamente.
-recruit_msg:Mi respuesta es... ¡sí! ¡Por supuesto!</t>
-  </si>
-  <si>
-    <t>Like:故事|浪漫
-Desc:El líder de la famosa Casa Kabir. La Casa Kabir es una de las familias más ricas del desierto después de generaciones de trabajar en la industria minera. Además de su inmensa riqueza, la Casa Kabir es conocida por un talento arcano especial: la capacidad de controlar el oro. Cualquier cosa hecha de oro puede ser un arma para la Casa Kabir. Cada miembro de la Casa tiene su propia arma personal de oro. A Goldie le gusta especialmente una bolsa llena de hojas doradas. Por lo general, no hay forma de recuperar tal arma, pero el joven líder de la Casa Kabir no se preocupa por el dinero. Goldie tiene una hermana diez años menor que él. Adora a su hermana menor, pero ella no parece apreciar a su hermano grandioso.
-Nature:kind=7,severe=3,honest=2,cunning=8,calm=6,anger=4,strong=5,weak=5
-fight_skills:冲刺重拳|升龙拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能金足赤</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Antes que nada, no me gusta nada de lo que le gusta a ese estúpido de Goldie! ¡Hmph! ¡Me gustan los &lt;color=red&gt;juegos&lt;/color&gt; &lt;color=red&gt;lindos&lt;/color&gt;! ¡O hermosos &lt;color=red&gt;instrumentos&lt;/color&gt; que suenen!
-hello: Ding-ding-dong, ¡no me molestes!
-refuse_recruit_0: ¡Hmph! Lo pensaré... lo pensaré...
-refuse_recruit_1: ¡Ugh, deja de intentarlo! ¡No va a suceder!
-refuse_recruit_2: ¡No lo haré! ¡No me dejaré usar por nadie! ¡Hmph!
-refuse_recruit_3: ¡Qué molesto! ¡Eres tan molesto como Goldie! ¡Te odio!
-recruit_msg: ¡Hmph! ¡Bien! Sigues preguntando una y otra vez, ¡es realmente molesto!
-enemy_hello: Deja de molestarme. No quiero hablar contigo.
-be_attack: ¡Ugh! ¡Eres la persona más molesta que he conocido hoy!
-be_attack_enemy: ¡Ding-dong, ding-dong, ahora estás en problemas!</t>
-  </si>
-  <si>
-    <t>Like:玩具|可爱|乐器
-Desc:Lotus, miembro de la Casa Kabir, posee un don extraordinario para la magia que supera incluso a los practicantes más hábiles. Sin embargo, su poder es indómito y volátil, causando caos y destrucción dondequiera que vaya. La campana dorada que empuña actúa como un conducto para su magia, amplificando su potencia pero también magnificando su naturaleza impredecible. Temiendo las repercusiones de sus habilidades incontroladas, Lotus tomó la difícil decisión de abandonar su hogar y embarcarse en una búsqueda para encontrar la manera de dominar su magia y aprovechar su potencial para el bien.
-Durante su viaje, Lotus se encuentra con seres místicos ancestrales y busca la guía de sabios sabios y magos experimentados. Aprende de rituales antiguos y conocimientos prohibidos que podrían desvelar los secretos para controlar su inmenso poder. En el camino, enfrenta numerosos desafíos y pruebas, tanto internas como externas, mientras lucha con sus propios demonios internos y se esfuerza por encontrar su verdadero propósito. A pesar de los riesgos y dificultades que enfrenta, Lotus está determinada a encontrar el equilibrio y convertirse en una portadora responsable de sus formidables habilidades mágicas, con la esperanza de utilizar sus poderes para proteger y traer armonía al mundo.
-Nature:kind=9,severe=1,honest=7,cunning=3,calm=5,anger=5,strong=1,weak=9
-fight_skills:踩脚趾|直拳|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能金玉叶</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Hm... Me gustaría aprender &lt;color=red&gt;geografía&lt;/color&gt;.
-hello:Te encontraré, padre.
-refuse_recruit_0:Eres muy amable, pero aún debo buscar a mi padre.
-refuse_recruit_1:No puedo, gracias por entender.
-refuse_recruit_2:Ya debes saber que te rechazaré.
-refuse_recruit_3:¡No quiero verte!
-recruit_msg:Esta espada me fue dada por mi padre. Espero no decepcionarlo. Iré contigo.</t>
-  </si>
-  <si>
-    <t>Like:地理
-WildMonsterKiller:1
-Desc:El padre de Saqie es un famoso guerrero Nasir. Hace veinte años, se le ordenó a su padre destruir a los Oryx. Sin embargo, él era de buen corazón y sabía que los Oryx eran viejos y débiles, al borde de la derrota. Otro ataque contra ellos sería como una carnicería. Tras mucha deliberación, el padre de Saqie decidió llevarse a Saqie y huir. Fueron marcados como traidores y desertores por los Nasir. Guerreros los persiguieron, con la esperanza de cobrar una recompensa. Saqie y su padre estuvieron huyendo durante cinco años hasta que un día, su padre desapareció sin dejar rastro. Saqie no creía que su padre simplemente hubiera desaparecido, así que tomó la espada de su padre y emprendió un viaje para encontrarlo.
-Nature:kind=4,severe=6,honest=5,cunning=5,calm=3,anger=7,strong=8,weak=2
-fight_skills:踩脚趾|直拳|飞腿|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能独孤霜</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Me gustan las cosas &lt;color=red&gt;románticas&lt;/color&gt; y &lt;color=red&gt;ocultas&lt;/color&gt;. ¡Y todo lo relacionado con la hermosa &lt;color=red&gt;diosa&lt;/color&gt; es una maravillosa obra de arte!
-hello:¡Rojo! ¡La esencia de este mundo!
-refuse_recruit_0:Si te cambias de ropa carmesí, tal vez lo considere.
-refuse_recruit_1:¿Oh? ¿Quieres que trabaje para ti? No me estás ofreciendo lo suficiente como para considerarlo.
-refuse_recruit_2:¿Por qué quieres que te ayude?
-refuse_recruit_3:¡Jajaja! Mira, seguramente eres la peor creación del Creador.
-recruit_msg:Teñiré el mundo de rojo sangre por ti.</t>
-  </si>
-  <si>
-    <t>Like:浪漫|女神|神秘
-WildMonsterKiller:1
-Robber:100
-Desc:Nabiha, apodado el Artista Carmesí o el Loco Rojo, disfruta de los colores más finos y los objetos más elegantes. Es un espíritu libre e impredecible, que actúa ocasionalmente movido por un sentido de rectitud, pero sin principios estrictos que lo guíen. Simplemente hace lo que le place. No es una buena persona, pero tampoco es del todo mala. Nabiha busca su propio sentido de valor artístico, así como el alma artística de la tierra. Cree firmemente que el mundo eventualmente se teñirá de su color favorito, y solo entonces se convertirá en una obra de arte suprema.
-Nature:kind=5,severe=5,honest=5,cunning=5,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能舒禹舟</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Los escaladores disfrutan de &lt;color=red&gt;leer&lt;/color&gt; o escuchar &lt;color=red&gt;historias&lt;/color&gt;.
-hola: Todas las respuestas se encuentran en la cima de una montaña.
-refuse_recruit_0: Me gustaría acompañarte, pero Ilyas está esperándome.
-refuse_recruit_1: Aún no he escalado la cumbre más alta de la cadena más oriental. No tengo tiempo para nada más.
-refuse_recruit_2: Hmph. No tengo una respuesta para ti.
-refuse_recruit_3: ¡No te confíes demasiado!
-recruit_msg: Muy bien. Tal vez encuentre nuevas formas de ejercitarme.</t>
-  </si>
-  <si>
-    <t>Like:故事|文学|地理
-Desc:Sur es un famoso montañista de las montañas alpinas. Tiene un compañero al que llama "Ilyas", aunque pocos saben que este delicado nombre en realidad es un piolet de escalada encantado. Para Sur, un piolet de escalada es un compañero en situaciones de vida o muerte. Sur es un montañista profesional. Trabaja duro para entrenarse y enfrentar montañas aún más altas. El objetivo más grande de Sur es la gran montaña hacia el este: Ilyas.
-Nature:kind=5,severe=5,honest=6,cunning=4,calm=7,anger=3,strong=9,weak=1
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能石哈</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Vas a apostar conmigo? Me gustan las &lt;color=red&gt;joyas&lt;/color&gt; o cosas que &lt;color=red&gt;eleven mi moral en la batalla&lt;/color&gt;.
-hello:¿Quieres apostar conmigo?
-refuse_recruit_0:Juguemos una partida. Iré contigo si ganas. Mmm... no pareces tener nada que darme si pierdes. Olvídalo.
-refuse_recruit_1:¿Alguien como tú quiere que me una?
-refuse_recruit_2:¡Jajaja! Vete al infierno.
-refuse_recruit_3:¡Me recuerdas a aquel que me lo quitó todo! ¡Lárgate!
-recruit_msg:Está bien. Jugaré una partida contigo.</t>
-  </si>
-  <si>
-    <t>Like:珠宝|格斗
-Robber:100
-Desc:Mousa era un fantástico apostador cuando era joven, con una suerte aparentemente ilimitada. Como tal, tenía dinero, estatus, mujeres y una vida muy extravagante. Un día, Mousa recibió un desafío. El retador era un guerrero de las Montañas Zagros, quien reunió toda la riqueza de su tribu para apostarlo todo contra Mousa. Arrogantemente, Mousa aceptó, creyendo que su oponente era un tonto. Pero durante la batalla, no solo Mousa perdió todo, sino que su oponente le cortó ambas manos... En un estado de desesperación, Mousa encontró al técnico Infan. Infan le colocó taladros en los muñones de los brazos de Mousa. Ahora Mousa está armado con armas extremadamente poderosas. Después de renacer, Mousa todavía tiene un problema con el juego, pero ahora solo apuesta por una cosa: el Destino.
-Nature:kind=2,severe=8,honest=1,cunning=9,calm=3,anger=7,strong=9,weak=1
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒|绝技裂地
-fight_dgskill:刺拳,1
-AssSkill:统率技能完颜黑</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan las cosas &lt;color=red&gt;tristes&lt;/color&gt; que resuenan con mi alma. Además de eso, espero encontrar &lt;color=red&gt;equipamiento especial&lt;/color&gt; que pueda ayudarme en la batalla.
-hello:El estilo de lucha de mi familia nunca morirá mientras yo esté presente.
-refuse_recruit_0:Sabes que cargo con una gran responsabilidad. No puedo aceptar.
-refuse_recruit_1:Tú no eres el tipo de persona que admiro.
-refuse_recruit_2:No, y no vuelvas a preguntar.
-refuse_recruit_3:No puedo controlar mi ira por mucho más tiempo. Vete ahora.
-recruit_msg:Está bien. Espero que puedas dar a conocer mi estilo de lucha al mundo entero.</t>
-  </si>
-  <si>
-    <t>Like:特殊装备|忧伤
-WildMonsterKiller:1
-Desc:Mathali nació en una familia inmersa en la guerra. Los miembros de la familia podían usar el maná para potenciar sus espadas. Cuando comenzó la guerra, la familia de Mathali, que solo se destacaba en duelos, fue ignorada. Muchos miembros de la familia tuvieron que encontrar nuevas carreras. Sus técnicas de combate únicas estaban al borde de perderse para siempre. Mathali es el único joven de su generación que ha aprendido a utilizar el maná para luchar. Sobre sus hombros recae no solo la carga de revivir la gloria de la familia, sino también la misión de transmitir estas artes secretas.
-Nature:kind=8,severe=2,honest=5,cunning=5,calm=6,anger=4,strong=8,weak=2
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能韩靖</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gusta cuando las personas están &lt;color=red&gt; tristes&lt;/color&gt; y sufren. También me gusta pasar tiempo contemplando &lt;color=red&gt; pinturas&lt;/color&gt;.
-hello: Me gusta tu expresión melancólica...
-refuse_recruit_0: Hey, aún no has llegado lo suficientemente lejos.
-refuse_recruit_1: Ah... todavía no es suficiente para que me arrodille.
-refuse_recruit_2: Estás delirando.
-refuse_recruit_3: Ni siquiera vales la pena ser triturado para obtener componentes arcanos.
-recruit_msg: Espero que puedas ayudarme a cosechar más dolor y sufrimiento.</t>
-  </si>
-  <si>
-    <t>Like:绘画|忧伤
-WildMonsterKiller:1
-Robber:100
-Desc:Sanjay, un poderoso y enigmático mago, proviene de un reino distante envuelto en misterio. Impulsado por una curiosidad insaciable, atravesó tierras peligrosas y cruzó reinos traicioneros para llegar a esta tierra, atraído por los rumores de un poder arcano sin explotar oculto en el caos de la guerra. Su búsqueda de conocimiento prohibido lo llevó a sumergirse en rituales oscuros y textos prohibidos, buscando desentrañar los secretos de cómo aprovechar la energía cruda generada por el dolor y la tragedia.
-A medida que se adentraba más en su investigación, la brújula moral de Sanjay comenzó a difuminarse y su obsesión por el poder lo consumió. Se obsesionó con la idea de manipular la esencia misma del sufrimiento, aprovechando su energía para alimentar sus propias habilidades arcanas. Con cada experimento, se fue distanciando más de la difícil situación de los demás, viendo su dolor como mera fuente para su propio avance. Ahora, deambula por la tierra como una figura temida y fascinante, impulsado por su incansable búsqueda de conocimiento prohibido y su insidioso deseo de dominar las artes oscuras de extraer poder arcano de los rincones más oscuros del sufrimiento humano.
-Nature:kind=2,severe=8,honest=2,cunning=8,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能萨加</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:No tengo amor por nada en este mundo. Sin embargo, me interesa la &lt;color=red&gt;historia&lt;/color&gt;, los &lt;color=red&gt;cuentos&lt;/color&gt; y encontrar el equilibrio.
-hello: Equilibrio para todos.
-refuse_recruit_0: ¿Yo? ¿Seguirte? Hm, no, eso no puede ser correcto.
-refuse_recruit_1: No quiero perturbar las aguas tranquilas.
-refuse_recruit_2: Eso no sería justo, ¿verdad?
-refuse_recruit_3: ... Te destruiré.
-recruit_msg: Bien, juntos haremos del mundo un lugar más justo.</t>
-  </si>
-  <si>
-    <t>Like:历史|故事
-Desc:Zafeera siempre lleva consigo escalas de plata en sus deambulaciones sin rumbo. Se enorgullece de su naturaleza pacífica. No es una maga que mata, pero sigue siendo una pesadilla para los aldeanos cercanos. Si Zafeera ve a alguien con un pantalón remangado en una pierna, entonces remangará el otro lado. Si ve a alguien con la mitad del cabello faltante, entonces lo afeitará de forma gratuita. Si ve a alguien sin un brazo, entonces Zafeera cortará el otro brazo. Su comportamiento errático no se basa en su estado de ánimo en ese momento ni en ninguna otra circunstancia, sino en la búsqueda de su idea de "equilibrio". Su compromiso con el equilibrio es extremo y nunca deja de buscarlo.
-Nature:kind=5,severe=5,honest=5,cunning=5,calm=9,anger=1,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能韦利纳</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan &lt;color=red&gt;la música&lt;/color&gt; y algunas cosas &lt;color=red&gt;tristes&lt;/color&gt; o &lt;color=red&gt;románticas&lt;/color&gt;. Las emociones son muy importantes para un bailarín.
-hello: ¡Me gusta bailar! Algún día bailaré en el gran escenario de la ciudad de Jamal.
-refuse_recruit_0: Creo que nos llevamos muy bien, pero... No renunciaré a mi sueño por ti.
-refuse_recruit_1: Me gusta bailar. Si quieres que luche... lo siento.
-refuse_recruit_2: ¿Estás hablando en serio? Está bien, si solo estabas bromeando.
-refuse_recruit_3: Bueno, no voy a mentirte. No me caes muy bien.
-recruit_msg: Eres digno de seguir. Vamos, espero que me aconsejes en el futuro.</t>
-  </si>
-  <si>
-    <t>Like:音乐|浪漫|忧伤
-Desc:Ella a menudo baila junto al río, su reflejo en el agua es su único público. Desde que era niña, Umara soñaba con convertirse en una bailarina real. Cuando el viejo rey fue derrocado, los Nasir ocuparon la ciudad de Jamal, la antigua capital. A medida que la guerra no terminaba y los combates continuaban, la ciudad de Jamal permanecía en constante alerta. Umara ni siquiera sabía cómo lucía Jamal City, ni tenía los documentos necesarios para ir allí. Aun así, Umara practica todos los días para poder unirse al grupo de artistas más famoso de la ciudad y convertirse en una bailarina profesional. Cuando ella esté en el escenario más grandioso de la tierra, el público bajo sus pies conocerá la mayor felicidad.
-Nature:kind=7,severe=3,honest=8,cunning=2,calm=5,anger=5,strong=7,weak=3
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能希云娜</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：¡Me gusta la &lt;color=red&gt;cultura&lt;/color&gt; y la &lt;color=red&gt;música&lt;/color&gt;! ¿Vas a darme un regalo?
-hello:¿Soy un guardabosques o un boticario? ¡Soy ambos!
-refuse_recruit_0:No te preocupes, déjame pensarlo, ¿de acuerdo?
-refuse_recruit_1:Lo he pensado, pero por ahora debo rechazarlo.
-refuse_recruit_2:Lo siento, debo rechazar tu invitación. Espero que no estés muy decepcionado.
-refuse_recruit_3:No, no pareces gustar mucho de los boticarios.
-recruit_msg:Te advierto de antemano que puedo ser un poco complicado. ¡Espero que estés bien con eso!
-enemy_hello:No te metas con el suministro de un boticario.
-be_attack:Realmente me has decepcionado.
-be_attack_enemy:Serás un excelente sujeto de prueba para mi nueva poción.</t>
-  </si>
-  <si>
-    <t>Like:文学|音乐
-Desc:Tiqin nació como miembro de una noble casa Nasir. Podría haber llevado una vida refinada y pacífica, pero al conocer las malas acciones de los Nasir a través de su gran amor por la historia, decidió abandonar su hogar y elegir la paz en lugar de la guerra. Utilizando los conocimientos de alquimia que le fueron transmitidos durante su juventud, se convirtió en una alquimista viajera.
-Nature:kind=7,severe=3,honest=3,cunning=7,calm=6,anger=4,strong=8,weak=2
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能提可沁</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gusta escuchar &lt;color=red&gt;cuentos&lt;/color&gt; y admirar &lt;color=red&gt;pinturas&lt;/color&gt;.
-hello:No te acerques más... te haré daño.
-refuse_recruit_0:Yo... quiero unirme a ti, pero... lo siento.
-refuse_recruit_1:Ahora no es el momento. Lo siento.
-refuse_recruit_2:No... No puedo darte la respuesta que deseas.
-refuse_recruit_3:No quiero mirarte. No puedo controlar mi poder. Deberías irte.
-recruit_msg:Todavía no puedo controlar el poder que hay dentro de mí. Espero que puedas ayudarme a dominarlo.
-enemy_hello:Te aconsejo que no me enfades. No puedo controlarme.
-be_attack:Esta es la peor decisión que pudiste haber tomado.
-be_attack_enemy:¡Ahora me enfureceré!</t>
-  </si>
-  <si>
-    <t>Like:绘画|故事
-Desc:Él era una vez un ciudadano común de un pueblo común. Cuando tenía 12 años, unos bandidos saquearon y asesinaron a la gente de su pueblo. Presenciar la masacre de sus compañeros desencadenó las habilidades mágicas latentes de Assel. Una poderosa magia se desató en el pueblo. Assel expulsó a los bandidos, pero también hirió a muchos habitantes del lugar. La vida nunca volvió a ser igual para Assel. Aunque nadie lo expresaba abiertamente, Assel podía sentir que la gente ya no lo veía de la misma manera. Assel tomó la decisión de dejar su ciudad natal por su cuenta y recorrer el mundo. Espera tener suficiente control sobre su poder algún día para proteger a los inocentes como un poderoso mago.
-Nature:kind=6,severe=4,honest=8,cunning=2,calm=3,anger=7,strong=2,weak=8
-fight_skills:踩脚趾|直拳|飞腿|冲刺重拳
-fight_dgskill:刺拳,1
-AssSkill:统率技能阿塞尔</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Algunos objetos ocultos o equipamiento especial me distraen el tiempo suficiente como para bajar mi espada.
-hello: Juicio. Juicio por todos los pecados de este mundo.
-refuse_recruit_0: No vales la pena para que levante mi espada.
-refuse_recruit_1: Pregunta de nuevo y te cortaré la lengua.
-refuse_recruit_2: Desprendes un olor a pecado.
-refuse_recruit_3: ¿Quieres que mi espada responda por mí?
-recruit_msg: Juntos, ejerceremos justicia.
-enemy_hello: Otros te condenarán, yo te juzgaré.
-be_attack: He visto demasiadas almas lamentables como tú.
-be_attack_enemy: Tu juicio: ¡ejecución!</t>
-  </si>
-  <si>
-    <t>Like:神秘|特殊装备
-WildMonsterKiller:1
-Robber:100
-Desc:Basit fue una vez el mejor verdugo del antiguo imperio. Ha separado innumerables cabezas de sus cuerpos. Hacía cumplir estrictamente todas las leyes y actuaba como símbolo de la ley y el orden en el Antiguo Imperio. Cuando la ciudad de Jamal cayó, el verdugo se convirtió en un paria odiado. Las familias de aquellos a quienes había matado se unieron para encarcelarlo y arrojar la llave, pensando que Basit moriría de hambre o se convertiría en alimento para los roedores. Basit comió ratas para sobrevivir, sin embargo, una de las ratas que comió estaba maldita. La maldición se transfirió a él. Ahora Basit era inmortal... pero estaba condenado a conocer siempre el sufrimiento. La forma de Basit se retorció en su infernal prisión. Creció la cola de una rata y exhalaba gases nocivos. Basit rebuscó entre las ruinas de la ciudad de Jamal hasta que encontró su antigua espada de verdugo. Una vez que la sostuvo en sus manos, solo tuvo un deseo: castigar a todos los pecadores del mundo.
-Nature:kind=1,severe=9,honest=1,cunning=9,calm=4,anger=6,strong=9,weak=1
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能卜烈</t>
-  </si>
-  <si>
-    <t>没耐心: ¡Disculpa! Hay muchas personas importantes esperándome. Hablemos en otro momento.
-拒绝指教: ¿Crees que puedes ser como yo? ¡Jajaja!... Lo siento. No enseño.
-完成委托: No está mal. Parece que sabes cómo hacer el trabajo.
-乞讨冷却中: ¿Ya estás pidiendo más limosnas tan pronto? No es una buena imagen...
-乞讨成功: ¡Jajaja! ¡Bien! Has alegrado mucho a este viejo. ¡Aquí tienes tu recompensa!
-喜欢的礼物: ¿Un regalo de más allá del río? Dame &lt;color=red&gt;joyas&lt;/color&gt; o algunos objetos &lt;color=red&gt;ocultos&lt;/color&gt;.
-hello: ¿Qué has adquirido del río?
-refuse_recruit_0: Puedo agradecer respetuosamente por adquirir tales joyas para mí, pero no puedo darte la respuesta que deseas.
-refuse_recruit_1: A tu lado, solo vería extensiones áridas interminables. Estas tierras no me atraen.
-refuse_recruit_2: No puedes compararte con el río en movimiento.
-refuse_recruit_3: Persona repugnante. Serás un alma perdida en el fondo del río.
-recruit_msg: Debes querer algo importante del río si estás contratando a un hombre de salvamento como yo. ¡Emin está a tu servicio!</t>
-  </si>
-  <si>
-    <t>Like:神秘|珠宝
-Robber:100
-Desc:En el este se encuentra un largo y sinuoso río. Donde hay ríos, hay gente. Emin es un rescatista que vive y trabaja en el río. Por suficiente Utar, Emin rescatará cualquier cosa que yace en el fondo del río para cualquiera, ya sean bienes, cadáveres o tesoros. No le importa si el tesoro que recupera vale más que la tarifa que le pagan por rescatarlo, o si el cadáver del lecho del río tiene alguna trágica historia detrás. El río lava su alma y se lleva estas emociones innecesarias e inútiles.
-Nature:kind=5,severe=5,honest=5,cunning=5,calm=5,anger=5,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能罗夫</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan las &lt;color=red&gt;artesanías&lt;/color&gt; o algunos objetos &lt;color=red&gt;ocultos&lt;/color&gt;.
-hello:Cuida tu sombra.
-refuse_recruit_0:Lo he pensado. No tienes motivo para arriesgar mi vida.
-refuse_recruit_1:¿Qué puedes ofrecerme? ¿Por qué debería seguirte?
-refuse_recruit_2:Ugh. Delirante.
-refuse_recruit_3:Lárgate de aquí. Siento deseos de matar.
-recruit_msg:Tal vez al seguirte, pueda comprender mejor mis propios deseos.
-enemy_hello:Actuar irracionalmente te costará la vida.
-be_attack:¿Los asesinos no te asustan? Te mostraré por qué deberían.
-be_attack_enemy:Eres mi próximo objetivo.</t>
-  </si>
-  <si>
-    <t>Like:工艺|神秘
-Desc:Shahid nació en un pequeño pueblo estéril en el Valle de Twinluna. Casi todos los hombres nacidos allí se unieron a los Dakn Night Rangers para ganarse la vida, y Shahid no fue la excepción. Los Night Rangers eran responsables de peligrosas misiones de reconocimiento en cuevas llenas de monstruos. La mayoría de los Night Rangers provenían de orígenes humildes y tenían un entrenamiento limitado. Pocos regresaban de sus misiones bajo tierra. Shahid utilizó su excepcional agilidad y reflejos para sobrevivir a múltiples incursiones en las oscuras guaridas, lo que le valió la atención de su comandante. El comandante tomó a Shahid como aprendiz y lo ascendió a Capitán de los Night Rangers. Un hombre común aprovecharía esta posición para escapar de esta vida de oscuridad y muerte, pero Shahid entendió que su comandante, su maestro, era quien formaba a los Night Rangers. Eso lo convirtió en el hombre responsable de la muerte de su padre y su tío. Ahora Shahid debe elegir entre la venganza y la vida.
-Nature:kind=3,severe=7,honest=0,cunning=10,calm=9,anger=1,strong=6,weak=4
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能邵影</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gusta muchas cosas, como cosas &lt;color=red&gt;tristes&lt;/color&gt; y &lt;color=red&gt;románticas&lt;/color&gt;, o instrumentos &lt;color=red&gt;finos&lt;/color&gt;. Oh, también cosas relacionadas con la &lt;color=red&gt;diosa&lt;/color&gt;... Es mucho, ¡pero amo este mundo!
-hello:¡Amo el mundo!
-refuse_recruit_0:Sé que somos buenos amigos, pero... lo siento, no tengo la valentía suficiente para embarcarme en un viaje contigo.
-refuse_recruit_1:Perdóname por decir "no". Uf, ¡no soy bueno diciendo que no!
-refuse_recruit_2:Gracias por invitarme, pero hay otras cosas que debo hacer.
-refuse_recruit_3:... No quiero hablar contigo.
-recruit_msg:Veo una luz brillando sobre ti. Esta luz calma mi corazón.</t>
-  </si>
-  <si>
-    <t>Like:乐器|忧伤|浪漫|女神
-Desc:Takiyah perdió una pierna durante los tiempos turbulentos de su juventud. Aunque su cuerpo era débil, su corazón era fuerte. Un día, rescató a un viajero herido que se desplomó en las puertas de su aldea. Cuando el viajero despertó, no dijo nada y se marchó por las puertas. A la mañana siguiente, todas las personas en la aldea de Takiyah habían perdido su pierna izquierda. Takiyah no se dio cuenta de que su bondad traería tal desastre a la aldea. Su culpa la llevó a abandonar su ciudad natal...
-Nature:kind=10,severe=0,honest=9,cunning=1,calm=5,anger=5,strong=4,weak=6
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能耶雅莉瓦</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Entendido, &lt;color=red&gt;cultura&lt;/color&gt; y &lt;color=red&gt;artesanía&lt;/color&gt;. Ahora no me distraigas con mi investigación.
-hello:No importa cuán fuerte seas, nunca podrás derrotarme por completo.
-refuse_recruit_0:Me halaga que me respetes de esa manera, pero deseo vivir en libertad.
-refuse_recruit_1:Lo siento, pero mis máquinas son más interesantes para mí.
-refuse_recruit_2:¿Ves estas herramientas que tengo en mis manos? Aún tengo cosas que hacer.
-refuse_recruit_3:Deberías ir a algún lugar a despejarte.
-recruit_msg:De acuerdo. No me dejas muchas opciones.</t>
-  </si>
-  <si>
-    <t>Like:文学|工艺
-Robber:100
-Desc:El abuelo de Infan fue un técnico muy famoso en su época. Sin embargo, su abuelo fue acusado de ser leal al Viejo Imperio y fue encarcelado. Una generación de artesanos legendarios murió con él. Infan era originalmente un granjero común. Mientras empacaba las pertenencias de su abuelo, encontró accidentalmente el manual del técnico dejado por su abuelo. Al principio, solo sentía curiosidad, pero rápidamente se obsesionó. No pudo evitar trabajar en sus habilidades mecánicas, trabajando día y noche, olvidando comer y dormir. Finalmente, dominó por completo las habilidades de su abuelo e incluso comenzó a incorporar sus propias ideas. Nació un maestro de la maquinaria.
-Nature:kind=7,severe=3,honest=5,cunning=5,calm=6,anger=4,strong=8,weak=2
-fight_skills:踩脚趾|冲刺重拳|绝技裂地|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能封大木</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Solo quiero &lt;color=red&gt;equipo especial&lt;/color&gt; y &lt;color=red&gt;adornos&lt;/color&gt;. Lo demás ya lo tengo.
-hello: ¿Dónde está el legendario Maestro de la Espada de Zagros?
-refuse_recruit_0: ¡Ja ja ja, tienes valor! Pero tengo que decir que no, espero que esté bien.
-refuse_recruit_1: Simplemente no estás calificado.
-refuse_recruit_2: ¡Ja ja ja! ¡En tus sueños!
-refuse_recruit_3: Eres una cosa descaradamente fea.
-recruit_msg: ¡Genial! No hay tiempo para tonterías, ¡vamos!</t>
-  </si>
-  <si>
-    <t>Like:特殊装备|装饰
-WildMonsterKiller:1
-Desc:Zina nació en una pequeña tribu. Su padre era un hábil luchador y un famoso líder militar dentro de la tribu. Cada uno de los cinco hermanos de Zina era un guerrero de la tribu. Zina era la niña mimada de su padre y amada por su familia. Pero ella no quería vivir una vida protegida, así que se escapó. Zina planeaba encontrar al famoso Maestro de la Espada en las Montañas Zagros. La leyenda dice que este maestro podía derribar a cien enemigos de un solo golpe.
-Nature:kind=6,severe=4,honest=5,cunning=5,calm=5,anger=5,strong=8,weak=2
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能日娜</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan las cosas llenas de misterio oculto y tristeza. Además, me gusta mucho tocar instrumentos musicales, aunque hace mucho tiempo que no lo hago.
-hello: Al principio, todos somos uno. Al final, regresamos a esa unidad.
-refuse_recruit_0: Mmm, ¿de verdad? No puedo aceptar en este momento.
-refuse_recruit_1: No estoy acostumbrado/a a viajar con otros.
-refuse_recruit_2: No me gusta esa idea.
-refuse_recruit_3:...
-recruit_msg: Tal vez juntos podamos descubrir la verdad del mundo.</t>
-  </si>
-  <si>
-    <t>Like:乐器|神秘|忧伤
-Desc:Hina parece ser de otro mundo. Nadie sabe de dónde viene ni qué planes tiene. Es gentil y elegante, aunque su cabello blanco y sus ojos plateados contrastan con su rostro juvenil. Hina a menudo se sienta junto al río con una mirada perdida, su falda iridiscente como una concha reflejando un arcoíris. Es pálida y preciosa, como una perla arrastrada a la orilla.
-Nature:kind=6,severe=4,honest=5,cunning=5,calm=8,anger=2,strong=4,weak=6
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能韩瑶</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Gusto de regalos: &lt;color=red&gt;Combate&lt;/color&gt;, ¡pues el combate es la forma más elevada de &lt;color=red&gt;romance&lt;/color&gt;! Si pudiera tener algunos &lt;color=red&gt;instrumentos&lt;/color&gt; musicales, sería aún mejor, ¡para poder tocar la canción de la muerte!
-hello:¡Escucha! ¿Puedes oír el lamento de los moribundos?
-refuse_recruit_0:¿Crees que al darme baratijas puedes contratar al mejor asesino del desierto?
-refuse_recruit_1:¡Jajaja! No cualquiera se atrevería a pedirme esto. Pero aún así, debo rechazar.
-refuse_recruit_2:¿Estás suplicando mi ayuda o simplemente suplicando la muerte?
-refuse_recruit_3:Estoy deseando escuchar el sonido que harás cuando mueras.
-recruit_msg:Está bien. El olor de la sangre en ti me fascina.</t>
-  </si>
-  <si>
-    <t>Like:乐器|格斗|浪漫
-WildMonsterKiller:1
-Robber:100
-Desc:Toya era una vez un asesino impenitente. Tiene la sangre de innumerables almas en sus manos. A diferencia de un cazador de recompensas, Toya mataba sin importarle el beneficio y se convirtió en el criminal más buscado del antiguo imperio. Cumplió su condena en la prisión bajo la Ciudad de Jamal. Cuando cayó el Nefrit, Toya quedó libre una vez más. Su alma cantaba en esta tierra en guerra, llena de batallas y monstruos. Toya disfruta del nuevo mundo y del sufrimiento interminable que provoca en los demás.
-Nature:kind=1,severe=9,honest=0,cunning=10,calm=5,anger=5,strong=5,weak=5
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能托亚</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gusta el &lt;color=red&gt;combate&lt;/color&gt;... las cosas &lt;color=red&gt;ocultas&lt;/color&gt;... Realmente me gusta eso.
-hola:Jejeje, ¿qué es lo que deseas?
-refuse_recruit_0:Tú también tienes la sombra de un monstruo. Pero no es suficiente.
-refuse_recruit_1:Jejeje, ¿te gustan los monstruos? Pero no me gustas a mí.
-refuse_recruit_2:Jeje, ¡tienes el hedor de un humano! ¡Me da asco!
-refuse_recruit_3:¡Jajaja! ¡Presas! ¡Corran hacia la salida! ¡Corran por sus vidas, débiles!
-recruit_msg:Jejeje, me gusta tu persistencia.
-enemy_hello:Jejeje, pequeño lagarto, ¿ves quién ha venido?
-be_attack:Jejeje... jejeje...
-be_attack_enemy:¡Presas! ¡Entregadas a mi puerta!</t>
-  </si>
-  <si>
-    <t>Like:神秘|格斗
-Robber:100
-Desc:Yaya tuvo una infancia desafortunada. Fue abandonada por ser tan fea. Sin conocer el amor, Yaya se volvió cruel y despiadada. Rechazó todo en el mundo humano. Solo para probar un poco de sopa, Yaya aceptó convertirse en sujeto de experimentos de una hechicera a los dieciséis años. Cientos de personas perecieron en estos crueles experimentos, pero Yaya sobrevivió. ¡Se convirtió en parte mujer, parte monstruo! Su nuevo poder monstruoso se ajustaba bien a su egoísmo y crueldad. Camina por el mundo como una pesadilla. Ahora el nombre Yaya es sinónimo de muerte.
-Nature:kind=5,severe=5,honest=7,cunning=3,calm=3,anger=7,strong=9,weak=1
-fight_skills:踩脚趾|直拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能耶牙</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Hm, elijo &lt;color=red&gt;artesanías&lt;/color&gt;. Me pregunto si yo también podría considerarme una artesanía.
-hello:... ¿Qué deseas de mí?
-refuse_recruit_0:¿Te gusto yo, o a mi cuerpo mecánico? En cualquier caso, no me agradas.
-refuse_recruit_1:Si buscas la ayuda de esta guerrera mecánica, tendrás que trabajar en tu sinceridad.
-refuse_recruit_2:Ya he escuchado suficientes chistes. No digas nada más.
-refuse_recruit_3:Vete, inútil debilucho.
-recruit_msg:¡Presenciarás el mayor poder de la heredera de la Ciudad de Jamal!</t>
-  </si>
-  <si>
-    <t>Like:工艺
-WildMonsterKiller:1
-Desc:La implacable Galo Zahra, de corazón de acero. Una vez fue una joven noble de los Nephrit y heredera de la Casa Zahra. Fue abandonada cuando la alianza asedió la Ciudad de Jamal. Con solo seis años, sufrió un abuso inimaginable a manos de sus captores. Su cuerpo quedó destrozado y perdió su brazo y pierna izquierdos. Un guerrero en una armadura móvil rudimentaria la salvó de sus crueles captores y la ayudó a escapar de la Ciudad de Jamal. El guerrero le preguntó si quería vivir, pero Galo no pudo emitir sonido alguno. Luchó con todas sus fuerzas y asintió con la cabeza. Desde aquel día, una guerrera medio mecánica merodea por los Acantilados Umbra. Lleva consigo un legado de dolor y resistencia. Las tierras de los Acantilados Umbra se convirtieron en su hogar, donde acecha como una sombra en busca de justicia. Su rostro, que oculta una dulzura perdida entre las penurias, contrasta con la intensidad de sus profundos ojos azules que resplandecen con una luz inquebrantable en la oscuridad de la noche.
-Nature:kind=7,severe=3,honest=7,cunning=3,calm=5,anger=5,strong=10,weak=0
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能西河伽罗</t>
-  </si>
-  <si>
-    <t>喜欢的礼物：Me gusta... la &lt;color=red&gt;música&lt;/color&gt; de los nómadas, así como los finos &lt;color=red&gt;instrumentos&lt;/color&gt;.
-hello:Escucha. ¿Puedes oír la música del desierto?
-refuse_recruit_0:Eres buen oyente, pero no quiero tocar solo para ti.
-refuse_recruit_1:Nunca soñé con convertirme en asistente de alguien, ¿entiendes?
-refuse_recruit_2:Tal vez estarías satisfecho con algún adorno bonito, pero eso no es lo que yo quiero.
-refuse_recruit_3:Algo en ti realmente me desagrada.
-recruit_msg:Bueno, en los días venideros, permíteme cantar para ti.</t>
-  </si>
-  <si>
-    <t>Like:乐器|音乐
-Desc:Aganazzar, conocida como la Estrella de la Armonía, es una talentosa artista cuyo instrumento es la magia misma. Su voz celestial y sus habilidades mágicas tienen el poder de sanar no solo las heridas físicas, sino también las almas afligidas. Criada por su abuela hechicera, Aganazzar aprendió a canalizar su energía mágica a través de la música, convirtiendo cada canción en un hechizo sanador que toca los corazones de quienes la escuchan. Rechazando las ofertas de los poderosos nobles que deseaban poseerla, Aganazzar emprende un viaje como una errante, llevando su música y magia a aquellos que más lo necesitan, dejando un rastro de sanación y esperanza a su paso.
-Aganazzar se ha convertido en una leyenda en el reino, conocida por su habilidad para traer armonía y alivio a través de su música. Su espíritu libre y rebelde la lleva a viajar por tierras lejanas, siempre evitando ser capturada por aquellos que la consideran una posesión. En cada actuación, demuestra su destreza musical y su profundo conocimiento de la magia, creando un vínculo mágico con su audiencia y despertando emociones profundas. 
-Nature:kind=6,severe=4,honest=3,cunning=7,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能安古欢</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gusta todo lo relacionado con la &lt;color=red&gt;música&lt;/color&gt; o los cielos distantes.
-hello: Caí desde el firmamento solo para ser enterrado en el polvo.
-refuse_recruit_0: Tu futuro no requiere mi participación.
-refuse_recruit_1: Las estrellas me guían. No puedes bloquear su luz.
-refuse_recruit_2: Tu brillo es tan tenue que me deprime.
-refuse_recruit_3: No me gusta tu aura caída.
-recruit_msg: Te seguiré. ¿Puedes... llevarme a casa?</t>
-  </si>
-  <si>
-    <t>Like:音乐|乐器
-DescAunque aparenta tener diez años, tiene la sabiduría y la seriedad de una mujer de ochenta años. Muchos se sorprenden al ver a una niña hechicera. Su don innato para la profecía le ha ganado un gran número de seguidores, pero ella se niega a ejercer autoridad sobre ellos. Najima a menudo contempla fijamente un punto en el cielo con una expresión ausente. Nadie sabe de dónde proviene y nadie sabe a dónde irá.
-Nature:kind=5,severe=5,honest=10,cunning=0,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能天星</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Las cosas &lt;color=red&gt;románticas&lt;/color&gt; me relajan. También me hacen feliz algunos &lt;color=red&gt;artículos artesanales&lt;/color&gt; de calidad.
-hello: Desearía que este genio se relajara y me dejara hablar.
-refuse_recruit_0: Como puedes ver, esta cosa que llevo en mi espalda es un genio malvado. Podría ser peligroso para ti. Por eso... no puedo ayudarte.
-refuse_recruit_1: Tengo libertad, lujo, comodidad. Si me uno a ti, todas esas cosas desaparecen.
-refuse_recruit_2: No. No, no, no. Ve a buscar a alguien más.
-refuse_recruit_3: ¡Sal de aquí! ¡No puedo controlar a este genio!
-recruit_msg: Está bien. Te lo buscaste tú mismo.
-enemy_hello: Te insto a que tengas cuidado: este genio en mi espalda es peligroso.
-be_attack: Te advertí sobre las consecuencias. No puedo hacerme responsable.
-be_attack_enemy: Jaja, este genio debe estar hambriento a estas alturas.</t>
-  </si>
-  <si>
-    <t>Like:浪漫|工艺
-WildMonsterKiller:1
-Robber:100
-Desc:El Sol Negro despertó a un antiguo y malvado genio. Este perverso genio había perdido hace mucho tiempo su hogar original. Un desequilibrio en las fuerzas universales lo atrapó en una espada... una espada que pertenecía a Rwal. El genio nunca deja de intentar apoderarse del cuerpo de Rwal, mientras que Rwal se ve obligado a resistir constantemente. Rwal se debilita día a día. No pasará mucho tiempo antes de que esta tierra tenga otro espadachín poseído por un genio.
-Nature:kind=6,severe=4,honest=3,cunning=7,calm=4,anger=6,strong=4,weak=6
-fight_skills:踩脚趾|冲刺重拳|飞腿|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能墨敕</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:Me gustan... Déjame pensar... &lt;color=red&gt;baratijas&lt;/color&gt;, &lt;color=red&gt;juguetes&lt;/color&gt;, cosas &lt;color=red&gt;adorables&lt;/color&gt;, sí, todas estas cosas me hacen feliz.
-hello:Vengo de una tierra lejana al este, un lugar lleno de flores de durazno.
-refuse_recruit_0:¿Eh? ¿Quieres que me una a ti? Um... déjame pensarlo.
-refuse_recruit_1:Hm... No suelo viajar con otras personas.
-refuse_recruit_2:¡No, gracias! Me gusta estar sola.
-refuse_recruit_3:No es agradable rechazarte así, pero debo decir que has hecho algunas cosas desagradables y no me gusta.
-recruit_msg:¡Bien! Si tienes la oportunidad, deberíamos ir a mi ciudad natal.</t>
-  </si>
-  <si>
-    <t>Like:装饰|玩具|可爱
-Desc:Wakata vivía con su padre en una tierra lejana al este, cubierta de nieve. A pesar de la nieve, en esa tierra distante hay muchas aguas termales donde hermosas flores de durazno rosadas florecen. La tranquila vida de Wakata llegó a su fin abruptamente cuando su padre desapareció. Comenzó un viaje hacia el oeste para encontrar a su padre. Lo que no sabía era que la magia curativa que aprendió de su padre haría que su viaje hacia el oeste fuera increíblemente peligroso.
-Nature:kind=8,severe=2,honest=5,cunning=5,calm=5,anger=5,strong=8,weak=2
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒
-fight_dgskill:刺拳,1
-AssSkill:统率技能若桃</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:&lt;color=red&gt;Historia&lt;/color&gt;, &lt;color=red&gt;música&lt;/color&gt;. Si encuentras algún &lt;color=red&gt;equipo especial&lt;/color&gt;, déjame verlo y estaré agradecido.
-hello:El Creador construye y destruye sin miedo.
-refuse_recruit_0:Si quieres las armas que he creado, no tienes que ser tan indirecto.
-refuse_recruit_1:Es cierto que soy una buena pieza. Pero no deseo convertirme en la pieza de alguien más.
-refuse_recruit_2:He perdido el apetito por ser utilizado como un arma.
-refuse_recruit_3:Tú me llevarías hacia el mal.
-recruit_msg:Podría haber estado solo toda mi vida, pero tú... bueno, espero que me recuerdes.</t>
-  </si>
-  <si>
-    <t>Like:历史|特殊装备|音乐
-Desc:La magia no puede ser simplemente lanzada de la nada. Algunos tipos de magia requieren componentes o herramientas arcanas, mientras que otras consumen el poder espiritual del conjurador. Un artífice que utiliza la magia para forjar un arma mágica creará una reacción mágica opuesta cada vez que crea dicho arma. Esta especie de negación mágica duradera es un precio que todo artífice debe pagar. Cuanto más poderosa sea el arma, mayor será el precio, mayor será la resistencia. Con el tiempo, un artífice no puede utilizar un arma creada por su propio pueblo, y mucho menos su propia arma encantada. Este es el taller más solitario de la tierra. Han forjado armas durante toda su vida, pero ahora deben despedirse de la obra de su vida.
-Nature:kind=5,severe=5,honest=6,cunning=4,calm=7,anger=3,strong=5,weak=5
-fight_skills:踩脚趾|冲刺重拳|飞腿|吼叫
-fight_dgskill:刺拳,1
-AssSkill:统率技能贺若岚光</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¡Oh! A las mujeres como yo no podemos resistirnos a nada que sea &lt;color=red&gt;romántico&lt;/color&gt;... Si no puedes encontrar algo romántico, me encantaría una colección de atlas u otros libros de &lt;color=red&gt;geografía&lt;/color&gt; para poder explorar lugares interesantes a los que nunca he ido antes.
-hello: ¡Oh! Puedo escuchar los latidos de tu corazón.
-refuse_recruit_0:¡Wow! Realmente eres encantador. Permíteme pensarlo un momento.
-refuse_recruit_1:¡Ahem! ¿Estás enamorado de mí? Pero debo rechazar tu oferta.
-refuse_recruit_2:¡Oh~ No puedo imaginarme siguiendo a un grupo de chicos malolientes viviendo al aire libre. Suena terrible.
-refuse_recruit_3:¡Jajaja! ¡Ni en tus sueños!
-recruit_msg: ¿Cómo podría resistirme? Eres demasiado adorable para decir que no.</t>
-  </si>
-  <si>
-    <t>Like:浪漫|地理
-WildMonsterKiller:1
-Desc:Nura es una guerrera de orígenes misteriosos. Es tan habilidosa como hermosa y tiene una voluntad firme. Está versada en todo tipo de armas, y su combate desarmado también es excelente. Durante una misión secreta, descubrió salitre. Desde entonces, ha estado experimentando con pólvora. Viajó millones de codos hasta esta tierra asolada por la guerra para encontrar un lugar adecuado donde probar la fuerza de su pólvora.
-Nature:kind=6,severe=4,honest=5,cunning=5,calm=4,anger=6,strong=8,weak=2
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳
-fight_dgskill:刺拳,1
-AssSkill:统率技能薇卡</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me gusta escuchar los &lt;color=red&gt;lamentos&lt;/color&gt; de los muertos encarcelados. Si deseas impresionarme, debes buscar &lt;color=red&gt;equipamiento especial&lt;/color&gt; que solo se encuentra en leyendas.
-hello: La luz del sol es dura, pero he aprendido a apreciarla.
-refuse_recruit_0: Pareces ser una persona decente. Lo consideraré.
-refuse_recruit_1: Si hubieras vivido la vida que he llevado, también te costaría confiar en los demás.
-refuse_recruit_2: No veo futuro para mí en tu compañía. Solo puedo confiar en mí misma.
-refuse_recruit_3: Si estuviéramos en las mazmorras, serías el primero en perder la vida.
-recruit_msg: Mis pesadillas son constantes. Espero encontrar alivio entre tu compañía.
-enemy_hello: Te despedazaré en cuanto tenga la oportunidad, insecto.
-be_attack: Escapé del mismísimo infierno. No tienes ninguna posibilidad.
-be_attack_enemy: ¡Ahora te mostraré el verdadero significado del miedo!</t>
-  </si>
-  <si>
-    <t>Like:忧伤|特殊装备
-Robber:100
-Desc:La oscuridad sustenta el pecado y el deseo, así como a Raheel durante diez largos años. Después de que el sol negro se alzara en el cielo, el pueblo de Raheel creyó que el sol traía maldiciones y cataclismos, por lo que construyeron una ciudad subterránea y comenzaron una vida alejados del sol. Esta ciudad subterránea se mantuvo estable durante diez años, pero esta estabilidad se vio rápidamente socavada en medio de una gran hambruna... Raheel emergió como el único vencedor de esta sangrienta batalla por la supervivencia. Abandonó la oscuridad y salió de la mazmorra.
-Nature:kind=1,severe=9,honest=1,cunning=9,calm=7,anger=3,strong=10,weak=0
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳
-fight_dgskill:刺拳,1
-AssSkill:统率技能桑开</t>
-  </si>
-  <si>
-    <t>喜欢的礼物:... No puedo pensar en algo que quiera, pero si es un [[imp:juguetes]], puedo dárselo a mi hermana, ¿verdad? A ella también le encantan varias [[imp:historias]].
-hello:Pareces tener ciertas habilidades, compitamos en el torneo de artes marciales si tenemos la oportunidad. | ¿Alguna vez has conocido a mi hermanita? Es una niña muy dulce. | Si aún sientes dolor durante la batalla, eso es algo bueno, significa que todavía estás lejos de morir en combate.</t>
-  </si>
-  <si>
-    <t>Desc: Agura fue una vez un guerrero de la tribu del Caballo Salvaje. Cuando era joven, vivía con sus padres y su hermana menor cerca del desierto de la ciudad de Kuquan. Durante una guerra, la ciudad de Kuquan fue atacada por un grupo enemigo, mientras Agula luchaba con otras tropas enemigas en la línea del frente. Cuando Agula regresó a casa, descubrió que solo su hermana había sobrevivido. En su dolor, Agula abandonó su juramento al Rey del Caballo Salvaje y llevó a su hermana a la Ciudad de las Flores porque a ella le gustaban las flores.
-En la Ciudad de las Flores, Agula descubrió que no tenía habilidades aparte de la lucha, pero no quería unirse al ejército y alejarse de su familia. Eventualmente, Agula encontró su lugar en el torneo local de artes marciales.
-Pensó que la vida mejoraría a partir de entonces, pero poco después, la hermana de Agura enfermó gravemente y murió. Devastado, Agula encontró en el campo de batalla un escape y se dedicó a buscar el combate definitivo.
-Like: Story|Toy.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Me encantan las historias, ¡es tan fácil saber mis preferencias! ¡Me gusta mucho escuchar [[imp:historias]] y también compartir las mías! Además, disfruto de todo tipo de [[imp:artesanías]].
-hello:¡al ver tu rostro supe que tienes muchas historias para compartir! | Un hombre debe experimentar una gran aventura en su vida, ¡al igual que yo! | Siempre les digo a los demás que vengo de la otra parte de la Gran Montaña Nevada, ¡pero siempre piensan que estoy exagerando! | ¡Un hacha puede cortar árboles y también puede usarse para cortar personas! Aunque no recomiendo la segunda opción. | ¡Maldición! ¿Dónde está mi cuerno de bebida? ¡Oh, está en mi mano todo este tiempo! ¡Ja, ja, ja, ja! | Una vez me tropecé y el hacha salió volando, ¡y resulta que golpeó a un gigante! ¡Ja! Te estoy tomando el pelo, en realidad golpeó a un dragón gigante.</t>
-  </si>
-  <si>
-    <t>Desc: Khrasisson afirma venir del otro extremo de las montañas, donde se puede ver un denso bosque después de cruzar peligrosas cordilleras. Después de caminar hacia el este durante varios días, se puede avistar un gran río, y al otro lado del río se encuentra el pueblo donde nació Khrasisson.
-Tras cruzar las montañas, Khrasisson llegó por primera vez al pueblo de Spring Valley, donde repelió a más de veinte bandidos él solo. Luego pasó por Weeping Spring Town, North Wilderness Village y el oasis de Wo Lake, y finalmente llegó al Mercado de la Campana del Camello. Cada vez que llegaba a un lugar nuevo, Khrasisson dejaba su propia historia. Al principio, los lugareños no podían comunicarse con Khrasisson debido a la barrera del idioma, y muchos pensaban que era una persona callada. Pero ahora, en las tabernas del Mercado de la Campana del Camello, siempre hay animación cuando Khrasisson está presente.
-Like: Craft | Story.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: ¿Mis preferencias? Como una mujer hermosa como yo, necesito algo de misterio, así que te invito a adivinar~
-hello: Muchos creen que los miembros del clan escorpión naturalmente amamos a los escorpiones, pero en realidad los detesto.
-¡Te ves muy poderoso! Estoy ansiosa por ver cómo reaccionarás a mis pociones~
-¿Cómo se puede considerar hacer trampas al usar veneno? Como una mujer delicada como yo, naturalmente necesito usar algunos trucos~
-Soy la mejor alquimista de venenos del desierto. No hay veneno que no pueda neutralizar.</t>
-  </si>
-  <si>
-    <t>Desc: Jamilla proviene de la antigua aristocracia de la tribu Escorpión. Ella y su hermana, Shariya, recibieron una educación de élite dentro de la tribu desde temprana edad y a menudo visitaban la tienda del jefe. Su mentor solía decir: "Jamilla es talentosa e inteligente, mientras que Shariya es meticulosa. Cuando las dos están juntas, pueden ejercer su máxima fuerza". Sin embargo, las dos hermanas se volvieron hostiles entre sí porque ambas se enamoraron del mismo hombre, quien más tarde se convirtió en el jefe de la tribu Escorpión, Longclaw. Sin poder soportar ver florecer la relación de su hermana con Longclaw, Jamila finalmente completó una poción altamente tóxica bajo la instigación de Amantha. Cualquiera que tome esta poción se convertirá en una persona inútil. El resto de la historia es bien conocida.
-Like: mysterious</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Es un hábito poco saludable indagar sobre los gustos de los demás...
-hello: No tengo habilidades mágicas y tampoco me gustan. | Puedo sentir tu gran presencia, si puedo enfrentarme a ti, mejoraré mi técnica de puñetazos. | El oro falso y el oro verdadero tienen una gran diferencia de precio, pero si se convierten en joyas, no se distinguen en absoluto. | Siempre llevo mis puños conmigo, la preparación marcial es constante.</t>
-  </si>
-  <si>
-    <t>Desc: Jaina era originaria de la Familia Dorada, un clan famoso en el desierto, pero fue desterrada porque no heredó el poder mágico para controlar el oro. Cuando era joven, Jaina aprendió artes marciales bajo la guía de su padre. Debido a la muerte temprana de sus padres, Jaina comenzó a vivir por su cuenta a temprana edad, practicando habilidades de combate en tabernas y en las calles. Combinó estas habilidades con las artes marciales de su padre para desarrollar su propio estilo y se convirtió en una luchadora conocida. Ella cree que algún día regresará a la Familia Dorada para demostrar su fuerza.
-Like: Fighting</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Hmm... lo que más me gusta son las cosas que registran la [[imp:historia]], ya que me ayudan a recordar muchas cosas.
-hello: ¿Acaso nos hemos conocido antes? Siento que hay algo familiar en ti. | Mi memoria no es muy buena... Si alguna vez te ofendo, sería genial si pudieras perdonarme. | Parece que alguna vez tuve un acuerdo importante con alguien, pero no puedo recordarlo... | Dices que los seres estelares realmente existen? Si es así, ¿por qué me abandonaron? | Hay una persona importante para mí en las montañas nevadas, pero no puedo recordar su apariencia ni su nombre...</t>
-  </si>
-  <si>
-    <t>Desc: Antes una poderosa hechicera del Clan Estelar, Zann era responsable de registrar y presenciar todo en este desierto. Se integró a la civilización del desierto, experimentando innumerables estaciones y presenciando el ascenso y caída de un régimen tras otro. A lo largo de los años, se sumergió demasiado en los roles que desempeñaba: guerrera, aventurera, sanadora... Cuando finalmente recobró la razón, descubrió que sus compañeros del clan habían desaparecido hace mucho tiempo.
-Like: History</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: Todos los nacidos en el Bazar Dorado aman las joyas de &lt;color=red&gt;oro y plata&lt;/color&gt;... Y yo no soy una excepción. Además de las joyas, también me encantan los finos &lt;color=red&gt;artículos artesanales&lt;/color&gt;.
-hello: ¿Por qué me molestas? Estoy ocupado.
-refuse_recruit_0: No eres una mala persona, pero no puedo renunciar a mis sueños para estar contigo, aunque sea por un breve período de tiempo.
-refuse_recruit_1: Prefiero buscar la riqueza por mi cuenta antes que unirme a ti.
-refuse_recruit_2: ¿Cuáles son las mejoras en tus cualificaciones? Aún no has alcanzado un nivel digno de mí.
-refuse_recruit_3: Por favor, vete ahora mismo.
-recruit_msg: Está bien, me has convencido... Creo que serás de utilidad para mí.
-enemy_hello: ¿Sabes qué pienso de ti? Mira a mis ojos.
-be_attack: No encontrarás trabajo en el bazar. ¿Viniste aquí para darme dinero?
-be_attack_enemy: Muy bien. Estás en nuestra lista de buscados.</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: &lt;color=red&gt;¡Lindos&lt;/color&gt; &lt;color=red&gt;adornos&lt;/color&gt;! ¿Qué? ¿No te gustan?
-hello: ¡Permítele a Batu darte un abrazo pacífico!
-refuse_recruit_0: Eres una persona interesante. Pero Batu tiene otras cosas que hacer.
-refuse_recruit_1: Deja que Batu lo piense.
-refuse_recruit_2: ¿Oh, ¿en serio? Pero no tengo ninguna razón para aceptar tu oferta.
-refuse_recruit_3: ¡Eres una persona violenta! ¡Batu te odia!
-recruit_msg: ¡De acuerdo, acepto! ¡Permíteme darte un abrazo!
-enemy_hello: Batu no quiere pelear.
-be_attack: ¿No podemos hablar de esto? Batu no se deja intimidar tan fácilmente.
-be_attack_enemy: ¡Eres realmente molesto! ¡Batu te aplastará!</t>
-  </si>
-  <si>
-    <t>Like:装饰|可爱
-Desc:En un mundo lleno de caos y violencia, Batu emerge como un enigma singular. Su imponente figura, adornada con músculos poderosos, contrasta con su aprecio por la paz y su aversión al conflicto. Sin embargo, cuando la injusticia se manifiesta en forma de una pelea, Batu no puede resistirse a actuar. En esos momentos, su fuerza imponente se desata, y sus puños se convierten en instrumentos para poner fin a la violencia, siempre con la intención de restaurar la armonía y la tranquilidad.
-A pesar de su aspecto imponente, Batu guarda un corazón amable y gentil. Durante la mayoría de los días, busca la serenidad en sus actividades cotidianas y ha encontrado un inusual pasatiempo en la costura. Con destreza inesperada, utiliza aguja e hilo para reparar las rasgaduras que suelen ocurrirle a su ropa durante sus momentos de acción. Este singular contraste entre su naturaleza imponente y su habilidad para el bordado muestra la diversidad de facetas que conforman a Batu, un protector comprometido con la paz y dedicado a encontrar la belleza en las más inesperadas habilidades.
-Nature:kind=9,severe=1,honest=9,cunning=1,calm=9,anger=1,strong=1,weak=9
-fight_skills:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳
-fight_dgskill:刺拳,1
-AssSkill:统率技能巴图</t>
-  </si>
-  <si>
-    <t>喜欢的礼物: La habilidad en &lt;color=red&gt;combate&lt;/color&gt; me hace más fuerte en la batalla. La familiaridad con la &lt;color=red&gt;geografía&lt;/color&gt; me ayuda a sobrevivir. No necesito nada más.
-hello: ¡Ey! Estás en mi camino.
-refuse_recruit_0: Déjame considerarlo.
-refuse_recruit_1: Olvídalo. Claramente no eres lo suficientemente fuerte.
-refuse_recruit_2: ¿Yo? Hmph. Yo no caigo junto con otros.
-refuse_recruit_3: Si continúas hablando así, terminarás muerto.
-recruit_msg: Tú y yo somos similares.  ¡Te seguire!
-enemy_hello: No te acerques más.
-be_attack: Veamos qué tan capaz eres.
-be_attack_enemy: Eres audaz. ¡Ven!</t>
-  </si>
-  <si>
-    <t>Like:地理|格斗
-Robber:100
-WildMonsterKiller:1
-Desc:Nacida en el seno de una familia de fugitivos, esta joven mujer creció en la ciudad de Nagukka, sumida en la opresión del Viejo Imperio. Con la caída del imperio, se vio obligada a huir de su hogar y enfrentar las adversidades del árido desierto. Durante años, luchó por sobrevivir en un entorno implacable, enfrentando peligros y desafíos que moldearon su carácter y le otorgaron habilidades excepcionales.
-Su valentía y determinación la llevaron a desarrollar una destreza sin igual en el combate, aprovechando su conocimiento de las tierras desérticas para su beneficio. Con el paso del tiempo, se convirtió en una experta en la navegación del desierto y en el arte de la supervivencia. Su astucia y habilidades tácticas le permiten sortear cualquier obstáculo que se presente en su camino, convirtiéndola en una fuerza a tener en cuenta en cualquier situación. 
-Nature:kind=3,severe=7,honest=1,cunning=9,calm=4,anger=6,strong=7,weak=3
-fight_skills:踩脚趾|直拳|飞腿|心清如水
-fight_dgskill:刺拳,1
-AssSkill:统率技能尉迟月</t>
+    <t>喜欢的礼物: Minhas necessidades são simples e modestas; Não preciso de grandes presentes. Olá: O destino de Salzaar está inexoravelmente ligado ao meu governo como Nasir Sultan, seja por meios pacíficos ou pela força. recusar_recruit_0: Se eu mantiver minha coragem sem recuar, recuperarei esta terra e honrarei o legado de meu pai. recusar_recruit_1: Eu sou o Sultão Nasir, um verdadeiro líder e não seguirei as ordens daqueles que são estranhos à nossa terra. recusar_recruit_2: Como você ousa fazer uma pergunta tão tola e sem sentido? recusar_recruit_3: Eu jamais cometeria tal ato que vai contra meus princípios e deveres! recruta_msg: Embora eu não tenha mais o título de Nasir Sultan, valorizo ​​seu apoio e dedicação para comigo. Eu te seguirei lealmente. inimigo_hello: Fique longe. Minha lança é infalível e não errará o alvo. ser_attack: Hoje você se tornou um inimigo de Nasir. Prepare-se para enfrentar as consequências de suas ações. be_attack_enemy: Um pequeno pássaro ousa desafiar a majestosa águia bicando suas asas.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Você está tentando me vencer? Kkkkk! Impossível! olá: Poucos ousariam me desafiar nas majestosas montanhas Zagros! Meu nome é Ruha, a guardiã dessas terras sagradas e a defensora de seu povo. recusar_recruit_0: Se eu me juntar a você, quem protegerá o bravo povo da montanha? Durante gerações, garanti sua segurança e bem-estar. recusar_recruit_1: Obrigado, mas com o apoio e a lealdade do povo da montanha, ainda posso superar qualquer desafio que surgir no meu caminho. recusar_recruit_2: Por que você está me fazendo essa pergunta? Minha lealdade e compromisso são com meu povo e com essas terras ancestrais. recusar_recruit_3: Não se superestime! As montanhas me transformaram em um guerreiro temível e não permitirei que ninguém subestime minha força. recruta_msg: Você, Com a sua promessa de garantir a segurança e o bem-estar do povo da montanha, você conseguiu conquistar o meu respeito. Ruha deixará as piadas de lado e se juntará à sua causa. inimigo_hello: Por que você está aqui? Estas montanhas são a minha casa e protegerei os seus segredos e o seu povo com a minha vida. be_attack: Se você deseja testemunhar a fúria das montanhas em primeira mão, prepare-se para enfrentar minhas proezas de combate. Eu não vou decepcionar você! be_attack_enemy: Venha! Mostrarei a você a habilidade e a ferocidade que emana dessas montanhas majestosas! Prepare-se para enfrentar minha habilidade de combate. Eu não vou decepcionar você! be_attack_enemy: Venha! Mostrarei a você a habilidade e a ferocidade que emana dessas montanhas majestosas! Prepare-se para enfrentar minha habilidade de combate. Eu não vou decepcionar você! be_attack_enemy: Venha! Mostrarei a você a habilidade e a ferocidade que emana dessas montanhas majestosas!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Agradecemos sua gentileza, mas não exigimos nenhum presente neste momento. Nossa história está entrelaçada com o legado do Antigo Império, e somos os dignos herdeiros e legítimos reis de Salzaar. recusar_recruit_0：Também estamos procurando por Ilayda, mas infelizmente não podemos aceitar. Nossa lealdade e comprometimento são inabaláveis ​​e apenas seguimos as ordens e projetos de Ilayda. recusar_recruit_1：Nossos movimentos são determinados exclusivamente pelas ordens de Ilayda. Só nos movemos quando ela assim o decidir. recusar_recruit_2：Mesmo se estivéssemos envolvidos em assuntos semelhantes, não nos juntaríamos à sua causa. Nossa lealdade está enraizada em Ilayda e em seguir nossos próprios caminhos. recusar_recruit_3：Não se surpreenda se nossa espada acabar com você por essa insolência. Não toleramos desrespeito à nossa causa e ao nosso líder. recruta_msg：Se Ilayda estivesse presente, ela gostaria que nos anexássemos a você. Nossa espada está à sua disposição, pois a vontade dele é o nosso guia. inimigo_hello：Se você se opor a nós, você enfrentará o herdeiro do deserto. Nossa autoridade e poder representam a herança das areias áridas. Entendido? be_attack：Então deixe nossos caminhos se cruzarem em duelo. Vamos mostrar quem tem a verdadeira força. be_attack_enemy：Você cairá diante do nosso poder indomável! Não subestime nossa determinação e habilidades de combate. você enfrenta o herdeiro do deserto. Nossa autoridade e poder representam a herança das areias áridas. Entendido? be_attack：Então deixe nossos caminhos se cruzarem em duelo. Vamos mostrar quem tem a verdadeira força. be_attack_enemy：Você cairá diante do nosso poder indomável! Não subestime nossa determinação e habilidades de combate. você enfrenta o herdeiro do deserto. Nossa autoridade e poder representam a herança das areias áridas. Entendido? be_attack：Então deixe nossos caminhos se cruzarem em duelo. Vamos mostrar quem tem a verdadeira força. be_attack_enemy：Você cairá diante do nosso poder indomável! Não subestime nossa determinação e habilidades de combate.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah! Este velho já viveu o suficiente. Só quero ter uma boa noite de sono... e nada mais. olá: Os Umbra Cliffs são um lugar agradável. Venha e vá quando quiser, sem restrições. recusar_recruit_0: Admiro suas conquistas em tão tenra idade! Mas ainda não é suficiente para convencer este velho. recusar_recruit_1: Você não tem o que é preciso para conquistar esse veterano. recusar_recruit_2: Você tem alguma habilidade, mas não o suficiente para me impressionar. recusar_recruit_3: Perda de tempo! Vá embora! recruta_msg: Sou um homem velho que não serve outro há muito tempo. Você pode ser o primeiro! inimigo_hello: Pense duas vezes antes de agir de forma imprudente. be_attack: Ainda tenho energia para te dar uma lição, meu jovem! be_attack_enemy: Prepare-se para ser esmagado sob meus pés!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah, eu adoro as estrelas no céu! Você poderia me trazer um? No entanto, o meu verdadeiro desejo é conquistar o mundo inteiro e vê-lo colocado sob o meu domínio implacável. Olá, o que você quer? Vejo ambição e determinação em seus olhos. recusar_recruit_0: Devo cuidar do meu irmão mais velho, Hassan. Seu bem-estar é minha prioridade. Peço desculpas por não poder acompanhá-lo neste momento. recusar_recruit_1: Você é tão inocente~! Você não tem medo de que eu te envenene secretamente? É melhor você seguir seu caminho sem mim. recusar_recruit_2: Você realmente tem muita audácia em pensar que posso me juntar à sua causa. Minha ambição é muito maior e meus planos mais complexos. recusar_recruit_3: Eu te odeio! Não há nada em você que me impressione ou me faça mudar de ideia. Você pode ir embora agora, antes que se arrependa. recruta_msg: Se eu concordar em me juntar a você, Você deve compreender que meu irmão Hassan e eu merecemos tratamento privilegiado. Certifique-se de que nossas necessidades sejam atendidas e nosso poder reconhecido. inimigo_hello: Escorpiões são mais perigosos de perto. E eu sou como um escorpião mortal, pronto para atacar sem piedade. be_attack: Oh, vou gostar de torturar você lentamente, observando sua resistência desaparecer enquanto eu dobro você à minha vontade. be_attack_enemy: Ah, isso não vai ser rápido, hehehe! Prepare-se para sofrer e testemunhar minha sede implacável de poder. Gostarei de torturá-lo lentamente, observando sua resistência desaparecer enquanto eu o submeto à minha vontade. be_attack_enemy: Ah, isso não vai ser rápido, hehehe! Prepare-se para sofrer e testemunhar minha sede implacável de poder. Gostarei de torturá-lo lentamente, observando sua resistência desaparecer enquanto eu o submeto à minha vontade. be_attack_enemy: Ah, isso não vai ser rápido, hehehe! Prepare-se para sofrer e testemunhar minha sede implacável de poder.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Cansei de procurar por Utar. Se você quer ser meu amigo, tente me conquistar com uma boa &lt;color=red&gt;história&lt;/color&gt;. olá: Os problemas dos ricos estão além da sua imaginação, infelizmente. recusar_recruit_0: Você não precisa me olhar assim, eu sei o que você está pensando, e a resposta é: de jeito nenhum! recruta_msg: Parece que existem alguns prazeres que o dinheiro não compra, hahaha! Você me conquistou com sua história inteligente. inimigo_hello: Junte-se a mim e haverá uma recompensa de Utar para você. be_attack: Estúpido! Você é como Wildfire, um mero brinquedo para mim. be_attack_enemy: Venha, deixe-me ver como as pessoas comuns lutam. Vamos nos preparar para um duelo de verdade.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah! Por que não comparamos nossos &lt;color=red&gt;itens de combate&lt;/color&gt;? olá: Quando a espada descansa, seu verdadeiro significado é revelado. Por trás de cada arma há uma história de honra e habilidade. recusar_recruit_0: Existe apenas um alfa no pacote. Se a matilha precisar se render a você, primeiro você deverá desafiar e derrotar o líder atual. A hierarquia é respeitada em nossa tradição. recruta_msg: Você provou ser um líder formidável! Sua habilidade em combate e visão estratégica me convenceram a me juntar à sua causa. inimigo_hello: Se você deseja me desafiar, você deve respaldar suas palavras com ações. Não tolero palavras vazias e só a força do combate revelará quem é realmente digno. be_attack: Que esta batalha seja uma prova de nossas habilidades e um teste de nosso valor. Não se subestime, Bem, não vou lhe dar uma luta fácil. be_attack_enemy: Submeta-se à minha espada, seu idiota! Não se engane com falsas esperanças, pois minha capacidade de combate excede em muito a sua. Prepare-se para enfrentar seu destino.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Minha paixão é investigar o &lt;color=red&gt;oculto&lt;/color&gt;. Nada mais me intriga tanto quanto os mistérios e segredos que estão além da nossa compreensão. Olá: Existem dois tipos de pessoas que eu desprezo: os arrogantes que se acham superiores e os ingênuos que se deixam enganar pela ignorância. recusar_recruit_0: Você não está me oferecendo nada que eu já não tenha encontrado em minha pesquisa. Busco conhecimentos e verdades além do comum. recruta_msg: Em meus estudos perturbadores descobri tesouros de sabedoria oculta. Se você for capaz de apreciar e valorizar esse conhecimento, poderemos estabelecer um relacionamento lucrativo. inimigo_hello: Eu me pergunto o quanto você estaria disposto a sacrificar para desvendar os segredos que eu protejo. be_attack: Eu planejei esse confronto e minhas habilidades ocultas irão surpreendê-lo. be_attack_enemy:</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Tenho sempre interesse em dar uma olhada nos seus &lt;color=red&gt;artesanato&lt;/color&gt;, eles são uma expressão única de criatividade. Olá: Meus olhos de águia não perdem nenhum detalhe. recusar_recruit_0: Você é uma pessoa comum, por que eu deveria apoiá-lo? recruta_msg: Ajudar você é minha melhor opção no momento. Juntos podemos alcançar grandes coisas. inimigo_hello: O que fez você me procurar? Espero que você tenha um bom motivo. be_attack: Atacar de forma imprudente, confiando apenas em suas habilidades sem estratégia, é um caminho seguro para a derrota. be_attack_enemy: Você se superestimou! Sua confiança cega em suas habilidades não será suficiente para me enfrentar.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Quando eu era menina, meus irmãos Wildfire me deram muitos &lt;color=red&gt;jogos&lt;/color&gt;. Embora eu já seja adulto, esses objetos evocam lembranças de tempos mais felizes. Porém, coisas &lt;color=red&gt;tristes&lt;/color&gt; também me lembram da minha missão atual: vingança! Olá: Enquanto eu estiver aqui, o fogo arderá sem cessar, iluminando o caminho para a justiça. recusar_recruit_0: Tenho uma missão muito mais importante do que a busca por conquistas e riquezas mundanas. recruta_msg: Prometa-me que juntos encontraremos os responsáveis ​​por prejudicar o Wildfire e faremos com que paguem por suas ações. inimigo_hello: Como você é inteligente para se esconder como uma sombra! Mas você não conseguirá se esconder por muito tempo do meu fogo ardente. be_attack: Vilão, você não receberá piedade de mim! Minha raiva se inflama como uma torrente de fogo incontrolável. be_attack_enemy: Eu estava preparado para esse confronto. Minha determinação e ferocidade superam todas as expectativas. Prepare-se para enfrentar as chamas da minha vingança.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Embora meu entusiasmo por artesanato tenha diminuído, ainda aprecio &lt;color=red&gt;itens artesanais&lt;/color&gt;. Além disso, itens relacionados à &lt;color=red&gt;luta&lt;/color&gt; são muito úteis para mim. Olá: Não baixe a guarda! Você não poderia se esforçar um pouco mais e mostrar um sorriso? recusar_recruit_0: Trabalhei muito para conseguir tudo o que tenho. Não estou disposto a simplesmente desistir. recruta_msg: Espero poder contribuir com minha parte para a causa. inimigo_hello: Além da minha posição de nascimento, você pode confiar em mim em qualquer circunstância. be_attack: Pegue sua arma e prepare-se para o combate! be_attack_enemy: Você será uma insignificância perto do monumento da minha glória!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: &lt;color=red&gt;pinturas&lt;/color&gt; requintadas sempre trazem cor e alegria à minha vida, como uma tela que ganha vida. olá: Em busca da presa! recusar_recruit_0: Um nobre caçador prefere a solidão em sua caçada. recruta_msg: Você é um caçador habilidoso e um líder digno. Eu te seguirei lealmente. inimigo_hello: Você é minha presa. Não há medo em meu coração. be_attack: Venha, garanto que não irei atingir seus órgãos vitais. Deixe-me lhe ensinar uma lição. be_attack_enemy: A presa se rebela contra seu caçador. Vamos assistir esse confronto acontecer.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Sou apaixonado por pesquisar o &lt;color=red&gt;oculto&lt;/color&gt;. Nada me intriga mais do que descobrir os mistérios escondidos nas sombras. Olá: Você precisa de ajuda? Estou disposto a oferecer minha experiência em assuntos ocultos. recusar_recruit_0: Lamento informar que neste momento não estou interessado em assumir quaisquer responsabilidades adicionais. recruta_msg: Se você puder me fornecer um ambiente propício para continuar minha pesquisa no reino oculto, considerarei me juntar a você. Preciso de mais do que Husnu pode me oferecer. inimigo_hello: Ah, uma pessoa curiosa como você. Tenha cuidado com o que você procura, pois isso pode revelar verdades que você preferiria não saber. be_attack: Você acha que pode me empurrar de volta com ataques simples? be_attack_enemy: Você acha que os mercenários são supersticiosos e covardes? Eu vou te mostrar.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Sou apaixonado por colecionar &lt;color=red&gt;equipamentos especiais&lt;/color&gt;. Também gosto de &lt;color=red&gt;itens artesanais&lt;/color&gt;. Hum? Você tem um presente para mim? Olá sou eu! Aqui estou. recusar_recruit_0: O último líder em quem não pude confiar tornou-se meu inimigo. Não estou disposto a cometer o mesmo erro novamente. recruta_msg: O valor do ouro nunca será transformado em madeira ou pedra. Agradeço sua apreciação e consideração. inimigo_hello: Hm, Bahat poderia estar tramando algo nas sombras? be_attack: Preparem suas lanças! É hora de lutar. be_attack_enemy: Vou te mostrar que você merece vergonha!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah! Por que não comparamos nossos &lt;color=red&gt;itens de combate&lt;/color&gt;? Olá: As cicatrizes não são apenas um testemunho de dor, elas também contam histórias de bravura e resistência. recusar_recruit_0: Eu admiro você, mas isso não significa que vou ceder a você. Ainda tenho minhas próprias metas e objetivos. recruta_msg: Deixe-me mostrar o caminho e juntos alcançaremos a vitória! inimigo_hello: Se você tem algo para me dizer, não tenha medo de me confrontar cara a cara. be_attack: Observe minha espada responder a este desafio! be_attack_enemy: Venha então! Vamos encarar com toda a nossa determinação!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Você sabe, você não pode agradar a todos. Além dos estudos de &lt;color=red&gt;ocultismo&lt;/color&gt;, existem poucos itens adequados para uma sacerdotisa como eu. olá: As chamas dão origem às fênix, mas também à minha pequena! O fogo é meu aliado e protetor. recusar_recruit_0: Por que eu deveria ouvir você? Prefiro confiar no meu fiel escorpião, ele nunca me falha. recruta_msg: De agora em diante, meus leais escorpiões estarão ao seu serviço. Juntos, levaremos nossa força a novos patamares. inimigo_hello: Você é um sacrifício adequado para alimentar o fogo. Não subestime o poder que possuo. be_attack: Em breve você verá a perfeição da minha arte e se arrependerá de ter me enfrentado. be_attack_enemy: Eu invoco você, oh meu pequenino! Deixe meu inimigo saber o calor da minha raiva.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Hm? Me dê aqueles itens de &lt;color=red&gt;luta&lt;/color&gt;, eu adoro eles! olá: O bloqueador de gancho... nunca... erra... recusar_recruit_0: Você não é digno da minha habilidade. recruta_msg: Seu desejo é uma ordem para mim, estarei ao seu dispor. inimigo_hello: Pare, você já está dentro do alcance do meu gancho de bloqueio. be_attack: Gancho bloqueador, pronto para atacar. be_attack_enemy: Deixe o pesadelo começar, você não escapará do meu alcance.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Traga-me &lt;color=red&gt;artesanato&lt;/color&gt;! Quero ver como outros professores os criam! olá: Não existe arma que eu não consiga forjar com maestria! recusar_recruit_0: Você não é digno da minha lealdade! recruta_msg: Perfeito! Eu poderia até forjar uma espada especial para você! inimigo_hello: O que há de errado, não seja tão amargo. be_attack: Ha! Agora posso testar minha nova arma em combate! be_attack_enemy: Você pediu por isso! Venha enfrentar o seu destino!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah? Você tem algum item &lt;color=red&gt;mágico&lt;/color&gt; que eu nunca tenha visto antes? Adoro surpresas e objetos mágicos que despertam minha curiosidade. Olá: Ei! Você quer ouvir uma melodia especial? Posso criar uma sinfonia mágica que irá transportá-lo para outros mundos. recusar_recruit_0: Você tem uma aparência interessante, mas ainda não consegue me fascinar o suficiente para me juntar à sua causa. recusar_recruit_1: Você não vê que estou imerso em meus experimentos de alquimia? Prefiro manter minha liberdade e explorar o potencial da magia sozinho. recusar_recruit_2: Suas habilidades são impressionantes, mas não pense que vou me contentar em ser apenas mais um membro do seu grupo. recusar_recruit_3: Você é insignificante, um mero flash em comparação com o poder e a grandeza que busco. recruta_msg: A magia que emana de você é fascinante e desperta meu interesse. Estou disposto a me juntar à sua causa e descobrir juntos novos horizontes mágicos. inimigo_hello: Aquela poção que você acabou de beber foi apenas uma pequena prévia das minhas habilidades alquímicas. Prepare-se para enfrentar o poder da magia no seu melhor. be_attack: Você é fofo, vou ficar com você para testar meus venenos e feitiços. be_attack_enemy: Nagukka é um lugar adequado para testar suas habilidades. Aqui decidiremos se você merece viver ou ser enterrado sob o peso do meu poder mágico. be_attack: Você é fofo, vou ficar com você para testar meus venenos e feitiços. be_attack_enemy: Nagukka é um lugar adequado para testar suas habilidades. Aqui decidiremos se você merece viver ou ser enterrado sob o peso do meu poder mágico. be_attack: Você é fofo, vou ficar com você para testar meus venenos e feitiços. be_attack_enemy: Nagukka é um lugar adequado para testar suas habilidades. Aqui decidiremos se você merece viver ou ser enterrado sob o peso do meu poder mágico.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Minha mãe era uma pintora excepcional. Não há nada que eu aprecie mais do que &lt;color=red&gt;obras de arte&lt;/color&gt; que me lembrem de seu talento. Olá: instale medo ou enfrente seu destino. Mantenha sua arma por perto. recusar_recruit_0: Deixe-me pensar um pouco mais sobre isso. recusar_recruit_1: Não confio em ninguém. Por que eu deveria confiar em você? recusar_recruit_2: Quem é você... e por que devo me juntar à sua causa? recusar_recruit_3: Me deixe em paz, não quero conversar... inimigo_hello: Cada passo mais perto de mim, a morte se aproxima de você. recruta_msg: Posso realmente confiar em você? be_attack: Vamos lutar até o fim! be_attack_enemy: É melhor morrer em batalha do que se render sem honra.</t>
+  </si>
+  <si>
+    <t>Desc: Uma nobre gosta de &lt;color=red&gt;música&lt;/color&gt;, &lt;color=red&gt;pintura&lt;/color&gt; e, claro, &lt;color=red&gt;história&lt;/color&gt;. O Sr. Hassan gostava de discutir essas coisas comigo. Olá: Um dia! Um dia o Sr. Hassan retornará! recusar_recruit_0: Ainda estou esperando o retorno do Sr. Hassan. recusar_recruit_1: Ambição requer força. Você não tem os dois. recusar_recruit_2: Você se atreveria a tentar comprar um diplomata? A sério? recusar_recruit_3: ...Você é ambicioso. Você precisa da minha ajuda? Por enquanto.. Não posso... inimigo_hello: Você é tão cruel quanto aquela mulher... be_attack: Que vergonha! be_attack_enemy: Você se atreve a intimidar uma senhora com força? Você não é nada comparado aos poderes que testemunhei.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Sou apaixonado por minha coleção de &lt;color=red&gt;equipamentos especiais&lt;/color&gt;. Olá: Quer praticar tiro com arco? inimigo_hello: Aproxime-se e você terá que tomar cuidado com minhas flechas. recusar_recruit_0: Você é forte, mas sua mira não é precisa. Deixe-me pensar. recusar_recruit_1: Você nem merece amarrar a corda do meu arco. recusar_recruit_2: Vá embora, não me incomode. recusar_recruit_3: Você nem veria como eu desenho a flecha. recruta_msg: Ok. Espero que você possa aprender tiro com arco comigo. be_attack: Se é assim que você quer que seja... be_attack_enemy: Você acha que pode se esquivar das minhas flechas? Ridículo.</t>
+  </si>
+  <si>
+    <t>Enredo: Meu sonho de infância era liderar uma magnífica caravana de camelos e explorar terras desconhecidas. &lt;color=red&gt;geografia&lt;/color&gt; sempre foi minha paixão, ouvirei com atenção se você falar comigo sobre esses assuntos. olá: Nunca se esqueça de quem você é, mantenha sempre sua essência presente. recusar_recruit_0: Você não pode encarar a realidade. É difícil acreditar em você. recruta_msg: Seguirei um líder consistente como você. Estou pronto para embarcar nesta aventura juntos. inimigo_hello: O que você está tentando alcançar com tudo isso? Qual é o seu verdadeiro propósito? be_attack: Então resta apenas a batalha, e estou disposto a enfrentá-la com bravura. be_attack_enemy: Com meus camelos você não conseguirá me derrotar! Eu desafio qualquer obstáculo que esteja no meu caminho.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Quando finalmente tenho algum tempo para mim, gosto de tocar meus &lt;color=red&gt;instrumentos musicais&lt;/color&gt;. É nesses momentos que posso mergulhar no mundo da melodia e da harmonia, deixando a música me levar a lugares distantes e a emoções profundas. olá: Mesmo as menores alterações podem levar a resultados muito diferentes. Lembre-se sempre do poder transformador que reside em cada decisão. recusar_recruit_0: É um pouco tarde para me juntar a você agora. Meu compromisso já está em outro lugar. recruta_msg: Esta é, sem dúvida, a decisão mais sábia que você tomou, meu senhor. Estou pronto para atendê-lo com fidelidade e habilidades musicais que irão surpreendê-lo. inimigo_hello: Parece que você não pensou o suficiente sobre as consequências de suas ações. Prepare-se para enfrentar as consequências de suas decisões. be_attack: Eu não esperava que você fosse tão rebelde. be_attack_enemy: Vamos, isso é algo que planejei há muito tempo! Antecipei cada movimento e estou pronto para enfrentar qualquer desafio.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Os &lt;color=red&gt;brinquedos&lt;/color&gt; lindamente elaborados me lembram da minha infância feliz, quando meu pai era governador de Redstone Keep... Eles evocam memórias... Cada detalhe desses objetos me transporta para aqueles lugares cheios. dias de inocência e alegria, relembrando as risadas e os momentos compartilhados naquela época. Olá: Neste mundo há quem procure sempre atacar, assim como há quem se dedique à defesa constante daquilo que ama. recusar_recruit_0: Você é diferente dos outros, mas minhas prioridades estão me levando por um caminho diferente agora. recruta_msg: Você pode vingar meu pai, como eu desejo? inimigo_hello: Se você valoriza sua vida, eu recomendo que você não se torne meu inimigo. be_attack: Você descobrirá a vergonha que pesa sobre o legado do meu pai. be_attack_enemy: Perdoe-me... mas terei que ser implacável.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Nobres só ficam satisfeitos com coisas dignas de &lt;color=red&gt;nobres&lt;/color&gt;! Olá: Nossas tradições são o tesouro mais precioso do mundo inteiro. recusar_recruit_0: Você é um guerreiro corajoso, mas não segue nossas tradições. recusar_recruit_1: Posso confiar em você, mas não vou lutar ao seu lado. recusar_recruit_2: Você não respeita as tradições Akhal, o que significa que você não me respeita. recusar_recruit_3: Por favor, retire-se e deixe-nos em paz. recruta_msg: Você respeita as regras do Akhal, portanto, irei segui-lo lealmente. inimigo_hello: Mesmo sendo inimigos, eu tenho respeito por você. be_attack: Tudo bem, vamos resolver isso seguindo as regras da nossa linhagem! be_attack_enemy: Ótimo, você tem a chance de morrer como um verdadeiro guerreiro!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Todo mundo nascido no Bazar Dourado adora joias de &lt;color=red&gt;ouro e prata&lt;/color&gt;... E eu não sou exceção. Além de joias, também adoro &lt;color=red&gt;itens artesanais&lt;/color&gt;. Olá: Por que você está me incomodando? Estou ocupado. recusar_recruit_0: Você não é uma pessoa má, mas não posso desistir dos meus sonhos para estar com você, mesmo que por um curto período de tempo. recusar_recruit_1: Prefiro buscar riqueza sozinho do que me juntar a você. recusar_recruit_2: Quais são as melhorias nas suas qualificações? Você ainda não atingiu um nível digno de mim. recusar_recruit_3: Por favor, saia agora. recruta_msg: Ok, você me convenceu... Acho que você será útil para mim. inimigo_hello: Você sabe o que penso de você? Olhe nos meus olhos. be_attack: Você não encontrará trabalho no bazar. Você veio aqui para me dar dinheiro? be_attack_enemy: Muito bom. Você está em nossa lista de procurados.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Adoro &lt;color=red&gt;jóias&lt;/color&gt; ou &lt;color=red&gt;enfeites&lt;/color&gt;, qualquer coisa que me deixe mais bonita. Olá Olá! Por que você está me procurando? recusar_recruit_0: Você tem um certo charme, mas há muito pouco mais que me entusiasma em você. recusar_recruit_1: Minha beleza seria desperdiçada ao seu lado. recusar_recruit_2: Amigos? Não, definitivamente não somos. recusar_recruit_3: Criatura nojenta, imploro que você vá embora. recruta_msg: Ok. Parece que estou atraído por você, e estou atraído por você... então não posso te rejeitar. inimigo_hello: Você já se atreve a falar comigo? Ah, você realmente deve estar louco. be_attack: Sério? Quem se atreveria a intimidar uma garota? be_attack_enemy: Achei que em você... finalmente encontrei alguém que praticaria o oculto comigo~</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Uma mulher madura valoriza o conhecimento. Gosto de mergulhar na &lt;color=red&gt;cultura&lt;/color&gt;, pois isso me dá paz e serenidade. olá: Você se encontra diante do líder da Casa Giddah. recusar_recruit_0: Embora eu o admire profundamente, a Casa Giddah precisa da minha liderança neste momento. recusar_recruit_1: Você não merece minha atenção agora. recusar_recruit_2: Hmph. Não se superestime. recusar_recruit_3: Fraco. Saia da minha frente. recruta_msg: Você é forte, talvez juntos possamos enfrentar todos. inimigo_hello: Espero que você entenda claramente sua posição e possa avaliar melhor a minha. be_attack: Não tenho problemas com você. Pensar claramente! be_attack_enemy: Você chega na hora certa. Minha espada estava sedenta por almas.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Do que eu gosto? Objetos &lt;color=red&gt;escondidos&lt;/color&gt; são bons acessórios. Falando em acessórios, os &lt;color=red&gt;ornamentos&lt;/color&gt; não são ruins. Olá: Ugh! Está ventando hoje, hein? recusar_recruit_0: Você é uma boa pessoa, mas... você pode impedir meu progresso. recusar_recruit_1: Acabamos de nos conhecer. Você não precisa fazer tanto por mim. recusar_recruit_2: Você é um sem-teto, sem nome ou casa. Você tem coragem de falar comigo? recusar_recruit_3: Fora, insignificante. recruta_msg: Hahaha! Serei seu aliado e te ajudarei em tudo. Em troca, você me ajudará a ascender à chefia da Casa Giddah! inimigo_hello: Não deveríamos estar conversando, certo? be_attack: Você tem muita coragem de falar assim comigo. be_attack_enemy: Haha! Você chega na hora certa... meus corvos estão com fome!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Gosto de &lt;color=red&gt;combate&lt;/color&gt;... e de &lt;color=red&gt;história&lt;/color&gt;. Olá: Você veio ver Misod? recusar_recruit_0:...Para ser honesto, suas façanhas me emocionam, mas tenho outras coisas que preciso fazer. recusar_recruit_1:Desculpe, devo recusar. recusar_recruit_2:Por favor, saia. Eu tenho outras coisas pra fazer. recusar_recruit_3:Vá embora agora, vilão. recruta_msg: Vamos lutar juntos por um futuro pacífico. inimigo_hello: Procuramos coisas diferentes. Você deveria ir embora. be_attack: Você parece determinado a lutar. Eu lhe darei o que você procura. be_attack_enemy: Estou feliz que você veio. Você evitou brigar comigo por um tempo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: &lt;color=red&gt;História&lt;/color&gt; é a &lt;color=red&gt;história&lt;/color&gt; da vida. Gosto de história e adoro as próprias histórias. Olá Olá! Você quer ouvir uma música? recusar_recruit_0: Agradeço você, mas valorizo ​​​​minha liberdade. recusar_recruit_1: Obrigado, mas não posso lhe dar a resposta que você procura. recusar_recruit_2: Não tenho motivos para acompanhá-lo, tenho? recusar_recruit_3: Não trilhamos o mesmo caminho. Por favor vá. recruta_msg: ♫ Um aventureiro e um bardo, agora o caminho será mais fácil ♫ inimigo_hello: Você fez algumas coisas malignas. Estou errado? be_attack: Ei! Você tem certeza de que quer fazer isso? Você realmente é louco. be_attack_enemy: Então você me encontrou. Você me salvou algum tempo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Me gustan las cosas &lt;color=red&gt;tristes&lt;/color&gt;, &lt;color=red&gt;románticas&lt;/color&gt;... o cualquier cosa relacionada con la &lt;color=red&gt;Diosa del Río&lt;/color&gt; , claro. Olá: Você... por que você me encontrou? recusar_recruit_0: Você é uma boa pessoa, mas eu... eu... não posso te ajudar. recusar_recruit_1: Eu... eu não gosto de viajar com outras pessoas. recusar_recruit_2: Não quero ser um fardo, por favor, não me pergunte isso. recusar_recruit_3: Você poderia sair? recruta_msg: Tenho cabelos pretos e olhos azuis de Nefrit. Acredito que há um poder em minha linhagem esperando que eu o desperte. Obrigado por acreditar em mim. Eu vou lutar com você. inimigo_hello: Dizem... que você não é uma boa pessoa... be_attack: Ok. Não terei medo. be_attack_enemy: Vou impedir você. Vir.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Gosto de &lt;color=red&gt;equipamentos muito especiais&lt;/color&gt; ou &lt;color=red&gt;tesouros&lt;/color&gt; desconhecidos pelos mortais. Olá: Você está procurando por mim ou minha espada? recusar_recruit_0: Você é corajoso, mas não é forte. recusar_recruit_1: Hmph. Não somos da mesma casa. recusar_recruit_2: Hum. recusar_recruit_3: Eu não gosto de você! recruta_msg: A esgrima da Casa Giddah é invencível. inimigo_hello: Você é tão desprezível quanto aquelas minhas duas irmãs. be_attack: Já fui traído. Não há nada que você possa fazer para me machucar. be_attack_enemy: Você quer testemunhar a arte da espada da Casa Giddah? Então testemunhe!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Meu pai é ceramista em Cotta City, então desde que eu era jovem eu gosto de &lt;color=red&gt;artesanato&lt;/color&gt;, especialmente esculturas. Também gosto do &lt;color=red&gt;equipamento muito especial&lt;/color&gt; que ouvi ser mencionado nas lendas. Descrição: A única coisa que você pode proteger é seu próprio punho. Exemplo: Sinto muito. Eu estou muito ocupado. 拒绝指教: Haha! Eu conheço você? Por que eu deveria te ensinar? 完成委托: Nada mal. Eu não esperei nada menos. 乞讨冷却中: Você está implorando de novo tão cedo? Não é uma boa imagem. Olá: O que você precisa de mim? recusar_recruit_0: Você...suspiro Não, ainda não posso entrar na sua equipe. recusar_recruit_1: Ainda somos estranhos e não há nada que me atraia em você. recusar_recruit_2: Lut Jahim não serve aos fracos. recusar_recruit_3: Saia! recruta_msg: Você me lembra meu pai, não o homem que me gerou, mas aquele que me ensinou a viver. Eu te ajudarei. Espero que você não traia minha confiança. inimigo_hello: Você é um verme. E tão cego quanto um também. be_attack: Eu sou excelente em batalha! be_attack_enemy: Haha! Você é corajoso e tolo ao mesmo tempo!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Do que eu gosto? Dinheiro. Quem não gosta de dinheiro? Ah, objetos? &lt;color=red&gt;Jóias&lt;/color&gt; podem ser convertidas em dinheiro. E itens para &lt;color=red&gt;combate&lt;/color&gt; que me ajudam a ganhar dinheiro. olá: Um andarilho, sem casa para onde voltar. recusar_recruit_0: Infelizmente, você está errado. Gostaria de te acompanhar, mas... também quero viver. recusar_recruit_1: Você também não parece rico. Esqueça. recusar_recruit_2: Se quiser me contratar, siga o caminho certo. recusar_recruit_3: Nojento! Vá para o inferno, verme. recruta_msg: Espero que você encontre um lugar para esse sem-teto retornar. inimigo_hello: Esse sem-teto odeia você. be_attack: Lute! Luta! be_attack_enemy: Vou adorar tirar seu Utar de você.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Gosto de &lt;color=red&gt;artesanato&lt;/color&gt;, &lt;color=red&gt;joias&lt;/color&gt;... e da Astrid! Olá: Está aqui para me pagar uma rodada? recusar_recruit_0: Se você fosse Astrid, eu não hesitaria. Mas você não é ela. recusar_recruit_1: Eu? Tem certeza? Esqueça. Olá! recusar_recruit_2: Você deve estar bêbado. Eu estou bêbado. Não se pode fazer. recusar_recruit_3: Fique longe, vou vomitar. recruta_msg: Bom! Eu tenho que perguntar, tem bebida alcoólica? inimigo_hello: Olá! Seu rosto me deixa enjoado. be_attack: Espere, deixe-me clarear minha cabeça. be_attack_enemy: Estou trabalhando. Espere um segundo, você é meu alvo? Obrigado.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Não gosto de muitas coisas, só de bugigangas ou instrumentos interessantes. Mas odeio muitas coisas, principalmente rosas brancas e capas brancas. olá: O Sol Negro introduziu um poder primordial no mundo. Os pensativos o terão acordado. recusar_recruit_0: Você não é ruim. Mas devo fazer algumas pesquisas importantes primeiro. recusar_recruit_1: Por que eu deveria concordar se você não tem nenhum vestígio de poder primordial? recusar_recruit_2: Saia daqui. Você é tão irritante quanto um druida. recusar_recruit_3: Deixe-me ou você será estrangulado pelas minhas vinhas. recruta_msg: Bom. Talvez eu faça uma descoberta com você. inimigo_hello: Idiota arrogante! Só de olhar para você posso dizer que você não respeita a natureza. be_attack: Contemple o poder da natureza! be_attack_enemy: Muito bom. Estava te procurando.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物：Eu definitivamente adoro &lt;color=red&gt;artesanato&lt;/color&gt;. Gosto de ver a emoção que um artesão coloca em seu trabalho. Cada artesanato tem sua própria alma. Olá: (Tosse seguida de risada) Olá! tosse Desculpe, o que você disse? recusar_recruit_0:Você parece uma pessoa muito sensata, mas... me desculpe. recusar_recruit_1:tosse Perdoe-me. Você simplesmente não é meu tipo. recusar_recruit_2: Hehe. Você deve estar brincando. Você tem que perguntar de novo? recusar_recruit_3:Não tenho nada para lhe contar. recruta_msg:Tenho certeza que um humilde artesão como eu tem muito pouco a oferecer. Muito bem. É estranho ser tão admirado. inimigo_hello:Você e eu somos inimigos agora. tosse Você não deveria me procurar. be_attack:Eu não gosto de discutir. tosse be_attack_enemy:Não há outra opção. Prefiro não discutir.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto de &lt;color=red&gt;brinquedos&lt;/color&gt; &lt;color=red&gt;fofos&lt;/color&gt; Hehe, hmm! Também gosto de alguns tipos de &lt;color=red&gt;equipamentos especiais&lt;/color&gt;. olá: Olá, sou Muta'aliq! recusar_recruit_0: Você parece bem, mas... tenho que continuar procurando pelos meus pais. recusar_recruit_1: Obrigado pela oferta, mas não posso aceitá-la. recusar_recruit_2: Eu nem conheço você. recusar_recruit_3: Bem... na verdade, eu realmente não gosto de pessoas como você. Por favor, não me pergunte novamente. recruta_msg: Ok... vou acompanhá-lo. Espero que você não se importe com minha presença. inimigo_hello: Não! Não chegue mais perto! be_attack: Então você realmente é esse tipo de pessoa. Estou decepcionado. be_attack_enemy: Não estou surpreso que você tenha feito isso.</t>
+  </si>
+  <si>
+    <t>Sou apaixonado por &lt;color=red&gt;combate&lt;/color&gt;, é o que mais gosto! Nada me deixa mais feliz do que estar no meio da batalha. Além disso, adoro ouvir &lt;color=red&gt;histórias&lt;/color&gt;. Desde pequeno fiquei fascinado por ouvir histórias e lendas. Olá: Você nunca viu um guerreiro antes? Não me olhe Assim. recusar_recruit_0:Você poderia ser um bom aliado, mas tenho assuntos inacabados que preciso resolver primeiro. recusar_recruit_1:Você ainda não provou seu valor. recusar_recruit_2:Você está brincando comigo? recusar_recruit_3:Diga mais uma palavra e eu enfiarei minha lança em seu peito. recruta_msg:Você conquistou o respeito de Astrid, a Não Juramentada! inimigo_hello:Fuja. Vou te dar tempo para escapar. be_attack: Ha! Aceito seu desafio. be_attack_enemy:Você é um oponente formidável. Eu, Astrid, aceito com prazer o seu desafio!</t>
+  </si>
+  <si>
+    <t>Gosto de coisas &lt;color=red&gt;românticas&lt;/color&gt;, &lt;color=red&gt;instrumentos&lt;/color&gt; e alguns &lt;color=red&gt;brinquedos divertidos&lt;/color&gt;. Desculpe, eu sei que pareço um pouco ingênuo. Olá Olá! Precisa de ajuda? recusar_recruit_0: Gostaria de ajudá-lo, mas há outras pessoas que precisam de mim. recusar_recruit_1: Sinto muito, não há nada que eu possa fazer por você. recusar_recruit_2: Não posso, há outras coisas que preciso fazer. recusar_recruit_3: Você é uma pessoa má, não quero ter nada a ver com você. recruta_msg: Espero que rosas brancas floresçam em todos os cantos do mundo! inimigo_hello: Oh, espero que nossos lados possam se comunicar mais. be_attack: Você realmente vai fazer isso? Eu esperava que pudéssemos ser amigos. be_attack_enemy: Não faz sentido. Não posso negar nada aos outros.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Adoro &lt;color=red&gt;artesanato&lt;/color&gt; como escudos e estátuas. Estas criações têm um encanto místico que me fascina. 招募对话: Normalmente prefiro não me juntar a outros, mas se você estiver disposto a investir Utar para me contratar... talvez eu possa reconsiderar. Olá, como posso ajudá-lo? recusar_recruit_0:...Sinto muito, mas não posso. recusar_recruit_1:Não estou convencido. recusar_recruit_2:Não, obrigado. recusar_recruit_3:Saia, não estou interessado. recruta_msg:...Ok, conto com você. Espero que você não me decepcione. inimigo_hello:Você e eu somos inimigos agora. be_attack:Para a batalha, então! be_attack_enemy:Você pediu por isso.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Hm, carne Ifrit grelhada? Ou frango assado? Embora esses não tenham um gosto bom frio. O que mais eu gosto além de comida... ah! &lt;color=red&gt;Artesanato&lt;/color&gt; e atlas de &lt;color=red&gt;geografia&lt;/color&gt;. Desejo viajar pelo mundo um dia. olá: Olá, olá, olá! Eu sou um mágico, não um guerreiro. recusar_recruit_0:Hein? Um convite para mim? Ah... não, ainda não é hora. recusar_recruit_1:Você quer minha ajuda? Claro. Que? Você quer minha ajuda por quanto tempo? Deixa eu pensar. recusar_recruit_2:Não, não, não. Tenho que estar em casa para jantar. recusar_recruit_3:Infelizmente, Kunju não pode ir com você. recruta_msg:Ah, que bom! Lutaremos juntos! Quem disse que um homem da minha altura não pode ser mágico? inimigo_hello: Olá! Olá, olá, oh! É você. Eu não posso falar com você. be_attack:Ei! Fiz algo mal? be_attack_enemy: Você chegou bem na hora! Tenho um novo feitiço que quero experimentar... Na verdade, aprendi há muito tempo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Habilidade em &lt;color=red&gt;combate&lt;/color&gt; me torna mais forte na batalha. A familiaridade com a &lt;color=red&gt;geografia&lt;/color&gt; me ajuda a sobreviver. Não preciso de nada mais. Olá: Ei! Você está no meu caminho. recusar_recruit_0: Deixe-me considerar. recusar_recruit_1: Esqueça. Você claramente não é forte o suficiente. recusar_recruit_2: Eu? Hmph. Eu não caio junto com os outros. recusar_recruit_3: Se continuar falando assim, você acabará morto. recruta_msg: Você e eu somos parecidos. Te seguirei! inimigo_hello: Não chegue mais perto. be_attack: Vamos ver o quão capaz você é. be_attack_enemy: Você é ousado. Vir!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Adoro &lt;color=red&gt;pinturas&lt;/color&gt; e &lt;color=red&gt;histórias&lt;/color&gt;... Essas coisas me fazem esquecer as partes mais desagradáveis ​​da vida. Eu não gosto de mais nada. Olá: sou Hartum, de Diresprings. recusar_recruit_0:...Não, meus pais recusariam. recusar_recruit_1:Não posso me juntar a você. Sinto muito. recusar_recruit_2:Hartum abaixa a cabeça recusar_recruit_3:Saia daqui! Deixa-me só. recruta_msg:Espero não ser um incômodo para você. inimigo_hello:Diga-me o que você tem a dizer. be_attack:Outro inimigo? Não me surpreende. be_attack_enemy:Não está em nosso destino ser companheiros. Desculpas.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Estou interessado principalmente em &lt;color=red&gt;História&lt;/color&gt;. De vez em quando, também fico curioso sobre &lt;color=red&gt;objetos&lt;/color&gt; ocultos. 招募对话: Eu prefiro ser um solitário, a menos que você esteja disposto a financiar minha pesquisa com algum Utar... ou você pode me fazer mudar de ideia. Olá: Existem muitos estranhos neste deserto. recusar_recruit_0: Você pode ser um bom recurso para estudar materiais antigos. Mas... hah. Esqueça. É algo que tenho que fazer sozinho. recusar_recruit_1: Hum. Não é suficiente. Você não parece inteligente o suficiente. recusar_recruit_2: Escute, cara, tenho outras coisas para fazer. recusar_recruit_3: Troglodita. Você não tem algo interessante para me contar? recruta_msg: Muito bom. Sua equipe pode se beneficiar de uma pessoa experiente, para variar. inimigo_olá: Você não está procurando problemas, está? be_attack: Leia um livro; Isso o tornará menos imprudente. be_attack_enemy: São tolos como você que atrapalham o progresso.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Você quer saber como são os ceifadores de almas do deserto? Nós sobrevivemos apenas com humor negro... e na verdade, os &lt;color=red&gt;tesouros escondidos&lt;/color&gt; e os &lt;color=red&gt;equipamentos especiais&lt;/color&gt; não são ruins. Olá: Você viu o líder dos Corsacs? recusar_recruit_0: Você e eu somos muito parecidos, mas você ainda me deve algo. recusar_recruit_1: O cheiro de sangue não é forte o suficiente em você. recusar_recruit_2: Ha ha! Em teus sonhos! recusar_recruit_3: Você quer ser uma alma que colhe? recruta_msg: Vamos caçar juntos! inimigo_hello: Você está trabalhando com os Corsacs? Seja honesto. be_attack: Vou matar seus descendentes e Khurram Aslae também! be_attack_enemy: Yaaaaah! Então vamos!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Bem, eu gosto de &lt;color=red&gt;cultura&lt;/color&gt;, &lt;color=red&gt;tesouros&lt;/color&gt; e &lt;color=red&gt;equipamentos especiais&lt;/color&gt;. Também gosto de justiça para todas as pessoas do mundo! Olá: A justiça prevalecerá! recusar_recruit_0: O deserto precisa de talentos como você, mas é uma pena que esse velho esteja ficando rígido. Eu não quero ir muito longe. recusar_recruit_1: Obrigado pelo convite! Estou muito velho para ir embora. recusar_recruit_2: Não posso, tenho coisas importantes para fazer. recusar_recruit_3: Você deveria fugir e não dizer palavras tão malucas. recruta_msg: Aja com justiça e a justiça o seguirá. inimigo_hello: Não negocia com bandidos. be_attack: Parece que só meu nome não é suficiente para assustar você. be_attack_enemy: Ha!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Prefiro não ser incomodado. Considerando o que eu gosto é um pouco chato. Hm... Se você tiver que perguntar, provavelmente são livros cheios de &lt;color=red&gt;histórias&lt;/color&gt; ou &lt;color=red&gt;artesanato&lt;/color&gt;. Olá: Ah... que incômodo. recusar_recruit_0:Recebo tão poucas visitas, mas não quero me mudar. recusar_recruit_1:É muito problemático. Esqueça. recusar_recruit_2:Eu recuso. Não quero entrar em águas turvas. recusar_recruit_3:É melhor você calar a boca. recruta_msg:Que incômodo... Ai! Bom. Bom. Posso ver que você é muito sincero. inimigo_hello:Pare de me incomodar. be_attack:Eu disse para parar de me incomodar. be_attack_enemy:Então você quer "consertar as coisas", hein?</t>
+  </si>
+  <si>
+    <t>喜欢的礼物：Eu gosto de músicas &lt;color=red&gt;românticas&lt;/color&gt; ou &lt;color=red&gt;tristes&lt;/color&gt;. Minha esposa também gosta de ouvi-los. olá:Magia de cura...muito importante. recusar_recruit_0:Eu admiro você, mas isso não é suficiente. recusar_recruit_1:Não consigo fazer isso. Eu tenho ordens. recusar_recruit_2:Espero que você esteja brincando. recusar_recruit_3:É uma pena que minha magia de cura não consiga consertar o que há de errado com sua cabeça. recruta_msg:Muito bom. Informarei a Sociedade da minha partida. inimigo_hello: Renda-se agora e sua proteção como prisioneiro estará garantida. be_attack:Seu absurdo não pode ser curado com arcano, apenas a lâmina pode fazer isso. be_attack_enemy:Reze à Deusa do Rio para que seus ferimentos não sejam muito graves. Não estou interessado em ver você implorar por misericórdia.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Não há ninguém que resista a uma &lt;color=red&gt;história romântica&lt;/color&gt;. Assim como ninguém resiste a um jovem nobre generoso e elegante! olá: Pare de olhar, há algo errado com seus olhos? recusar_recruit_0:Hahaha, outro sucumbiu aos meus encantos? Claro. Claro! No entanto... estou muito animado para ver o que mais você tem a oferecer. recusar_recruit_1: Ah? Você acha que um nobre pode ser comprado e vendido tão facilmente? recusar_recruit_2:Infelizmente, outro fã obcecado. Deixe-me dizer devagar para que você entenda: eu. Eu me recuso. recusar_recruit_3:Oh, odeio ser cruel, mas você é o tipo de pessoa que detesto absolutamente. recruta_msg:Minha resposta é... sim! Claro!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Em primeiro lugar, não gosto de nada que o estúpido do Goldie goste! Hmph! Eu gosto de &lt;color=red&gt;jogos&lt;/color&gt; &lt;color=red&gt;fofos&lt;/color&gt;! Ou belos &lt;color=red&gt;instrumentos&lt;/color&gt;! olá: Ding-ding-dong, não me incomode! recusar_recruit_0: Hmph! Vou pensar sobre isso... vou pensar sobre isso... recusar_recruit_1: Ugh, pare de tentar! Isso não vai acontecer! recusar_recruit_2: Não vou! Não vou me deixar usar por ninguém! Hmph! recusar_recruit_3: Que chato! Você é tão chato quanto Goldie! Te odeio! recruta_msg: Hmph! Bom! Você fica perguntando de novo e de novo, é realmente chato! inimigo_hello: Pare de me incomodar. Não quero falar contigo. be_attack: Ugh! Você é a pessoa mais chata que já conheci hoje! be_attack_enemy: Ding-dong, ding-dong, agora você está com problemas!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物：Hm... Eu gostaria de aprender &lt;color=red&gt;geografia&lt;/color&gt;. Olá: eu vou te encontrar, pai. recusar_recruit_0:Você é muito gentil, mas ainda tenho que procurar meu pai. recusar_recruit_1:Não posso, obrigado pela compreensão. recusar_recruit_2:Você já deve saber que irei rejeitá-lo. recusar_recruit_3:Eu não quero ver você! recruta_msg:Esta espada me foi dada pelo meu pai. Espero não decepcioná-lo. Eu vou com você.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物：Eu gosto de coisas &lt;color=red&gt;românticas&lt;/color&gt; e &lt;color=red&gt;ocultas&lt;/color&gt;. E tudo sobre a linda &lt;color=red&gt;deusa&lt;/color&gt; é uma obra de arte maravilhosa! Olá: Vermelho! A essência deste mundo! recusar_recruit_0:Se você trocar suas roupas vermelhas, talvez eu considere isso. recusar_recruit_1: Ah? Você quer que eu trabalhe para você? Você não está me oferecendo o suficiente para considerar isso. recusar_recruit_2:Por que você quer que eu te ajude? recusar_recruit_3: Hahaha! Olha, você é certamente a pior criação do Criador. recruta_msg:Vou deixar o mundo vermelho como sangue para você.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Os escaladores gostam de &lt;color=red&gt;ler&lt;/color&gt; ou ouvir &lt;color=red&gt;histórias&lt;/color&gt;. Olá: Todas as respostas são encontradas no topo de uma montanha. recusar_recruit_0: Gostaria de acompanhá-lo, mas Ilyas está esperando por mim. recusar_recruit_1: Ainda não escalei o pico mais alto da cordilheira mais a leste. Não tenho tempo para mais nada. recusar_recruit_2: Hmph. Eu não tenho uma resposta para você. recusar_recruit_3: Não fique muito confiante! recruta_msg: Muito bom. Talvez eu encontre novas maneiras de me exercitar.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Você vai apostar comigo? Gosto de &lt;color=red&gt;jóias&lt;/color&gt; ou coisas que &lt;color=red&gt;aumentam meu moral na batalha&lt;/color&gt;. Olá: Quer apostar comigo? recusar_recruit_0:Vamos jogar. Eu irei com você se você vencer. Hmm... você não parece ter nada para me dar se perder. Esqueça. recusar_recruit_1:Alguém como você quer que eu participe? recusar_recruit_2: Hahaha! Ir para o inferno. recusar_recruit_3:Você me lembra daquele que tirou tudo de mim! Sair! recruta_msg:Ok. Vou jogar um jogo com você.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto de coisas &lt;color=red&gt;tristes&lt;/color&gt; que ressoam em minha alma. Além disso, espero encontrar &lt;color=red&gt;equipamentos especiais&lt;/color&gt; que possam me ajudar na batalha. olá: O estilo de luta da minha família nunca morrerá enquanto eu estiver por perto. recusar_recruit_0:Você sabe que carrego uma grande responsabilidade. Eu não posso aceitar. recusar_recruit_1:Você não é o tipo de pessoa que eu admiro. recusar_recruit_2:Não, e não pergunte novamente. recusar_recruit_3:Não consigo controlar minha raiva por muito mais tempo. Saia agora. recruta_msg:Ok. Espero que você possa divulgar meu estilo de luta para o mundo inteiro.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Gosto quando as pessoas ficam &lt;color=red&gt; tristes&lt;/color&gt; e sofrem. Também gosto de passar o tempo olhando &lt;color=red&gt; pinturas&lt;/color&gt;. olá: Gosto da sua expressão melancólica... recusar_recruit_0: Ei, você ainda não foi longe o suficiente. recusar_recruit_1: Ah... ainda não o suficiente para me fazer ajoelhar. recusar_recruit_2: Você está delirando. recusar_recruit_3: Você nem vale a pena trabalhar em busca de componentes misteriosos. recruta_msg: Espero que você possa me ajudar a colher mais dor e sofrimento.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Não tenho amor por nada neste mundo. No entanto, estou interessado em &lt;color=red&gt;histórias&lt;/color&gt;, &lt;color=red&gt;histórias&lt;/color&gt; e em encontrar equilíbrio. olá: Equilíbrio para todos. recusar_recruit_0: Eu? Seguir você? Hm, não, isso não pode estar certo. recusar_recruit_1: Não quero perturbar as águas calmas. recusar_recruit_2: Isso não seria justo, seria? recusar_recruit_3: ...Eu vou destruir você. recruta_msg: Bem, juntos tornaremos o mundo um lugar mais justo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto de &lt;color=red&gt;música&lt;/color&gt; e algumas coisas &lt;color=red&gt;tristes&lt;/color&gt; ou &lt;color=red&gt;românticas&lt;/color&gt;. As emoções são muito importantes para um dançarino. Olá: eu gosto de dançar! Algum dia irei dançar no grande palco de Jamal City. recusar_recruit_0: Acho que nos damos muito bem, mas... não vou desistir do meu sonho por você. recusar_recruit_1: Eu gosto de dançar. Se você quer que eu lute... me desculpe. recusar_recruit_2: Você está falando sério? Tudo bem, se você estivesse apenas brincando. recusar_recruit_3: Bem, não vou mentir para você. Eu não gosto muito de você. recruta_msg: Vale a pena seguir você. Vamos, espero que você me aconselhe no futuro.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物：Eu gosto de &lt;color=red&gt;cultura&lt;/color&gt; e &lt;color=red&gt;música&lt;/color&gt;! Você vai me dar um presente? Olá: Sou guarda-caça ou boticário? Eu sou ambos! recusar_recruit_0:Não se preocupe, deixe-me pensar sobre isso, ok? recusar_recruit_1:Já ​​pensei nisso, mas por enquanto devo rejeitá-lo. recusar_recruit_2:Sinto muito, devo recusar seu convite. Espero que você não esteja muito desapontado. recusar_recruit_3:Não, você não parece gostar muito de boticários. recruta_msg:Vou avisar com antecedência que posso ser um pouco complicado. Espero que você esteja bem com isso! inimigo_hello:Não mexa com o suprimento de um boticário. be_attack:Você realmente me decepcionou. be_attack_enemy:Você será uma excelente cobaia para minha nova poção.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Gosto de ouvir &lt;color=red&gt;histórias&lt;/color&gt; e admirar &lt;color=red&gt;pinturas&lt;/color&gt;. Olá: Não chegue mais perto... vou te machucar. recusar_recruit_0:Eu... quero me juntar a você, mas... sinto muito. recusar_recruit_1:Agora não é a hora. Sinto muito. recusar_recruit_2:Não... não posso lhe dar a resposta que você deseja. recusar_recruit_3:Eu não quero olhar para você. Não consigo controlar meu poder. Você deveria ir embora. recruta_msg:Ainda não consigo controlar o poder dentro de mim. Espero que você possa me ajudar a dominá-lo. inimigo_hello:Aconselho você a não me irritar. Eu não posso me controlar. be_attack:Esta é a pior decisão que você poderia ter tomado. be_attack_enemy:Agora vou ficar com raiva!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Alguns itens escondidos ou equipamentos especiais me distraem por tempo suficiente para que eu abaixe minha espada. Olá: Julgamento. Julgamento por todos os pecados deste mundo. recusar_recruit_0: Você não vale a pena erguer minha espada. recusar_recruit_1: Pergunte novamente e corto sua língua. recusar_recruit_2: Você exala um cheiro de pecado. recusar_recruit_3: Você quer que minha espada responda por mim? recruta_msg: Juntos, exerceremos a justiça. inimigo_hello: Outros vão te condenar, eu vou te julgar. be_attack: Já vi muitas almas lamentáveis ​​como você. be_attack_enemy: Seu julgamento: execução!</t>
+  </si>
+  <si>
+    <t>没耐心: Com licença! Há muitas pessoas importantes esperando por mim. Vamos conversar outra hora. 拒绝指教: Você acha que pode ser como eu? Hahaha, sinto muito. Eu não ensino. 完成委托: Nada mal. Parece que você sabe como fazer o trabalho. 乞讨冷却中: Você já está implorando por mais esmolas tão cedo? Não é uma boa foto... 乞讨成功: Hahaha! Bom! Você fez este velho muito feliz. Aqui está sua recompensa! 喜欢的礼物: Um presente do outro lado do rio? Dê-me &lt;color=red&gt;jóias&lt;/color&gt; ou alguns itens &lt;color=red&gt;escondidos&lt;/color&gt;. Olá: O que você adquiriu do rio? recusar_recruit_0: Posso agradecer-lhe respeitosamente por adquirir essas joias para mim, mas não posso lhe dar a resposta que deseja. recusar_recruit_1: Ao seu lado, eu só veria extensões áridas e infinitas. Estas terras não me atraem. recusar_recruit_2: Você não pode se comparar ao rio em movimento. recusar_recruit_3: Pessoa nojenta. Você será uma alma perdida no fundo do rio. recruta_msg: Você deve querer algo importante do rio se estiver contratando um resgatador como eu. Emin está ao seu serviço!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto de &lt;color=red&gt;artesanato&lt;/color&gt; ou de alguns itens &lt;color=red&gt;escondidos&lt;/color&gt;. Olá: Cuide da sua sombra. recusar_recruit_0:Já pensei sobre isso. Você não tem motivos para arriscar minha vida. recusar_recruit_1:O que você pode me oferecer? Por que eu deveria seguir você? recusar_recruit_2:Ugh. Delirante. recusar_recruit_3:Saia daqui. Sinto vontade de matar. recruta_msg:Talvez seguindo você eu possa entender melhor meus próprios desejos. inimigo_hello:Agir irracionalmente custará sua vida. be_attack: Assassinos não te assustam? Eu vou te mostrar por que eles deveriam. be_attack_enemy:Você é meu próximo alvo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Gosto de muitas coisas, como coisas &lt;color=red&gt;tristes&lt;/color&gt; e &lt;color=red&gt;românticas&lt;/color&gt;, ou instrumentos &lt;color=red&gt;bons&lt;/color&gt;. Ah, também coisas relacionadas à &lt;color=red&gt;deusa&lt;/color&gt;... É muita coisa, mas eu amo esse mundo! Olá: eu amo o mundo! recusar_recruit_0:Sei que somos bons amigos, mas... sinto muito, não tenho coragem suficiente para embarcar em uma jornada com você. recusar_recruit_1:Perdoe-me por dizer "não". Ugh, não sou bom em dizer não! recusar_recruit_2:Obrigado por me convidar, mas há outras coisas que preciso fazer. recusar_recruit_3:...Eu não quero falar com você. recruta_msg:Vejo uma luz brilhando em você. Essa luz acalma meu coração.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Entendido, &lt;color=red&gt;cultura&lt;/color&gt; e &lt;color=red&gt;artesanato&lt;/color&gt;. Agora não me distraia com minha pesquisa. olá: Não importa o quão forte você seja, você nunca será capaz de me derrotar completamente. recusar_recruit_0:Estou lisonjeado por você me respeitar dessa forma, mas quero viver em liberdade. recusar_recruit_1:Desculpe, mas minhas máquinas são mais interessantes para mim. recusar_recruit_2:Você vê essas ferramentas que tenho em mãos? Ainda tenho coisas para fazer. recusar_recruit_3:Você deveria ir a algum lugar para clarear sua cabeça. recruta_msg:Ok. Você não me deixa muitas opções.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Eu só quero &lt;color=red&gt;equipamentos especiais&lt;/color&gt; e &lt;color=red&gt;decorações&lt;/color&gt;. Eu já tenho o resto. olá: Onde está o lendário Mestre Espadachim de Zagros? recusar_recruit_0: Ha ha ha, você tem coragem! Mas tenho que dizer não, espero que esteja tudo bem. recusar_recruit_1: Você simplesmente não está qualificado. recusar_recruit_2: Ha ha ha! Em teus sonhos! recusar_recruit_3: Você é uma coisa flagrantemente feia. recruta_msg: Ótimo! Não há tempo para bobagens, vamos lá!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Gosto de coisas cheias de mistério e tristeza ocultos. Além disso, gosto muito de tocar instrumentos musicais, embora já não o faça há muito tempo. Olá: No começo somos todos um. No final, voltamos a essa unidade. recusar_recruit_0: Hmm, é mesmo? Não posso aceitar neste momento. recusar_recruit_1: Não estou acostumado a viajar com outras pessoas. recusar_recruit_2: Não gosto dessa ideia. recusar_recruit_3:... recruta_msg: Talvez juntos possamos descobrir a verdade do mundo.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Sabor dos presentes: &lt;color=red&gt;Combate&lt;/color&gt;, pois o combate é a forma mais elevada de &lt;color=red&gt;romance&lt;/color&gt;! Se eu pudesse ter alguns &lt;color=red&gt;instrumentos musicais&lt;/color&gt;, seria ainda melhor, para que eu pudesse tocar a canção da morte! Olá: Ouça! Você consegue ouvir o lamento dos moribundos? recusar_recruit_0:Você acha que me dando bugigangas você pode contratar o melhor assassino do deserto? recusar_recruit_1: Hahaha! Nem todo mundo ousaria me perguntar isso. Mas ainda assim, devo recusar. recusar_recruit_2:Você está implorando pela minha ajuda ou apenas implorando pela morte? recusar_recruit_3:Mal posso esperar para ouvir o som que você fará quando morrer. recruta_msg:Ok. O cheiro de sangue em você me fascina.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto de &lt;color=red&gt;combate&lt;/color&gt;... das coisas &lt;color=red&gt;escondidas&lt;/color&gt;... Gosto muito disso. Olá: Hehehe, o que você quer? recusar_recruit_0:Você também tem a sombra de um monstro. Mas não é suficiente. recusar_recruit_1:Hehehe, você gosta de monstros? Mas eu não gosto de você. recusar_recruit_2:Hehe, você tem o fedor de um humano! Me dá nojo! recusar_recruit_3: Hahaha! Barragens! Corra em direção à saída! Corram por suas vidas, fracos! recruta_msg:Hehehe, gosto da sua persistência. inimigo_hello:Hehehe pequeno lagarto, você vê quem veio? be_attack:Hehehe... hehehe... be_attack_enemy: Presa! Entregue na minha porta!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Hm, eu escolho &lt;color=red&gt;artesanato&lt;/color&gt;. Eu me pergunto se eu também poderia me considerar uma arte. Olá:...O que você quer de mim? recusar_recruit_0:Você gosta de mim ou do meu corpo mecânico? De qualquer forma, eu não gosto de você. recusar_recruit_1:Se você procurar a ajuda deste guerreiro mecânico, terá que trabalhar sua sinceridade. recusar_recruit_2:Já ouvi piadas suficientes. Não diga mais. recusar_recruit_3:Vá embora, seu fracote inútil. recruta_msg:Você testemunhará o maior poder da herdeira da cidade de Jamal!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Gosto... da &lt;color=red&gt;música&lt;/color&gt; dos nômades, assim como dos finos &lt;color=red&gt;instrumentos&lt;/color&gt;. Olá: Ouça. Você consegue ouvir a música do deserto? recusar_recruit_0:Você é um bom ouvinte, mas não quero tocar só para você. recusar_recruit_1:Nunca sonhei em ser assistente de alguém, entendeu? recusar_recruit_2:Talvez você ficasse satisfeito com alguma decoração bonita, mas não é isso que eu quero. recusar_recruit_3:Algo em você realmente não gosta de mim. recruta_msg:Bem, nos próximos dias, permita-me cantar para você.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Gosto de tudo relacionado a &lt;color=red&gt;música&lt;/color&gt; ou céus distantes. Olá: caí do firmamento apenas para ser enterrado na poeira. recusar_recruit_0: Seu futuro não requer minha participação. recusar_recruit_1: As estrelas me guiam. Você não pode bloquear sua luz. recusar_recruit_2: Seu brilho é tão fraco que me deprime. recusar_recruit_3: Não gosto da sua aura caída. recruta_msg: Eu irei te seguir. Você pode me levar para casa?</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: &lt;color=red&gt;Fofos&lt;/color&gt; &lt;color=red&gt;ornamentos&lt;/color&gt;! Que? Não te agradam? olá: Deixe Batu te dar um abraço tranquilo! recusar_recruit_0: Você é uma pessoa interessante. Mas Batu tem outras coisas para fazer. recusar_recruit_1: Deixe Batu pensar sobre isso. recusar_recruit_2: Ah, é mesmo? Mas não tenho motivos para aceitar sua oferta. recusar_recruit_3: Você é uma pessoa violenta! Batu te odeia! recruta_msg: Ok, eu aceito! Deixa eu te dar um abraço! inimigo_hello: Batu não quer lutar. be_attack: Não podemos conversar sobre isso? Batu não se intimida tão facilmente. be_attack_enemy: Você é realmente chato! Batu vai esmagar você!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Coisas &lt;color=red&gt;românticas&lt;/color&gt; me relaxam. Alguns &lt;color=red&gt;artigos artesanais&lt;/color&gt; de qualidade também me deixam feliz. olá: gostaria que esse gênio relaxasse e me deixasse conversar. recusar_recruit_0: Como você pode ver, essa coisa nas minhas costas é um gênio do mal. Pode ser perigoso para você. É por isso que... não posso ajudá-lo. recusar_recruit_1: Tenho liberdade, luxo, conforto. Se eu me juntar a você, todas essas coisas desaparecerão. recusar_recruit_2: Não. Não, não, não. Vá encontrar outra pessoa. recusar_recruit_3: Saia daqui! Não consigo controlar esse gênio! recruta_msg: Ok. Você mesmo causou isso. inimigo_hello: Peço que você tenha cuidado: esse gênio nas minhas costas é perigoso. be_attack: Eu te avisei sobre as consequências. Não posso assumir a responsabilidade. be_attack_enemy: Haha,</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:Eu gosto deles... Deixe-me pensar... &lt;color=red&gt;bugigangas&lt;/color&gt;, &lt;color=red&gt;brinquedos&lt;/color&gt;, &lt;color=red&gt;coisas adoráveis&lt;/color&gt;, sim, todas essas coisas me fazem feliz. Olá: Venho de uma terra distante ao leste, um lugar cheio de flores de pessegueiro. recusar_recruit_0:Hein? Você quer que eu me junte a você? Hum... deixe-me pensar sobre isso. recusar_recruit_1:Hm... Eu não costumo viajar com outras pessoas. recusar_recruit_2:Não, obrigado! Eu gosto de estar sozinho. recusar_recruit_3:Não é legal rejeitar você assim, mas devo dizer que você fez algumas coisas desagradáveis ​​e eu não gosto disso. recruta_msg: Bom! Se você tiver uma chance, deveríamos ir para minha cidade natal.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: &lt;color=red&gt;Histórico&lt;/color&gt;, &lt;color=red&gt;música&lt;/color&gt;. Se você encontrar algum &lt;color=red&gt;equipamento especial&lt;/color&gt;, deixe-me ver e ficarei grato. olá:O Criador constrói e destrói sem medo. recusar_recruit_0:Se você quiser as armas que criei, não precisa ser tão indireto. recusar_recruit_1:É verdade que sou uma boa peça. Mas não quero me tornar peça de outra pessoa. recusar_recruit_2:Perdi o apetite por ser usado como arma. recusar_recruit_3:Você me levaria ao mal. recruta_msg:Eu poderia ter ficado sozinho a vida toda, mas você... bem, espero que se lembre de mim.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Ah! Mulheres como eu não resistem a nada &lt;color=red&gt;romântico&lt;/color&gt;... Se você não consegue encontrar algo romântico, eu adoraria uma coleção de atlas ou outros livros de &lt;color=red&gt;geografia&lt;/color&gt; .color&gt; para que eu possa explorar lugares interessantes onde nunca estive antes. Olá: Ah! Eu posso ouvir seu batimento cardíaco. recusar_recruit_0:Uau! Você realmente é encantador. Deixe-me pensar sobre isso por um momento. recusar_recruit_1: Aham! Você está apaixonado por mim? Mas devo rejeitar sua oferta. recusar_recruit_2:Oh~ Não consigo me imaginar seguindo um grupo de crianças fedorentas vivendo ao ar livre. Parece horrível. recusar_recruit_3: Hahaha! Nem mesmo em seus sonhos! recruta_msg: Como eu poderia resistir? Você é adorável demais para dizer não.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Gosto de ouvir os &lt;color=red&gt;lamentos&lt;/color&gt; dos mortos aprisionados. Se você quiser me impressionar, procure por &lt;color=red&gt;equipamentos especiais&lt;/color&gt; que só são encontrados em lendas. Olá: A luz solar é forte, mas aprendi a apreciá-la. recusar_recruit_0: Você parece uma pessoa decente. Vou considerar isso. recusar_recruit_1: Se você tivesse vivido a vida que eu vivi, também teria dificuldade em confiar nos outros. recusar_recruit_2: Não vejo futuro para mim na sua empresa. Só posso confiar em mim mesmo. recusar_recruit_3: Se estivéssemos nas masmorras, você seria o primeiro a perder a vida. recruta_msg: Meus pesadelos são constantes. Espero encontrar alívio em sua companhia. inimigo_hello: Vou acabar com você assim que tiver chance, inseto. be_attack: Eu escapei do próprio inferno. Você não tem chance. be_attack_enemy: Agora vou te mostrar o verdadeiro significado do medo!</t>
+  </si>
+  <si>
+    <t>喜欢的礼物:...Não consigo pensar em nada que eu queira, mas se for um [[imp:toys]], posso dar para minha irmã, certo? Ela também adora várias [[imp:stories]]. olá:Você parece ter certas habilidades, vamos competir no torneio de artes marciais se tivermos chance. | Você já conheceu minha irmã mais nova? Ela é uma menina muito doce. | Se você ainda sente dor durante a batalha, isso é bom, significa que você ainda está longe de morrer em combate.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Adoro histórias, é tão fácil saber minhas preferências! Gosto muito de ouvir [[imp:stories]] e também de compartilhar as minhas! Além disso, gosto de todos os tipos de [[imp:craft]]. Olá: Quando vi seu rosto soube que você tem muitas histórias para compartilhar! | Um homem deve vivenciar uma grande aventura em sua vida, assim como eu! | Sempre digo às pessoas que venho do outro lado da Grande Montanha Nevada, mas elas sempre acham que estou exagerando! | Um machado pode derrubar árvores e também pode ser usado para derrubar pessoas! Embora eu não recomende a segunda opção. | Xingamento! Onde está meu chifre para beber? Oh, está na minha mão esse tempo todo! Hahaha! | Uma vez tropecei e o machado voou e acertou um gigante! Ha! Estou brincando, ele realmente deu um soco em um dragão gigante.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Minhas preferências? Como uma mulher bonita como eu, preciso de um pouco de mistério, então convido você a adivinhar ~ olá: Muitos acreditam que nós, membros do clã dos escorpiões, amamos naturalmente os escorpiões, mas na realidade eu os odeio. Você parece muito poderoso! Estou ansioso para ver como você reagirá às minhas poções. Como usar veneno pode ser considerado trapaça? Como uma mulher delicada como eu, naturalmente preciso usar alguns truques. Sou a melhor alquimista de venenos do deserto. Não há veneno que não possa neutralizar.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Não é um hábito saudável perguntar sobre os gostos de outras pessoas... olá: Não tenho habilidades mágicas e também não gosto delas. | Posso sentir sua grande presença, se eu conseguir te encarar vou melhorar minha técnica de soco. | O ouro falso e o ouro verdadeiro têm uma grande diferença de preço, mas se forem transformados em joias, não serão distinguíveis. | Sempre carrego meus punhos comigo, a preparação marcial é constante.</t>
+  </si>
+  <si>
+    <t>喜欢的礼物: Hmm... o que eu mais gosto são coisas que registram [[imp:history]], pois me ajudam a lembrar de muitas coisas. Olá: Já nos conhecemos? Sinto que há algo familiar em você. | Minha memória não é muito boa... Se algum dia eu te ofender, seria ótimo se você pudesse me perdoar. | Parece que uma vez tive um negócio importante com alguém, mas não consigo me lembrar... | Você diz que os seres estelares realmente existem? Se sim, por que me abandonaram? | Há uma pessoa importante para mim nas montanhas nevadas, mas não consigo lembrar sua aparência ou seu nome...</t>
+  </si>
+  <si>
+    <t>Husnu é o legítimo herdeiro do trono Nasir. Embora o ex-rei Nasir ainda governe a cidade de Jamal, ele nomeou Husnu como sultão interino. Husnu é um homem de paz, mas luta internamente, temendo perder tudo o que ama em meio a tensões e conflitos. Natureza:gentil=4,severo=6,honesto=7,astúcia=3,calma=8,raiva=2,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能霍驹</t>
+  </si>
+  <si>
+    <t>Desc:Ruha é o líder do Dhib. Os Dhib vivem nas remotas montanhas Zagros. Os Dhib são um povo corajoso e pronto para a batalha, e Ruha não é exceção. Ela adora o combate com espadas, embora possa ser envolvida por uma fúria desenfreada devido à loucura da batalha. Ruha odeia mágicos e desconfia de seus truques. Ruha, um guerreiro formidável apaixonado pela arte da espada, lidera bravamente o Dhib nas inóspitas Montanhas Zagros. Sua habilidade no combate com espadas é lendária e sua habilidade com a lâmina foi forjada em inúmeras batalhas e desafios. Ruha personifica o espírito intrépido e ousado do seu povo, sempre pronto para enfrentar qualquer adversário que ameace o seu território sagrado. Natureza: gentil = 6, severo = 4, honesto = 8, astúcia = 2, calma = 2, raiva = 8, forte = 7, fraco = 3 habilidades de luta:</t>
+  </si>
+  <si>
+    <t>Desc: Bahat é o líder do Akhal, um antigo clã guerreiro que costumava ser leal aos Nefrit do Antigo Império. Durante séculos, os Akhal serviram como defensores e protetores do império, comprometidos com seus deveres e tradições antigas. No entanto, quando a guerra estourou e o Antigo Império caiu no caos, os Akhal perderam a esperança de restaurar seu antigo esplendor. Em meio ao desânimo e à desilusão, os Akhals procuraram um novo líder capaz de guiá-los para um novo destino. Bahat emergiu como uma figura carismática e corajosa, com uma herança que o ligava diretamente ao antigo rei Nefrit. Seu pai, um leal conselheiro e confidente do rei, garantiu o noivado com a princesa Ilayda, uma jovem de grande beleza e sabedoria. Porém, A tragédia atingiu Bahat e Akhal quando a cidade de Jamal caiu nas mãos do inimigo. Durante o caos e a confusão, a Princesa Ilayda desapareceu misteriosamente, mergulhando Bahat em profunda tristeza e determinação. Desde então, dedicou sua vida à procura de Ilayda, a mulher que deveria ser sua noiva, mas que nunca conheceu pessoalmente. Natureza:gentil=5,severo=5,honesto=7,astúcia=3,calma=1,raiva=9,forte=8,fraco=2 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能苍骐</t>
+  </si>
+  <si>
+    <t>Desc:Ludo Khan lidera os Thur, uma antiga tribo que resistiu ao teste do tempo e das dificuldades em uma floresta pantanosa infestada de perigos. Conhecido como o mais velho entre os cinco líderes tribais, Ludo Khan personifica a sabedoria acumulada ao longo dos anos e é reverenciado pela sua experiência e conhecimento. Graças a Ludo Khan, os Thur se estabeleceram no coração da floresta, um lugar marcado pelo sofrimento e pela luta. A terra onde residem viu inúmeros conflitos e batalhas e foi banhada pelas chamas da guerra. Apesar de enfrentarem a adversidade e a pobreza, os Thur mantiveram o seu espírito indomável e tornaram-se uma das tribos mais resistentes e fortes da região. Ludo Khan, apesar da idade avançada, Ele continua sendo uma figura respeitada e reverenciada entre os Thur. Diz-se que sua antiga sabedoria é um farol orientador para seu povo, e sua estratégia meticulosa garantiu a sobrevivência e o crescimento da tribo. Por trás de sua fachada de velho quieto e que gosta de cochilar, esconde-se um líder astuto e visionário, cujo desejo de ver seu povo prosperar é inabalável. Os Thur encontram nele uma fonte de inspiração e confiança, sabendo que o seu líder estará sempre presente para proteger e garantir o seu bem-estar neste mundo hostil. Natureza:gentil=7,severo=3,honesto=4,astúcia=6,calma=7,raiva=3,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|心清如水 fight_dgskill :刺拳,1 AssSkill:统率技能汗卢达 e que a sua estratégia meticulosa garantiu a sobrevivência e o crescimento da tribo. Por trás de sua fachada de velho quieto e que gosta de cochilar, esconde-se um líder astuto e visionário, cujo desejo de ver seu povo prosperar é inabalável. Os Thur encontram nele uma fonte de inspiração e confiança, sabendo que o seu líder estará sempre presente para proteger e garantir o seu bem-estar neste mundo hostil. Natureza:gentil=7,severo=3,honesto=4,astúcia=6,calma=7,raiva=3,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|心清如水 fight_dgskill :刺拳,1 AssSkill:统率技能汗卢达 e que a sua estratégia meticulosa garantiu a sobrevivência e o crescimento da tribo. Por trás de sua fachada de velho quieto e que gosta de cochilar, esconde-se um líder astuto e visionário, cujo desejo de ver seu povo prosperar é inabalável. Os Thur encontram nele uma fonte de inspiração e confiança, sabendo que o seu líder estará sempre presente para proteger e garantir o seu bem-estar neste mundo hostil. Natureza:gentil=7,severo=3,honesto=4,astúcia=6,calma=7,raiva=3,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|心清如水 fight_dgskill :刺拳,1 AssSkill:统率技能汗卢达 sabendo que o seu líder estará sempre lá para proteger e garantir o seu bem-estar neste mundo hostil. Natureza:gentil=7,severo=3,honesto=4,astúcia=6,calma=7,raiva=3,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|心清如水 fight_dgskill :刺拳,1 AssSkill:统率技能汗卢达 sabendo que o seu líder estará sempre lá para proteger e garantir o seu bem-estar neste mundo hostil. Natureza:gentil=7,severo=3,honesto=4,astúcia=6,calma=7,raiva=3,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|心清如水 fight_dgskill :刺拳,1 AssSkill:统率技能汗卢达</t>
+  </si>
+  <si>
+    <t>Descrição: Rebiya é a líder dos Dakn, uma tribo clandestina e temida composta por assassinos habilidosos. No início, os Dakn eram uma pequena organização paralela, mas ficaram mais fortes durante a guerra. Sangue assassino corre em suas veias, e Rebiya foi treinada por seu povo desde cedo na arte de matar furtivamente. O irmão mais velho de Rebiya foi reconhecido como general pelo Velho Rei, concedendo aos Dakn algum status no conflito. Na Batalha da Cidade de Jamal, Rebiya juntou-se a Husnu em uma ousada ofensiva para conquistar Nefrit. No entanto, quando chegou a hora de dividir o território conquistado, a aliança entre Dakn e Nasir foi quebrada, mergulhando o irmão de Rebiya à beira da morte. Foi nesse momento de crise que Rebiya, com sua calma inabalável, astúcia cruel e sutileza letal, ela assumiu seu lugar como a única líder feminina das cinco tribos, conhecida por sua habilidade distinta no uso de venenos mortais. Rebiya se tornou a personificação dos Dakn, usando sua inteligência e estratégia para guiar sua tribo a uma posição de poder e respeito no mundo perigoso ao seu redor. Além de suas habilidades de assassinato incomparáveis, Rebiya é conhecida por seu domínio na arte dos venenos, capaz de manipular e utilizar substâncias mortais com precisão mortal. Como líder feminina em um mundo dominado por homens e cercado por assassinos mortais, Rebiya desafiou expectativas e provou ser uma força a ser reconhecida. Sua presença inspira medo e respeito, e sua determinação inabalável levou os Dakn a superar obstáculos e lutar com astúcia e ferocidade por sua causa. Apesar de sua aparência calma, Rebiya é conhecida por sua ferocidade e sua habilidade de usar sutileza e astúcia para alcançar seus objetivos. Natureza:gentil=3,severo=7,honesto=1,astúcia=9,calma=8,raiva=2,forte=4,fraco=6 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能阿曼莎</t>
+  </si>
+  <si>
+    <t>Desc: Gizeh, conhecido no passado como um dos comerciantes mais prósperos do deserto, esconde zelosamente sua verdadeira história. Embora todos na região saibam que ele desempenhou um papel crucial na captura do infame bandido Hashim, o seu passado e as suas motivações permanecem envoltos em mistério. Embora Gizeh trabalhe atualmente sob a bandeira de Akhal, a sua lealdade não é fácil de definir. Apesar do seu aparente compromisso com a tribo, Gizeh continua a ser um indivíduo independente que é guiado pelos seus próprios interesses e objectivos. Ninguém sabe ao certo quais são as suas verdadeiras intenções e quanto tempo permanecerá ao serviço do Akhal. Com astúcia inata e perspicácia empresarial incomparável, Gizeh possui um profundo conhecimento dos segredos e da dinâmica da região. Sua capacidade de manter seu passado em segredo e de negociar com maestria fizeram dele uma figura intrigante e respeitada no deserto. Rumores sobre sua riqueza e conexões ocultas circulam entre comerciantes e líderes tribais, alimentando ainda mais o mistério que o rodeia. Tipo:文学|故事 Natureza:tipo=3,severo=7,honesto=1,astúcia=9,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能格罗瓦兹</t>
+  </si>
+  <si>
+    <t>Desc:Yusuf começou como aprendiz do grande Mestre Espadachim. Ele já foi um adversário de Ruha, mas deixou seu ódio para trás e apoiou Ruha como o novo líder do Dhib quando a testemunhou resistir aos invasores estrangeiros. Impressionado com a bravura e determinação de Ruha, Yusuf reconheceu sua força e qualidades de liderança. Ele viu nela uma verdadeira guerreira que lutou não só por si mesma, mas pela libertação e proteção do seu povo. Testemunhando o espírito inquebrantável de Ruha face à adversidade, Yusuf deixou para trás os seus ressentimentos do passado e abraçou um novo caminho de unidade e propósito partilhado. À medida que Yusuf continuava seu treinamento sob a orientação do Mestre da Espada, ele não apenas aprimorou suas habilidades com a espada, mas também cultivou um profundo respeito pela visão e pelos valores de Ruha. Juntos, criaram um forte vínculo baseado na confiança e num compromisso partilhado com a prosperidade e a independência da tribo Dhib. Tipo:格斗 Natureza:tipo=5,severo=5,honesto=6,astúcia=4,calma=2,raiva=8,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能武</t>
+  </si>
+  <si>
+    <t>Desc:Em sua vida anterior, Behrouz trabalhou ao lado de Gizeh, um dos comerciantes mais ricos do deserto de Docana Ocidental. Ele foi nomeado nobre honorário de Thur quando vendeu informações detalhadas sobre uma invasão iminente da terra natal de Thur, os Penhascos Umbra, para seu líder, Ludo Khan. Behrouz, hábil na arte da espionagem e coleta de informações, foi um colaborador próximo de Gizé. Durante sua associação, ele se infiltrou nos círculos mais exclusivos e adquiriu conhecimentos valiosos sobre os planos e movimentos de diferentes facções no deserto. No entanto, um acontecimento importante mudou o curso de sua vida. Quando Behrouz descobriu os planos de invasão que ameaçavam os Thur e a sua terra sagrada, Ele tomou a ousada decisão de encerrar seu relacionamento com Gizé e compartilhar essa informação com Ludo Khan, o líder dos Thur. Sua bravura e lealdade à causa de Thur lhe renderam o reconhecimento e a distinção de se tornar um nobre honorário. Desse ponto em diante, Behrouz tornou-se um aliado valioso dos Thur, usando suas habilidades de inteligência e conhecimento estratégico para proteger os Thurians e defender sua terra natal de ameaças externas. A sua experiência anterior no mundo da riqueza e do comércio deu-lhe uma perspectiva única e uma rede de contactos que utiliza para beneficiar os qui. Tipo:神秘 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能安纳西尔 Sua bravura e lealdade à causa de Thur lhe renderam o reconhecimento e a distinção de se tornar um nobre honorário. Desse ponto em diante, Behrouz tornou-se um aliado valioso dos Thur, usando suas habilidades de inteligência e conhecimento estratégico para proteger os Thurians e defender sua terra natal de ameaças externas. A sua experiência anterior no mundo da riqueza e do comércio deu-lhe uma perspectiva única e uma rede de contactos que utiliza para beneficiar os qui. Tipo:神秘 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能安纳西尔 Sua bravura e lealdade à causa de Thur lhe renderam o reconhecimento e a distinção de se tornar um nobre honorário. Desse ponto em diante, Behrouz tornou-se um aliado valioso dos Thur, usando suas habilidades de inteligência e conhecimento estratégico para proteger os Thurians e defender sua terra natal de ameaças externas. A sua experiência anterior no mundo da riqueza e do comércio deu-lhe uma perspectiva única e uma rede de contactos que utiliza para beneficiar os qui. Tipo:神秘 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能安纳西尔 usando suas habilidades de inteligência e conhecimento estratégico para proteger os Thurians e defender sua casa de ameaças externas. A sua experiência anterior no mundo da riqueza e do comércio deu-lhe uma perspectiva única e uma rede de contactos que utiliza para beneficiar os qui. Tipo:神秘 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能安纳西尔 usando suas habilidades de inteligência e conhecimento estratégico para proteger os Thurians e defender sua casa de ameaças externas. A sua experiência anterior no mundo da riqueza e do comércio deu-lhe uma perspectiva única e uma rede de contactos que utiliza para beneficiar os qui. Tipo:神秘 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能安纳西尔</t>
+  </si>
+  <si>
+    <t>Desc:Zaerur é o primo mais velho de Husnu, líder dos Nasir. Ele acompanhou Husnu e seu exército até Redstone Keep para desempenhar o papel de conselheiro. Zaerur, com a sua experiência e sabedoria, tem sido um apoio crucial para Husnu na sua liderança. Como conselheiro de confiança, partilhou o seu conhecimento estratégico e visão para ajudar a tomar decisões importantes em benefício dos Nasirs. O vínculo familiar fortalece ainda mais a conexão e a compreensão mútua. Zaerur esteve presente durante a ascensão de Husnu à liderança dos Nasir e testemunhou sua bravura e habilidades em batalha. Juntos, eles enfrentaram desafios e criaram um vínculo inseparável enquanto lutam para proteger e fortalecer sua tribo. Na Redstone Keep, Zaerur desempenha um papel fundamental como consultor estratégico, trazendo sua perspectiva e experiência para ajudar Husnu a tomar decisões informadas. A sua presença calmante e a sua capacidade de ver além do óbvio foram inestimáveis ​​para o sucesso e a sobrevivência dos Nasirs. Tipo:工艺 Natureza:tipo=4,severo=6,honesto=6,astúcia=4,calma=8,raiva=2,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能霍桑</t>
+  </si>
+  <si>
+    <t>Desc:Esfir, que já foi um membro importante da Gangue Wildfire e considerada uma irmã querida do Wildfire. Quando Wildfire foi morto e a organização se desintegrou, Esfir se cansou das intermináveis ​​lutas internas entre Rabia e Ishtar. Ele decidiu ingressar na Thur com alguns de seus subordinados e sua experiência em logística. Agora, ela não era mais ingênua e tentava secretamente encontrar a pessoa responsável pelo extermínio da Gangue do Fogo Selvagem. Esfir, com sua experiência e conhecimento estratégico, tornou-se um ativo valioso para o Thur. Suas habilidades de liderança e logística foram fundamentais para a organização e eficiência das operações de Thur. No entanto, dentro dele, ardia uma sede de vingança e justiça pela queda da Gangue Wildfire. Enquanto trabalhava nas fileiras do Thur, Esfir usou sua posição e recursos para investigar secretamente e descobrir a verdade por trás do assassinato de Wildfire e da destruição de sua gangue. Ela era uma caçadora furtiva, sempre um passo à frente de seus inimigos, em busca de pistas e trilhas que a levassem ao culpado final. Embora os Thurs fossem sua nova família e sua prioridade fosse servir seu líder, Ludo Khan, Esfir não conseguia esquecer seu passado e sua lealdade à Gangue Wildfire. Encontrar o responsável e fazê-lo pagar por seus atos tornou-se uma obsessão que alimentou sua determinação e motivação. Tipo:装饰|忧伤 Natureza:tipo=7,severo=3,honesto=8,astúcia=2,calma=4,raiva=6,forte=4,fraco=6 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能叶斯菲 em busca de pistas e vestígios que a levassem ao responsável final. Embora os Thurs fossem sua nova família e sua prioridade fosse servir seu líder, Ludo Khan, Esfir não conseguia esquecer seu passado e sua lealdade à Gangue Wildfire. Encontrar o responsável e fazê-lo pagar por seus atos tornou-se uma obsessão que alimentou sua determinação e motivação. Tipo:装饰|忧伤 Natureza:tipo=7,severo=3,honesto=8,astúcia=2,calma=4,raiva=6,forte=4,fraco=6 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能叶斯菲 em busca de pistas e vestígios que a levassem ao responsável final. Embora os Thurs fossem sua nova família e sua prioridade fosse servir seu líder, Ludo Khan, Esfir não conseguia esquecer seu passado e sua lealdade à Gangue Wildfire. Encontrar o responsável e fazê-lo pagar por seus atos tornou-se uma obsessão que alimentou sua determinação e motivação. Tipo:装饰|忧伤 Natureza:tipo=7,severo=3,honesto=8,astúcia=2,calma=4,raiva=6,forte=4,fraco=6 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能叶斯菲</t>
+  </si>
+  <si>
+    <t>Desc:Latif vive uma vida normal. Ele era um residente comum da cidade de Jamal que foi convocado para o exército por causa da guerra. Ele começou como soldado de infantaria e subiu lentamente. Agora ele se tornou um general incomparável, servindo ao grande líder das Montanhas Zagros. Latif gosta de atividades de &lt;color=red&gt;combate&lt;/color&gt; e &lt;color=red&gt;artesanato&lt;/color&gt;. Ele gosta de participar de lutas e desafios físicos, mostrando sua habilidade e habilidade marcial. Além disso, você tem interesse em habilidades artesanais e aprecia a beleza e o valor dos objetos feitos à mão. Apesar de sua ascensão no exército e de sua posição como general líder, Latif nunca esquece suas raízes e a vida comum que levava antes da guerra. Ele mantém sua humildade e se esforça para proteger e servir seu povo nas Montanhas Zagros. A sua experiência como soldado raso deu-lhe uma profunda compreensão dos desafios e dificuldades enfrentados pelos seus colegas soldados, e ele esforça-se para ser um líder compassivo e corajoso. Tipo:格斗|工艺 Natureza:tipo=6,severo=4,honesto=5,astúcia=5,calma=5,raiva=5,forte=9,fraco=1 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:重拳,1 AssSkill:统率技能洛尔</t>
+  </si>
+  <si>
+    <t>Desc:Uma mulher de linhagem nobre pertencente à tribo Dhib, reconhecida não só por sua posição de nobreza, mas também por ser a caçadora mais talentosa de seu povo. Além de suas proezas de caça, ele tem um profundo amor pela arte da pintura. Desde cedo demonstrou afinidade natural pela arte da caça, aprimorando suas habilidades com arco e flecha, rastreamento e conhecimento da fauna local. Sua habilidade e precisão na caça lhe renderam o respeito e a admiração de sua tribo, tornando-a uma figura icônica de coragem e sabedoria. Como nobre do Dhib, ela carrega consigo a responsabilidade de proteger e manter o equilíbrio em sua terra ancestral. Seu profundo conhecimento da natureza e sua conexão espiritual com criaturas selvagens permitem-lhe desempenhar um papel vital na sobrevivência e prosperidade de sua tribo. Além de sua habilidade como caçadora, ela também é uma líder respeitada na comunidade Dhib. Tipo:绘画 Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=6,raiva=4,forte=6,fraco=4 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill:刺拳,1 AssSkill:统率技能热丽莎</t>
+  </si>
+  <si>
+    <t>Desc:Janub, uma guerreira feroz e habilidosa, começou sua jornada como mercenária, vendendo sua espada pelo lance mais alto. Com sua excepcional capacidade de combate e mente estratégica, ela rapidamente ganhou a reputação de ser uma das lutadoras mais formidáveis ​​da região. Durante seu emprego na tribo Nasir, ele provou seu valor ao derrotar sozinho um grupo de cavalaria Akhal, demonstrando sua habilidade e bravura incomparáveis. Impressionados com seu feito notável, os Nasir reconheceram as habilidades excepcionais de Janub e concederam-lhe a adesão formal à sua tribo. Ele se tornou uma figura respeitada e admirada, admirado por suas proezas de combate e tenacidade indomável. Janub tornou-se um aliado confiável e uma força a ser reconhecida no campo de batalha. Seu passado como mercenária fala de sua resiliência e adaptabilidade, provando que ela pode enfrentar qualquer desafio com determinação e habilidade. Tipo:神秘 Natureza:tipo=7,severo=3,honesto=6,astúcia=4,calma=6,raiva=4,forte=8,fraco=2 habilidades de luta:升龙拳|吼叫|饮酒|飞腿 luta_dgskill:刺拳,1 AssSkill:统率技能雅南</t>
+  </si>
+  <si>
+    <t>Como:工艺|特殊装备 Ladrão:100 WildMonsterKiller:1 Desc:Mhan Hassan é natural de Akhal, mas sua família tem um relacionamento tumultuado com o Sultão de Akhal. Após um conflito público com o Sultão de Akhal, ele foi banido da tribo. Isso lhe deu a oportunidade de lutar ao lado de Bahat e se juntar aos Nasir. O exílio de Mhan Hassan do Akhal não só marcou uma ruptura na sua relação com a sua tribo de origem, mas também despertou nele um sentimento de determinação e sede de vingança. Com sua experiência e habilidades de combate, ele se tornou um valioso aliado de Bahat e um forte defensor da causa Nasir. Na sua união com os Nasirs, Mhan Hassan encontrou uma nova família e uma oportunidade de redenção, prometendo usar a sua habilidade e conhecimento para confrontar aqueles que antes o rejeitaram. Sua lealdade a Bahat e seu desejo por justiça o levam a lutar incansavelmente em busca da vingança que tanto almeja. Voz:NpcVoice.huyanmu BattleVoice:BattleVoice.huyanmu Natureza:tipo=5,severo=5,honesto=7,astúcia=3,calma=1,raiva=9,forte=9,fraco=1 habilidades de luta:升龙拳|吼叫|饮酒|飞腿 fight_dgskill:刺拳,1 AssSkill:统率技能呼延牧</t>
+  </si>
+  <si>
+    <t>Desc:Yakub desempenha o papel de um dos generais de Bahat, o Sultão de Akhal. A cicatriz em seu rosto é tão famosa quanto sua lendária esgrima. Com um olhar imponente e uma presença magnética, Yakub personifica a ferocidade e a coragem de um verdadeiro líder guerreiro. A cicatriz que adorna seu rosto é um testemunho vivo das muitas batalhas que travou e dos desafios que superou. É um símbolo de sua dedicação inabalável e determinação incansável na proteção e defesa da tribo Akhal. Sua habilidade no combate com espadas é lendária e sua mera presença no campo de batalha causa medo nos corações de seus inimigos. WildMonsterKiller:1 Como:格斗 Natureza:tipo=4,severo=6,honesto=5,astúcia=5,calma=3,raiva=7,forte=7,fraco=3 habilidades de luta:升龙拳|吼叫|饮酒|飞Em fight_dgskill:刺拳,1 AssSkill:</t>
+  </si>
+  <si>
+    <t>Desc:Úrsula, durante os tempos do Antigo Império, era uma acólita na cidade de Cotta. Depois que a cidade de Cotta foi anexada pelos Dakn, Ursula aceitou de bom grado as tradições de criação de escorpiões dos Dakn. Ele presidiu os sacrifícios diante das chamas durante o dia, mas realizou experimentos secretos à noite. Depois de inúmeros fracassos, ela finalmente conseguiu criar uma criatura que a satisfez: um escorpião que cresce próximo à chama sagrada e não tem medo de altas temperaturas. Úrsula, durante os tempos do Antigo Império, levou uma vida humilde como acólita na cidade de Cotta. No entanto, quando os Dakn anexaram a cidade, Ursula abraçou suas tradições de criar escorpiões de braços abertos. Durante o dia, ele presidia devotamente os sacrifícios sagrados diante das chamas, mas foi na calada da noite que suas verdadeiras ambições vieram à tona. Movida por uma busca incansável por conhecimento e experimentação, Ursula mergulhou nos segredos da criação de escorpiões. Ele passou inúmeras noites na solidão, trabalhando incansavelmente para criar uma criatura que superasse todas as expectativas. WildMonsterKiller:1 Como:神秘 Natureza:tipo=6,severo=4,honesto=4,astúcia=6,calma=6,raiva=4,forte=7,fraco=3 habilidades de luta:升龙拳|吼叫|饮酒|飞腿 fight_dgskill:刺拳,1 AssSkill:统率技能厄苏拉</t>
+  </si>
+  <si>
+    <t>Desc:Khaza, também apelidado de "Hook Grip", é reconhecido como um dos combatentes mais habilidosos recrutados por Rebiya, a Rainha dos Dakn. Desde jovem, Khaza dedicou sua vida ao aperfeiçoamento de suas habilidades marciais, dominando a técnica Hook Grasp. Um membro leal das forças de Rebiya, Khaza é conhecido por sua habilidade no combate corpo a corpo e seu domínio do Hook Grasp, tornando-o um adversário temível no campo de batalha. Com movimentos rápidos e precisos, ele consegue imobilizar e controlar seus oponentes, deixando-os à mercê de seus poderosos ataques. A lealdade de Khaza a Rebiya e sua dedicação incansável à causa Dakn fazem dele um trunfo indispensável na busca por poder e domínio. Sua presença imponente e sua capacidade de vencer no combate fazem dele uma figura respeitada e temida nos círculos de luta. Tipo:格斗 Natureza:tipo=2,severo=8,honesto=3,astúcia=7,calma=2,raiva=8,forte=5,fraco=5 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 fight_dgskill :刺拳,1 AssSkill:统率技能卡拉</t>
+  </si>
+  <si>
+    <t>Desc:Tua é um habilidoso mestre espadachim que recebeu seu treinamento do lendário Manal, um renomado ferreiro do antigo império. Dotado de talento excepcional e dedicação incansável, Tua dominou a arte de forjar espadas de qualidade insuperável. Sua habilidade em forjar era tão conhecida que o antigo império o empregou como ferreiro primário, confiando-lhe a criação de armas de grande valor e poder. Durante seu tempo no antigo império, Tua deixou sua marca na história ao forjar duas das três espadas icônicas usadas por Ruha, um corajoso líder militar. Essas espadas eram obras-primas da metalurgia, imbuídas de uma qualidade e magia especiais que as tornavam armas letais nas mãos de seu portador. Após a queda do império Tua encontrou um novo propósito e emprego nas fileiras do exército Dhib onde ele agora atua como comandante. Sua habilidade como ferreiro e sua experiência no campo de batalha fazem dele um recurso valioso para o Dhib, e seu legado como criador de armas lendárias continua vivo na história. WildMonsterKiller:1 Como:工艺 Natureza:tipo=5,severo=5,honesto=8,astúcia=2,calma=5,raiva=5,forte=9,fraco=1 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能图哈</t>
+  </si>
+  <si>
+    <t>Desc:Shirim é uma herbalista enigmática que vive nos Penhascos Umbra, conhecida por seu vasto conhecimento de plantas medicinais e sua capacidade de curar doenças. No entanto, existem rumores circulando sobre sua conexão sombria com as artes mágicas proibidas. Diz-se que Shirim explorou o lado mais sombrio da magia, experimentando feitiços e poções que transcendem os limites das convenções. À medida que a loucura toma conta de Nagukka e Mireton, muitos atribuem parte da responsabilidade a Shirim e sua suposta propensão à magia negra. Há rumores de que suas práticas ocultas desencadearam uma força obscura que corrompe mentes e altera a realidade nessas terras. Temido e sussurrado nos cantos mais sombrios, Shirim se torna um enigma envolto em mistério, cujos poderes e verdadeiras intenções só podem ser especulados. WildMonsterKiller:1 Como:魔力 Natureza:tipo=2,severo=8,honesto=3,astúcia=7,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能希可弥</t>
+  </si>
+  <si>
+    <t>Desc:Fayiz, uma guerreira corajosa, carrega consigo o legado da antiga tribo Oryx, cujos membros foram dispersos e sua cultura esquecida. Quando era uma menina vendida ao clã Dhib, foram sua excepcional determinação e habilidade que chamaram a atenção de Ruha, líder do Dhib. Reconhecendo seu potencial, Ruha a colocou sob sua proteção e a guiou no caminho da guerra. Com o passar dos anos, Fayiz provou ser um aliado leal e um combatente formidável. Sua habilidade no combate corpo a corpo e astúcia estratégica a levaram a se tornar o braço direito de Ruha. Juntos, eles criaram um vínculo forte e compartilharam inúmeras batalhas, defendendo o Dhib e enfrentando seus inimigos com determinação inabalável. Fayiz tornou-se um símbolo da resistência e do orgulho da sua tribo ancestral, lutando incansavelmente pelo seu povo e pelo legado que carrega no coração. WildMonsterKiller:1 Como:绘画 Natureza:tipo=5,severo=5,honesto=7,astúcia=3,calma=7,raiva=3,forte=10,fraco=0 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能云英</t>
+  </si>
+  <si>
+    <t>Desc:A família de Sharida é uma das famílias nobres mais antigas de Dakn, conhecedora da tradição de Dakn. Ela cresceu na tenda do líder Dakn ao lado de Hassan. Hassan juntou-se aos Nasir para atacar a cidade de Jamal. O conselho de Sharida foi indispensável. No entanto, quando Hassan adoeceu, sua irmã mais cruel abandonou a família de Sharida e tornou-se a única nobre. Sharida manteve isso em seu coração. Só ela sabe como responderá à traição de Rebiya no futuro. Apesar da traição e do frio desprezo da irmã de Hassan, Sharida permaneceu firme em sua lealdade à amiga. Ele manteve as memórias de sua educação compartilhada e do vínculo que formaram na tenda do líder Dakn. No fundo dela, um fogo ardia em Sharida, alimentando sua determinação em buscar justiça e restaurar a honra de sua família. Ele sabia que a traição de Rebiya não ficaria sem resposta e ele silenciosamente jurou recuperar o que era deles por direito. A cada dia que passa, Sharida aprimorou suas habilidades tanto na arte da diplomacia quanto nos costumes do guerreiro, preparando-se para o dia em que enfrentaria seu inimigo e remodelaria o destino de sua família e do povo Dakn. WildMonsterKiller:1 Como:音乐|历史|绘画 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=9,raiva=1,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能沙里娅 tanto na arte da diplomacia quanto nos costumes do guerreiro, preparando-se para o dia em que enfrentaria seu inimigo e remodelaria o destino de sua família e do povo Dakn. WildMonsterKiller:1 Como:音乐|历史|绘画 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=9,raiva=1,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能沙里娅 tanto na arte da diplomacia quanto nos costumes do guerreiro, preparando-se para o dia em que enfrentaria seu inimigo e remodelaria o destino de sua família e do povo Dakn. WildMonsterKiller:1 Como:音乐|历史|绘画 Natureza:tipo=5,severo=5,honesto=2,astúcia=8,calma=9,raiva=1,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能沙里娅</t>
+  </si>
+  <si>
+    <t>Desc:Fire Eye, desde cedo demonstrou uma paixão inata pelo tiro com arco. Embora suas habilidades nunca tenham atingido a perfeição, sua destreza única foi revelada durante o cerco de uma cidade. Num momento crucial, ao lançar uma flecha em direção ao seu alvo, um golpe de sorte fez com que ela pegasse fogo, causando uma reação explosiva ao entrar em contato com os tanques de combustível inimigos. O surto massivo resultou em uma vitória esmagadora para os Nasirs. Impressionado com sua bravura e a eficácia inesperada de sua técnica, Fire Eye foi promovido a Comandante, desafiando a noção convencional de que a precisão é o único critério para arqueiros. Daquele momento em diante, Fire Eye se tornou uma lenda viva entre as fileiras dos Nasir. Sua habilidade única de causar estragos nas defesas inimigas com suas flechas de fogo lhe valeu o apelido de “Olho de Fogo”. Inspirando medo e admiração, Fire Eye demonstrou que na guerra, a imprevisibilidade e a ousadia podem ser tão poderosas quanto a precisão. Seu legado tornou-se uma lição para futuros arqueiros, lembrando-lhes que coragem e determinação podem fazer a diferença no campo de batalha, mesmo quando a mira não é perfeita. WildMonsterKiller:1 Como:特殊装备 Natureza:tipo=4,severo=6,honesto=4,astúcia=6,calma=8,raiva=2,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能火眼 A imprevisibilidade e a ousadia podem ser tão poderosas quanto a precisão. Seu legado tornou-se uma lição para futuros arqueiros, lembrando-lhes que coragem e determinação podem fazer a diferença no campo de batalha, mesmo quando a mira não é perfeita. WildMonsterKiller:1 Como:特殊装备 Natureza:tipo=4,severo=6,honesto=4,astúcia=6,calma=8,raiva=2,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能火眼 A imprevisibilidade e a ousadia podem ser tão poderosas quanto a precisão. Seu legado tornou-se uma lição para futuros arqueiros, lembrando-lhes que coragem e determinação podem fazer a diferença no campo de batalha, mesmo quando a mira não é perfeita. WildMonsterKiller:1 Como:特殊装备 Natureza:tipo=4,severo=6,honesto=4,astúcia=6,calma=8,raiva=2,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能火眼</t>
+  </si>
+  <si>
+    <t>Desc:Vindo de uma longa linhagem de treinadores de camelos habilidosos, nosso protagonista aprimorou sua experiência no cuidado e no treinamento dessas majestosas criaturas do deserto. A reputação de sua família como proeminentes comerciantes de camelos lhes rendeu respeito e admiração entre as comunidades que viviam no deserto. No entanto, o destino reservou um caminho diferente quando a tribo Akhal emergiu como uma força dominante no vasto deserto ocidental de Docana. Impressionado com suas habilidades excepcionais e profundo conhecimento no manejo de camelos, Akhal reconheceu o potencial do protagonista e concedeu-lhe status de nobre dentro de suas fileiras. Agora elevado à posição de nobre, Nosso protagonista assume o importante papel de liderar os ilustres cavaleiros de camelo do Akhal. Seu comando estratégico e profundo conhecimento do terreno desértico fazem deles um recurso indispensável nas expedições da tribo, enquanto atravessam as areias implacáveis ​​ao lado de seus companheiros camelos, garantindo a prosperidade da tribo e estabelecendo sua reputação como formidáveis ​​nômades do deserto. WildMonsterKiller:1 Como:地理 Natureza:tipo=8,severo=2,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能维库那 garantindo a prosperidade da tribo e estabelecendo sua reputação como formidáveis ​​nômades do deserto. WildMonsterKiller:1 Como:地理 Natureza:tipo=8,severo=2,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能维库那 garantindo a prosperidade da tribo e estabelecendo sua reputação como formidáveis ​​nômades do deserto. WildMonsterKiller:1 Como:地理 Natureza:tipo=8,severo=2,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:蓄力冲刺|冲刺重拳|升龙拳|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能维库那</t>
+  </si>
+  <si>
+    <t>Desc:Dhaji, um político astuto, aspirava a se tornar Ministro de Jamal City, mas viu suas ambições serem interrompidas após a queda do Império Nefrite. Após o saque de Jamal City, ele retornou para sua casa ancestral nos Penhascos Umbra. Ali, sua capacidade de persuasão e sua língua eloqüente chamaram a atenção de Ludo Khan, figura poderosa da região, que rapidamente o contratou, reconhecendo sua astúcia política. Seu caminho é marcado pela redenção e pelo desejo de sucesso, enquanto navega por um cenário perigoso cheio de intrigas e lutas pelo poder. A cada dia que passa, Dhaji se torna uma figura influente, tecendo intrigas e estratégias para voltar ao topo do poder político. WildMonsterKiller:1 Como:乐器 Natureza:tipo=4,severo=6,honesto=2,astúcia=8,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:</t>
+  </si>
+  <si>
+    <t>Desc:Petra, a filha ilegítima do governador que governou Redstone Keep durante o Império Nefrit, teve sua vida revirada quando os Nasir tomaram a cidade. Apesar das circunstâncias adversas, sua vida foi poupada e ele ficou sob a proteção de Husnu. À primeira vista, sua lealdade parece inabalável, mas poucos sabem realmente quais pensamentos passam por sua mente. Como filha ilegítima, Petra aprendeu a navegar pelo mundo com astúcia e discrição. Suas experiências passadas e sua posição atual sob a tutela de Husnu criaram uma personalidade enigmática e secreta. Embora ele demonstre aparente lealdade, suas verdadeiras intenções e motivações permanecem ocultas da maioria. Petra é uma figura enigmática que guarda seus segredos e só o tempo revelará quais planos e pensamentos ela realmente guarda dentro de si. WildMonsterKiller:1 Gosto:玩具 Natureza:</t>
+  </si>
+  <si>
+    <t>Desc:Blackmane é o querido irmão de Bahat e General das forças Akhal. Como líder conservador, Blackmane insiste em manter inalteradas as tradições antigas. Sua devoção à preservação de costumes antigos é inquestionável e ele acredita que eles são fundamentais para a identidade e a força do Akhal. Como General, Blackmane segue estritamente as formas de batalha tradicionais e promove a disciplina e a honra entre seus soldados. A sua abordagem intransigente às práticas antigas reflecte a sua crença na sua eficácia e na preservação da herança Akhal. Embora alguns possam questionar a sua resistência à mudança, Blackmane permanece firme na sua convicção de que as tradições inalteradas são a base para o sucesso e a grandeza de Akhal. WildMonsterKiller:1 Como:高贵 Natureza:kind=8,</t>
+  </si>
+  <si>
+    <t>Tipo:珠宝|高贵 Desc:Kanaya nasceu em uma família de comerciantes. Desde cedo ele sonhava em alcançar uma riqueza deslumbrante e viver na próspera cidade de Jamal. No entanto, a guerra trouxe tempos difíceis para sua família. Apesar das adversidades, Kanaya não desistiu de seus sonhos de prosperidade e trabalha incansavelmente no movimentado bazar. Com determinação inabalável, Kanaya mergulha na agitação do mercado, buscando oportunidades para melhorar sua situação financeira. Suas habilidades de negociação e instintos empresariais aguçados permitem-lhe navegar pelos desafios e obstáculos que surgem em seu caminho. Embora o caminho para a riqueza possa ser árduo, Kanaya se apega à esperança e continua a trabalhar duro para realizar seus sonhos de sucesso e fortuna no fascinante mundo do bazar. Ladrão:100 Natureza:gentil=7,severo=3,honesto=2,astúcia=8,calma=6,raiva=4,forte=7,fraco=3 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能康牙</t>
+  </si>
+  <si>
+    <t>Tipo:珠宝|魔力|装饰 Desc:Miaya foi abandonada pelos pais durante a guerra. Sua infância no Vale Twinluna foi difícil e desafiadora. À medida que se tornava mulher, ela sentia inveja das meninas que tinham dinheiro para se vestir elegantemente. Carente e ávida por ganhar dinheiro, ela estava disposta a fazer trabalhos perigosos que os homens tinham medo de fazer, a ponto de colocar sua vida em perigo... já que sua outra saída era vender seu corpo. Foi então que um espíritomancer, apreciando sua bravura e determinação, aceitou-a como aprendiz. Sob a tutela do espíritomante, Miaya começou a explorar o mundo da magia e dos espíritos. Ela aprendeu a canalizar suas habilidades naturais e controlar os poderes que estavam dentro dela. A cada desafio superado, sua confiança crescia e ela se tornava uma especialista em sua arte. Agora, Miaya usa sua habilidade mágica e bravura para realizar tarefas arriscadas e desafiadoras. Seu caminho não convencional e sua capacidade de assumir trabalhos perigosos lhe renderam respeito nos círculos de espíritos. Embora seu passado tenha sido difícil, ele encontrou um novo propósito e uma nova família na comunidade dos espíritos. Natureza:tipo=3,severo=7,honesto=2,astúcia=8,calma=6,raiva=4,forte=8,fraco=2 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能百花</t>
+  </si>
+  <si>
+    <t>Como:文学|装饰 Desc:Yasmin, a irmã mais velha da família Giddah, sofreu humilhação quando foi derrotada por sua irmã mais nova, Bellen, em um torneio da família Giddah. Como resultado, ela foi forçada a entregar a espada da família a Bellen, tornando este último o líder da família Giddah. Secretamente, Yasmin conspirou com sua irmã Mumtali para incriminar Bellen e bani-la da família Giddah. Agora, Yasmin detém a liderança da Casa Giddah. A traição e o ressentimento no coração de Yasmin a levaram a tomar medidas drásticas para ganhar o poder que ela acreditava merecer. Aproveitando sua posição como líder da família Giddah, ele consolidou sua autoridade e estabeleceu seu domínio sobre os demais membros da casa. Porém, O peso da sua traição e a sombra do seu passado sombrio podem assombrá-la e ameaçar a sua liderança. Yasmin enfrenta a difícil tarefa de equilibrar seu desejo de poder e preservar a unidade e a honra da família Giddah. Natureza:gentil=2,severo=8,honesto=3,astúcia=7,calma=3,raiva=7,forte=7,fraco=3 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能公孙妍</t>
+  </si>
+  <si>
+    <t>Como:神秘|装饰 Desc:A segunda filha da família Giddah, Mumtali, conspirou com sua irmã mais velha, Yasmin, para incriminar sua irmã mais nova, a princesa Bellen. Com sua pegadinha concluída, Mumtali ascendeu à posição de segundo em comando da Casa Giddah. Contudo, a sua ambição não seria satisfeita simplesmente ocupando essa posição. Assim, ela começou a traçar um novo plano... Movida pela sede de poder e ansiosa por obter um papel ainda mais proeminente dentro da família, Mumtali arma novas intrigas. Sua mente maquiavélica e astúcia se combinam para levar a cabo sua nova trama, buscando alcançar o domínio absoluto sobre a Casa Giddah. Com sua determinação implacável e capacidade de manipular as situações a seu favor, Mumtali se torna uma figura intrigante e perigosa no ambiente familiar. Porém, O sucesso das suas maquinações e a aceitação dos seus planos estão longe de estar garantidos. As consequências das suas ações e a resposta daqueles que descobrem as suas verdadeiras intenções podem comprometer a sua posição e desencadear uma série de acontecimentos imprevisíveis. Mumtali embarca em um caminho cheio de incertezas e riscos, onde sua astúcia e desejo de poder serão testados a cada passo que ela der. Natureza:gentil=2,severo=8,honesto=1,astúcia=9,calma=7,raiva=3,forte=3,fraco=7 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能公孙弥 Mumtali embarca em um caminho cheio de incertezas e riscos, onde sua astúcia e desejo de poder serão testados a cada passo que ela der. Natureza:gentil=2,severo=8,honesto=1,astúcia=9,calma=7,raiva=3,forte=3,fraco=7 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能公孙弥 Mumtali embarca em um caminho cheio de incertezas e riscos, onde sua astúcia e desejo de poder serão testados a cada passo que ela der. Natureza:gentil=2,severo=8,honesto=1,astúcia=9,calma=7,raiva=3,forte=3,fraco=7 habilidades de luta:踩脚趾|丢酒瓶|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能公孙弥</t>
+  </si>
+  <si>
+    <t>Como:历史|格斗 WildMonsterKiller:1 Desc:Um órfão que aprendeu a lutar para sobreviver em tempos de guerra. Em sua juventude, ele conheceu o bardo Misod e ficou comovido com seu sonho de criar um mundo pacífico. Inspirado por esta visão, ele decidiu lutar pelo futuro que ele e Misod sonhavam. À medida que aprimorava suas habilidades de combate, esse órfão canalizou sua determinação e bravura para a causa da paz. Reconhecendo que a violência e o conflito apenas perpetuavam o sofrimento, juntou-se a Misod na busca por um mundo melhor. Guiado por um sonho partilhado de um futuro pacífico, este lutador órfão torna-se um incansável defensor da justiça e da harmonia. Em cada batalha, busque não apenas a vitória, mas também as sementes de uma mudança duradoura. Natureza: gentil = 6, severo = 4, honesto = 7, astúcia = 3, calmo = 2, raiva = 8, forte = 9,</t>
+  </si>
+  <si>
+    <t>Como:历史|故事 WildMonsterKiller:1 Desc:O bardo Misod vem da cabeceira do rio. Ele é um jovem nobre de posição inferior. Desfrute de poesia e literatura épica. No entanto, ele não queria participar de conflitos familiares, então decidiu seguir sua paixão por viagens e partiu sozinho para o leste. Em sua jornada, ele conheceu muitas pessoas que testemunharam a crueldade da guerra. Misod tomou a decisão de escrever suas histórias. Movido por seu profundo senso de empatia e justiça, Misod tornou-se um colecionador de histórias, um contador de testemunhos daqueles que sofreram os horrores da guerra. Ao viajar de um lugar para outro, ele ouviu as histórias das pessoas afetadas e as imortalizou na forma de escritos e canções. A sua dedicação em dar voz àqueles que foram silenciados pelo conflito levou-o a ser conhecido como um defensor da memória e da consciência colectiva. Através das suas obras, Misod não procura apenas documentar a realidade da guerra, mas também transmitir uma mensagem de esperança e compreensão. Natureza:gentil=8,severo=2,honesto=6,astúcia=4,calma=8,raiva=2,forte=6,fraco=4 habilidades de luta:冲刺膝盖顶|丢酒瓶|飞腿|心清如水 fight_dgskill :刺拳,1 AssHabilidade:统率技能米索德</t>
+  </si>
+  <si>
+    <t>Como:忧伤|浪漫|女神 Desc:Amira é filha de um dos comerciantes mais ricos do Bazar Dourado, que já foi nobre entre os Nefrites. Quando Jamal City caiu e o antigo império desapareceu, seus pais pegaram seu tesouro e fugiram para o Vale Twinluna. Como nobres do antigo império, seus pais eram pessoas trabalhadoras e honestas. A mãe de Amira Zahra era praticamente filha do ex-rei Nefrit. Sua sabedoria e ética de trabalho trouxeram sucesso para a família, mas ela faleceu ao dar à luz Amira. Após sua morte, o pai de Amira entrou em depressão, o que afetou a educação de Amira. A dor da perda e a tristeza que envolveu sua família deixaram uma marca profunda em Amira desde tenra idade. Criada num ambiente de melancolia, aprendeu a ser forte e resiliente, mas ele também desenvolveu o desejo de encontrar seu próprio propósito e superar as sombras do passado. À medida que cresce, Amira enfrenta o desafio de equilibrar a sua nobre herança e as expectativas que a acompanham com o seu desejo de traçar o seu próprio caminho. Com um misto de determinação e curiosidade, Amira embarca numa busca pessoal pela autodescoberta e melhoria. Ele deseja encontrar um senso de identidade e encontrar seu lugar em um mundo em mudança. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|冲刺膝盖顶|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能西河娜娅 Amira embarca em uma busca pessoal por autodescoberta e aprimoramento. Ele deseja encontrar um senso de identidade e encontrar seu lugar em um mundo em mudança. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|冲刺膝盖顶|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能西河娜娅 Amira embarca em uma busca pessoal por autodescoberta e aprimoramento. Ele deseja encontrar um senso de identidade e encontrar seu lugar em um mundo em mudança. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|冲刺膝盖顶|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能西河娜娅</t>
+  </si>
+  <si>
+    <t>Como:特殊装备|高贵 WildMonsterKiller:1 Desc:O fundador da Casa Giddah foi um general da primeira dinastia do Antigo Império. Ele se aposentou e se tornou sultão. Durante a Batalha do Sol Negro, a Casa Giddah defendeu suas terras usando o conhecimento da espada transmitido por seus ancestrais. O pai de Bellen faleceu há três anos. Segundo a tradição da Casa, as crianças da mesma geração tinham que lutar em um torneio para se tornarem o líder da Casa. Somente o vencedor poderia herdar a liderança da Casa Giddah e a valiosa espada da família. Bellen venceu o torneio, mas suas duas irmãs mais velhas conspiraram contra ela e a acusaram de envenenar o pai. Bellen não protestou. Ela entendia as motivações de suas irmãs. Ela deixou para trás sua vida como princesa de Giddah e se tornou uma espadachim errante. Impulsionada pelo desejo de proteger a honra e a herança de sua família, Bellen partiu em uma jornada solitária em busca de redenção e justiça. Seu caminho como espadachim errante é marcado pela determinação e bravura, ao enfrentar inúmeros desafios e perigos. Com a espada da família em mãos, Bellen se torna uma força imparável, usando sua habilidade na arte da espada para defender os desfavorecidos e combater a injustiça em um mundo turbulento. Embora enfrente a traição de suas irmãs e a perda de seu status nobre, Bellen encontra uma nova identidade e propósito em seu papel como espadachim errante. A cada batalha, ele fica mais perto de descobrir a verdade por trás da conspiração contra seu pai e desmascarar os verdadeiros responsáveis. Natureza: gentil = 7, severo = 3, honesto = 8, astuto = 2, calmo = 7,</t>
+  </si>
+  <si>
+    <t>Like:工艺|故事|特殊装备 WildMonsterKiller:1 Robber:100 Desc:Lut é filho de humildes agricultores da cidade de Cotta, que infelizmente perderam a vida durante uma praga devastadora. Desde cedo, Lut foi forçado a enfrentar a dura realidade da vida como um sem-teto. No entanto, seu destino mudou quando ele encontrou um desertor Dakn, que lhe ensinou as habilidades de combate necessárias para sobreviver em um mundo devastado pela guerra. Essas habilidades se tornaram sua salvação e lhe permitiram enfrentar os desafios que surgiram diante dele. Após a trágica morte de seu mentor, Lut Jahim tomou a decisão de ingressar oficialmente nas fileiras dos Dakn como um bravo guerreiro. Movido por uma sede insaciável de melhoria, Lut trabalha incansavelmente para subir na hierarquia Dakn. Sua dedicação e determinação são inabaláveis, e ele está disposto a enfrentar qualquer obstáculo para alcançar a grandeza. Natureza:gentil=6,severo=4,honesto=6,astúcia=4,calma=5,raiva=5,forte=8,fraco=2 habilidades de luta:冲刺膝盖顶|冲刺重拳|飞腿|蓄力冲刺 fight_dgskill :刺拳,1 AssSkill:统率技能赫连里德</t>
+  </si>
+  <si>
+    <t>Como:格斗|珠宝 Robber:100 WildMonsterKiller:1 Desc:Nativo dos pitorescos Umbra Cliffs, Jibirl costumava levar uma vida pacífica e satisfatória durante o reinado do Velho Rei. Seus dias foram preenchidos com o trabalho da terra e com as alegrias simples de sua humilde existência. No entanto, tudo mudou com a catastrófica Batalha do Sol Negro. As terras outrora férteis foram arrasadas, tornando-se áridas e inférteis. Forçado a abandonar seu lar idílico, Jibirl pegou uma lança robusta, despedindo-se de suas preciosas memórias e iniciando um novo caminho como mercenário errante. Agora uma alma nômade, Jibirl vagueia pela vasta extensão da terra, buscando propósito e fortuna através de suas habilidades como guerreiro de aluguel. O agricultor tranquilo adaptou-se às duras realidades de um mundo dominado por conflitos. A cada passo que dá, o peso do seu passado e a incerteza do seu futuro impulsionam-no para a frente. A lança de Jibirl torna-se sua fiel companheira, uma ferramenta para sobreviver em um mundo onde a capacidade de se defender tem grande valor. Natureza:gentil=5,severo=5,honesto=4,astúcia=6,calma=3,raiva=7,forte=7,fraco=3 habilidades de luta:冲刺膝盖顶|冲刺重拳|吼叫|蓄力冲刺 luta_dgskill:刺拳,1 AssSkill:统率技能车巴尔</t>
+  </si>
+  <si>
+    <t>Como:工艺|珠宝 Ladrão:100 WildMonsterKiller:1 Desc:Talat Hassan, um ferreiro habilidoso com um passado conturbado, costumava trabalhar nas perigosas minas de Redstone Keep. Sob a orientação de um mestre, ele aprimorou seu ofício e aprendeu a intrincada arte da ferraria. No entanto, sua propensão ao álcool e seu comportamento imprudente levaram a um incidente fatídico que cortou seus laços com a prestigiada instituição. Apesar de seu talento inegável, a falta de sobriedade de Talat o levou a ofender o próprio professor que o orientou. Determinado a encontrar seu próprio caminho, Talat deu as costas à vida mineira e adotou um novo papel como mercenário disponível para aluguel. Com seu martelo de forja na mão e um espírito perturbado dentro dele, ele atravessa o reino oferecendo seus serviços como ferreiro habilidoso e combatente competente. Embora assombrado por seus erros passados, as habilidades e perseverança de Talat permanecem insuperáveis, tornando-o um aliado procurado por aqueles que precisam de sua experiência. À medida que avança, Talat se esforça para superar seus demônios interiores, na esperança de conquistar uma nova reputação como ferreiro respeitado e redimir seu nome manchado. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=2,raiva=8,forte=5,fraco=4 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能呼延赭山 na esperança de conquistar uma nova reputação como ferreiro respeitado e resgatar seu nome manchado. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=2,raiva=8,forte=5,fraco=4 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能呼延赭山 na esperança de conquistar uma nova reputação como ferreiro respeitado e resgatar seu nome manchado. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=2,raiva=8,forte=5,fraco=4 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能呼延赭山</t>
+  </si>
+  <si>
+    <t>Como:秘宝|魔力 Desc:Hu'ud, um mago originário da cidade de Amaranth, tornou-se um guardião dedicado da natureza. Sua motivação surgiu quando sua mãe adoeceu gravemente, superando as possibilidades de cura mágica. Na esperança de encontrar uma solução no poder da natureza, Hu'ud interpretou as visões que lhe vieram através do Sol Negro como um sinal de redenção para o mundo. Convencido de que os espíritos primordiais poderiam ser canalizados pelos humanos, ele acreditava na possibilidade de usar esse poder para curar todas as doenças humanas e trazer cura ao mundo. Determinado a desvendar os segredos da magia da natureza, Hu'ud embarcou num caminho de estudo e prática intensivos. Através de sua dedicação, Adquiriu profundo conhecimento sobre o equilíbrio e a harmonia que regem o mundo natural. Agora, como guardião da natureza, ele busca preservar e proteger os recursos naturais, utilizando sua magia para curar e restaurar o equilíbrio nos locais afetados pela interferência humana. Seu desejo de usar seu dom mágico para um bem maior o leva a explorar novas maneiras de se conectar com a essência da natureza e encontrar soluções para os desafios que o mundo enfrenta. Natureza:gentil=4,severo=6,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能胡褐 Seu desejo de usar seu dom mágico para um bem maior o leva a explorar novas maneiras de se conectar com a essência da natureza e encontrar soluções para os desafios que o mundo enfrenta. Natureza:gentil=4,severo=6,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能胡褐 Seu desejo de usar seu dom mágico para um bem maior o leva a explorar novas maneiras de se conectar com a essência da natureza e encontrar soluções para os desafios que o mundo enfrenta. Natureza:gentil=4,severo=6,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能胡褐</t>
+  </si>
+  <si>
+    <t>Tipo:工艺 Ladrão:100 Desc:Ele trabalhava como oleiro em Cotta Town, mas perdeu o emprego e a casa durante a guerra. Buscando estabilidade, ele se tornou mercenário por um tempo, mas com o passar dos anos, ele ansiava por sua antiga vida. Ele decidiu retornar à cidade de Cotta e retomar seu ofício como artesão. Embora a vida continue difícil, ele encontrou paz em seu trabalho artesanal. Agora, ele trabalha com dedicação e desfruta da tranquilidade que seu trabalho lhe proporciona. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=6,raiva=4,forte=6,fraco=4 habilidades de luta:冲刺膝盖顶|冲刺重拳|饮酒|吼叫 luta_dgskill:刺拳,1 AssSkill:统率技能呼延鹿</t>
+  </si>
+  <si>
+    <t>Como:可爱|玩具|特殊装备 Desc:Triptych Rock é o lugar mais rico em minerais em Crying Rock. Durante a guerra, foi um campo de batalha e foi devastado. Inúmeras pessoas perderam tudo na guerra. Muta'aliq nasceu em Triptych Rock. Seus pais eram metalúrgicos. Na guerra, seus pais foram convocados para o exército e afastados de sua amada filha, sem saber seu destino. Sem os pais, Muta'aliq e sua avó dependiam um do outro. Eles trabalharam todos os dias durante dez anos, mas seus pais não voltaram. Cansada de esperar, Muta'aliq decidiu embarcar em uma jornada para encontrar seus pais. Ele decidiu aprender as artes arcanas e procurar o místico Furud. A lenda diz que o Furud pode ver o futuro. Muta'aliq deseja usar seu poder para encontrar seus pais. Sua determinação a leva a explorar os cantos mais sombrios e misteriosos em busca do paradeiro de seus pais. A cada passo, você mergulha no mundo da magia e dos segredos antigos. À medida que aprimora suas habilidades misteriosas, Muta'aliq encontra aliados e inimigos inesperados ao longo do caminho. Seu encontro com o místico Furud é o ponto de viragem que poderá revelar a verdade sobre o destino de seus pais. Com o poder de visão do futuro na ponta dos dedos, Muta'aliq enfrenta desafios e perigos para se reunir com sua família e encontrar a esperança perdida em tempos de guerra. Sua jornada é movida pela esperança e determinação para trazer luz às trevas que atormentam sua vida e encontrar o amor e a união perdidos nos escombros da guerra. Natureza: gentil = 7, severo = 3, honesto = 6, astuto = 4, calmo = 7,</t>
+  </si>
+  <si>
+    <t>Tipo:格斗|故事 WildMonsterKiller:1 Desc:Astrid era uma jovem que adorava lutar. Ela foi escolhida por um jovem nobre Nefrite para se tornar sua esposa. O nobre proibiu Astrid de praticar com armas... ou de deixar sua mansão. Um dia, o chefe do serviço da mansão do nobre descobriu que havia sido sequestrado por bandidos, que exigiam uma fortuna em Utar em troca da vida do nobre. Membros proeminentes do Nefrit se opunham a gastar tanto para resgatar uma única pessoa. Com a vida de seu ente querido em perigo, Astrid ignorou a ordem de ficar em casa e resgatou sozinha o marido. Ao retornar para Nefrite, seu marido a acusou falsamente de conluio com os bandidos. Atormentada, Astrid levou o marido ao líder da tribo para anular o casamento. Assim, Astrid se tornou uma lenda no deserto. Ela foi a primeira mulher a encerrar publicamente um casamento. Logo depois, Astrid voltou à sua paixão anterior e tornou-se uma guerreira. Natureza:gentil=6,severo=4,honesto=7,astúcia=3,calma=3,raiva=7,forte=10,fraco=0 habilidades de luta:蓄力冲刺|冲刺重拳|头槌|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能安红砂</t>
+  </si>
+  <si>
+    <t>Como:玩具|浪漫|乐器 Desc:A Sociedade Rosa Branca é a fonte de todos os curadores nesta terra. Riq é filha do líder da Sociedade Rosa Branca. Todos os membros da Sociedade Rosa Branca têm um símbolo de rosa na nuca. Este símbolo rosa é usado para supervisionar a magia de cura da sociedade, para garantir o controle sobre o preço e o status de cada curandeiro e a magia à sua disposição. Desta forma, Riq é única entre os curandeiros porque possui uma liberdade que nem mesmo os magos de mais alto nível da sociedade podem desfrutar. Riq não entendeu o motivo do controle estrito da Sociedade Rosa Branca, Então seu pai lhe disse para deixar os corredores sagrados da Sociedade para ver este mundo devastado com seus próprios olhos e aprender o valor de ser uma curandeira e ter uma compreensão mais profunda. Natureza:gentil=9,severo=1,honesto=7,astúcia=3,calma=6,raiva=4,forte=2,fraco=8 habilidades de luta:踩脚趾|直拳|飞腿|心清如水fight_dgskill:刺拳,1 AssSkill:统率技能曲玉</t>
+  </si>
+  <si>
+    <t>Como:工艺 Robber:100 WildMonsterKiller:1 Desc:A Águia Solitária, como o próprio nome sugere, é uma velha águia solitária que voa pelos céus do deserto. Ele tem um tapa-olho cobrindo uma cicatriz. Seu outro olho tem uma estranha cor dourada, sugerindo uma ancestralidade misteriosa. Ele é quieto e nunca fala sobre seu passado. As pessoas o reconhecem melhor pelo som metálico de seus passos e pelo falcão que ele carrega consigo. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=8,raiva=2,forte=7,fraco=3 habilidades de luta:蓄力冲刺|冲刺重拳|头槌|饮酒fight_dgskill:刺拳,1 AssSkill:统率技能独孤鹰</t>
+  </si>
+  <si>
+    <t>Como:工艺|地理 WildMonsterKiller:1 Desc:Kunju é um mágico excêntrico e desajeitado. À primeira vista, ninguém poderia suspeitar do seu verdadeiro potencial mágico. Seus pais eram mágicos excepcionalmente talentosos na cidade de Amaranth, mas devido à crescente pressão do círculo druida local, eles decidiram deixar sua casa e se estabelecer no Camel Bell Bazaar. Para Kunju, o movimentado bazar era muito mais atraente do que a monotonia dos magos na cidade de Amaranth. Lá ele encontrou pessoas fascinantes e experiências emocionantes que alimentaram sua paixão pela magia. Natureza:gentil=9,severo=1,honesto=9,astúcia=1,calma=4,raiva=6,forte=3,fraco=7 habilidades de luta:蓄力冲刺|冲刺重拳|头槌|饮酒fight_dgskill:刺拳,1 AssSkill:统率技能昆鹫</t>
+  </si>
+  <si>
+    <t>Like:地理|格斗 Robber:100 WildMonsterKiller:1 Desc:Nascida em uma família de fugitivos, essa jovem cresceu na cidade de Nagukka, imersa na opressão do Antigo Império. Com a queda do império, ela foi forçada a fugir de sua casa e enfrentar as adversidades do árido deserto. Durante anos, ele lutou para sobreviver em um ambiente implacável, enfrentando perigos e desafios que moldaram seu caráter e lhe deram habilidades excepcionais. Sua bravura e determinação a levaram a desenvolver habilidades incomparáveis ​​em combate, usando seu conhecimento das terras desérticas a seu favor. Com o passar do tempo, ela se tornou uma especialista em navegação no deserto e na arte da sobrevivência. Sua astúcia e habilidades táticas permitem que ele supere qualquer obstáculo que surja em seu caminho, tornando-a uma força a ser reconhecida em qualquer situação. Natureza: gentil=3,severo=7,honesto=1,astúcia=9,calma=4,raiva=6,forte=7,fraco=3 habilidades de luta:踩脚趾|直拳|飞腿|心清如水fight_dgskill:刺拳,1 AssSkill:统率技能尉迟月</t>
+  </si>
+  <si>
+    <t>Tipo:绘画|故事 Desc:A família de Hartum eram comerciantes no Bazar Dourado. Quando a guerra começou, sua família fugiu para Diresprings. Em Diresprings, eles começaram uma nova vida, mas à medida que a guerra se espalhava, bandidos saquearam sua casa. Muitos dos ricos perderam tudo o que tinham, incluindo amigos próximos da família. No entanto, os pais de Hartum recusaram-se a ajudá-los a garantir que o filho tivesse uma vida boa, o que gerou grande ressentimento. Hartum entendeu que seus pais estavam agindo no seu melhor interesse, mas não pôde deixar de se sentir culpado. Ele se sente desconfortável com sua vida confortável. Natureza:gentil=6,severo=4,honesto=6,astúcia=4,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能何风</t>
+  </si>
+  <si>
+    <t>Como:历史|神秘 Desc:Isa, a mulher sábia de Diresprings, é uma buscadora incansável de conhecimento e relíquias antigas. Ele vasculhou os cantos mais remotos da terra em busca de tecnologia perdida e fragmentos de sabedoria antiga. Sua paixão pelo passado a leva a ajudar outras pessoas a reconstruir suas casas usando os segredos escondidos nessas relíquias antigas. Contudo, o desejo mais profundo de Isa vai além da simples recuperação de artefatos. Ele sonha com um mundo em que os poderosos abandonem as armas e se comprometam com o desenvolvimento científico. Ele acredita fervorosamente que a ciência e o conhecimento são as verdadeiras ferramentas para garantir a estabilidade e a felicidade de todos os habitantes da terra. Com sua sabedoria e determinação, Isa trabalha incansavelmente para difundir a importância da educação e do progresso científico, em busca de um futuro melhor para todos. Natureza:gentil=8,severo=2,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能伊孤</t>
+  </si>
+  <si>
+    <t>Tipo:特殊装备|神秘 Ladrão:100 Desc:Bataru nasceu nos Penhascos Umbra, mas estava insatisfeito com a vida como fazendeiro lá. Ele viajou para o Grande Deserto e se juntou à Guilda Comercial Corsac. Ao cobrar uma dívida, ele matou um homem, traindo as regras do Corsac. Bataru foi excomungado da Guilda dos Comerciantes Corsac e exilado para sempre de Dunestorm. Após ser exilado, Bataru passou a odiar o Corsac. Ele se tornou cada vez mais violento e sedento de poder, até se tornar um temido e implacável bandido do deserto com um único objetivo: matar o imprudente líder dos Corsac. Natureza:gentil=2,severo=8,honesto=3,astúcia=7,calma=2,raiva=8,forte=8,fraco=2 habilidades de luta:冲刺重拳|升龙拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能巴塔鲁</t>
+  </si>
+  <si>
+    <t>Como:神秘|文学|特殊装备 WildMonsterKiller:1 Desc:Alaf Jahim era apenas um jovem quando veio para o Grande Deserto para ganhar a vida como escolta de caravana. Hoje, é amplamente conhecido como músculo de aluguel. Ele escoltou inúmeros viajantes e derrotou bandidos demais para contar. Mas o tempo não perdoou este herói. Alaf Jahim já tem mais de 60 anos e não tem a mesma energia de sua juventude. As tarefas de escolta mais difíceis escapam lentamente de seu alcance, mas seu nome ainda causa medo nos corações dos bandidos. Seu status lendário entre as arenas perdura. Natureza:gentil=5,severo=5,honesto=8,astúcia=2,calma=6,raiva=4,forte=10,fraco=0 habilidades de luta:冲刺重拳|升龙拳|吼叫|饮酒|绝技裂地 fight_dgskill :刺拳,1 AssSkill:统率技能赫连千百</t>
+  </si>
+  <si>
+    <t>Like:故事|工艺 WildMonsterKiller:1 Desc:Makan é um trabalhador de baixa reputação. Ele é um pouco preguiçoso e covarde, mas constantemente encontra trabalho devido à sua habilidade em reparos. Ele odeia aqueles que saqueiam e destroem porque isso cria mais trabalho para eles. Makan tem um talento inato para reparos, embora sua habilidade seja subestimada. Ele é conhecido como a pessoa certa quando algo precisa ser consertado. A sua especialidade reside na restauração de estruturas e objetos danificados, sejam edifícios, máquinas ou mesmo artefactos delicados. A sua atenção meticulosa aos detalhes e a capacidade de reviver coisas quebradas tornaram-no indispensável para aqueles que valorizam o seu trabalho artesanal. No fundo, Makan guarda um profundo ressentimento contra aqueles que se envolvem em saques e destruição. Ele despreza o caos que eles deixam, pois não só perturba a paz, mas também cria mais trabalho para ele ao ter que reparar os danos causados. Natureza:gentil=5,severo=5,honesto=4,astúcia=6,calma=5,raiva=5,forte=3,fraco=7 habilidades de luta:冲刺重拳|升龙拳|吼叫|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能何疆</t>
+  </si>
+  <si>
+    <t>Como:浪漫|忧伤|音乐 Desc:Yousef era um espadachim dos Nasir até que sua esposa morreu há três anos devido a uma doença grave. Devido a um desentendimento entre a Sociedade Rosa Branca e o Nasir, a Sociedade retirou todos os seus mágicos curandeiros do Nasir. Sem os mágicos de cura da Sociedade Rosa Branca, muitos Nasir morreram de doenças ou ferimentos graves, incluindo, é claro, a esposa de Yousef. Após seu falecimento, Yousef adquiriu um profundo apreço pela magia de cura e procurou a Sociedade Rosa Branca para receber treinamento nas artes de cura. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=8,raiva=2,forte=3,fraco=7 habilidades de luta:冲刺重拳|升龙拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能齐肃之</t>
+  </si>
+  <si>
+    <t>Like:故事|浪漫 Desc:O líder da famosa Casa Kabir. A Casa Kabir é uma das famílias mais ricas do deserto, depois de gerações trabalhando na indústria de mineração. Além de sua imensa riqueza, a Casa Kabir é conhecida por um talento arcano especial: a habilidade de controlar o ouro. Qualquer coisa feita de ouro pode ser uma arma para a Casa Kabir. Cada membro da Câmara tem sua própria arma de ouro pessoal. Goldie gosta especialmente de um saco cheio de folhas douradas. Geralmente não há como recuperar tal arma, mas o jovem líder da Casa Kabir não se importa com dinheiro. Goldie tem uma irmã dez anos mais nova que ele. Ele adora sua irmã mais nova, mas ela não parece gostar de seu irmão mais velho. Natureza:gentil=7,severo=3,honesto=2,astúcia=8,calma=6,raiva=4,forte=5,fraco=5 habilidades de luta:冲刺重拳|升龙拳|飞腿|饮酒 luta_dgskill:刺sim,</t>
+  </si>
+  <si>
+    <t>Como:玩具|可爱|乐器 Desc:Lotus, membro da Casa Kabir, possui um dom extraordinário para a magia que supera até mesmo os praticantes mais habilidosos. Porém, seu poder é indomável e volátil, causando caos e destruição por onde passa. O sino dourado que ele empunha atua como um canal para sua magia, amplificando seu poder, mas também ampliando sua natureza imprevisível. Temendo as repercussões de suas habilidades descontroladas, Lotus tomou a difícil decisão de deixar sua casa e embarcar em uma busca para encontrar uma maneira de dominar sua magia e aproveitar seu potencial para o bem. Durante sua jornada, Lotus encontra antigos seres místicos e busca orientação de sábios e mágicos experientes. Aprenda rituais antigos e conhecimentos proibidos que podem desvendar os segredos para controlar seu imenso poder. Ao longo do caminho, ele enfrenta inúmeros desafios e provações, tanto internas quanto externas, enquanto luta contra seus próprios demônios interiores e se esforça para encontrar seu verdadeiro propósito. Apesar dos riscos e dificuldades que enfrenta, Lotus está determinada a encontrar equilíbrio e tornar-se uma detentora responsável de suas formidáveis ​​habilidades mágicas, na esperança de usar seus poderes para proteger e trazer harmonia ao mundo. Natureza:gentil=9,severo=1,honesto=7,astúcia=3,calma=5,raiva=5,forte=1,fraco=9 habilidades de luta:踩脚趾|直拳|飞腿|心清如水fight_dgskill:刺拳,1 AssSkill:统率技能金玉叶 enquanto ele luta contra seus próprios demônios interiores e se esforça para encontrar seu verdadeiro propósito. Apesar dos riscos e dificuldades que enfrenta, Lotus está determinada a encontrar equilíbrio e tornar-se uma detentora responsável de suas formidáveis ​​habilidades mágicas, na esperança de usar seus poderes para proteger e trazer harmonia ao mundo. Natureza:gentil=9,severo=1,honesto=7,astúcia=3,calma=5,raiva=5,forte=1,fraco=9 habilidades de luta:踩脚趾|直拳|飞腿|心清如水fight_dgskill:刺拳,1 AssSkill:统率技能金玉叶 enquanto ele luta contra seus próprios demônios interiores e se esforça para encontrar seu verdadeiro propósito. Apesar dos riscos e dificuldades que enfrenta, Lotus está determinada a encontrar equilíbrio e tornar-se uma detentora responsável de suas formidáveis ​​habilidades mágicas, na esperança de usar seus poderes para proteger e trazer harmonia ao mundo. Natureza:gentil=9,severo=1,honesto=7,astúcia=3,calma=5,raiva=5,forte=1,fraco=9 habilidades de luta:踩脚趾|直拳|飞腿|心清如水fight_dgskill:刺拳,1 AssSkill:统率技能金玉叶</t>
+  </si>
+  <si>
+    <t>Como:地理 WildMonsterKiller:1 Desc:O pai de Saqie é um famoso guerreiro Nasir. Vinte anos atrás, seu pai recebeu ordens de destruir o Oryx. Porém, ele era de bom coração e sabia que os Oryx estavam velhos e fracos, à beira da derrota. Outro ataque contra eles seria como uma carnificina. Depois de muita deliberação, o pai de Saqie decidiu levar Saqie e fugir. Eles foram marcados como traidores e desertores pelos Nasir. Os guerreiros os perseguiram, na esperança de receber uma recompensa. Saqie e seu pai fugiram por cinco anos, até que um dia seu pai desapareceu sem deixar vestígios. Saqie não acreditava que seu pai tivesse simplesmente desaparecido, então ela pegou a espada de seu pai e partiu em uma jornada para encontrá-lo. Natureza: gentil = 4, severo = 6, honesto = 5, astúcia = 5, calmo = 3, raiva = 7, forte = 8, fraco = 2 habilidades de luta:</t>
+  </si>
+  <si>
+    <t>Like:浪漫|女神|神秘 WildMonsterKiller:1 Robber:100 Desc:Nabiha, apelidado de Crimson Artist ou Red Madman, gosta das cores mais finas e dos objetos mais elegantes. Ele é um espírito livre e imprevisível, ocasionalmente agindo por um senso de retidão, mas sem princípios rígidos para guiá-lo. Ele simplesmente faz o que lhe agrada. Ele não é uma boa pessoa, mas também não é de todo ruim. Nabiha busca seu próprio senso de valor artístico, bem como a alma artística da terra. Ele acredita firmemente que o mundo acabará sendo tingido com sua cor favorita e só então se tornará uma obra de arte suprema. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能舒禹舟</t>
+  </si>
+  <si>
+    <t>Like:故事|文学|地理 Desc:Sur é um famoso alpinista nas montanhas alpinas. Ele tem um companheiro que chama de "Ilyas", embora poucos saibam que esse nome delicado é na verdade um machado de escalada encantado. Para Sur, um machado de escalada é um companheiro em situações de vida ou morte. Sur é um alpinista profissional. Ele trabalha duro para treinar para enfrentar montanhas ainda mais altas. O maior alvo de Sur é a grande montanha a leste: Ilyas. Natureza:gentil=5,severo=5,honesto=6,astúcia=4,calma=7,raiva=3,forte=9,fraco=1 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能石哈</t>
+  </si>
+  <si>
+    <t>Tipo:珠宝|格斗 Robber:100 Desc:Mousa era um jogador fantástico quando era jovem, com uma sorte aparentemente ilimitada. Como tal, ele tinha dinheiro, status, mulheres e uma vida muito extravagante. Um dia, Mousa recebeu um desafio. O desafiante era um guerreiro das montanhas Zagros, que reuniu todas as riquezas de sua tribo para apostar tudo contra Mousa. Arrogantemente, Mousa aceitou, acreditando que o seu adversário era um tolo. Mas durante a batalha, Mousa não só perdeu tudo, mas seu oponente cortou ambas as mãos... Em estado de desespero, Mousa encontrou o técnico Infan. Infan colocou brocas nos cotos dos braços de Mousa. Mousa está agora armado com armas extremamente poderosas. Depois de renascer, Mousa ainda tem problemas com o jogo, mas agora só aposta em uma coisa: o Destino. Natureza: gentil = 2, grave = 8, honesto = 1,</t>
+  </si>
+  <si>
+    <t>Como:特殊装备|忧伤 WildMonsterKiller:1 Desc:Mathali nasceu em uma família imersa na guerra. Os membros da família poderiam usar mana para alimentar suas espadas. Quando a guerra começou, a família de Mathali, que só se destacava em duelos, foi ignorada. Muitos membros da família tiveram que encontrar novas carreiras. Suas técnicas únicas de combate estavam à beira de serem perdidas para sempre. Mathali é o único jovem de sua geração que aprendeu a usar mana para lutar. Sobre seus ombros recai não apenas o fardo de reavivar a glória da família, mas também a missão de transmitir essas artes secretas. Natureza:gentil=8,severo=2,honesto=5,astúcia=5,calma=6,raiva=4,forte=8,fraco=2 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒fight_dgskill:刺拳,1 AssSkill:统率技能韩靖</t>
+  </si>
+  <si>
+    <t>Como:绘画|忧伤 WildMonsterKiller:1 Robber:100 Desc:Sanjay, um mago poderoso e enigmático, vem de um reino distante envolto em mistério. Movido por uma curiosidade insaciável, ele atravessou terras perigosas e reinos traiçoeiros para chegar a esta terra, atraído por rumores de poder arcano inexplorado escondido no caos da guerra. Sua busca pelo conhecimento proibido o levou a mergulhar em rituais obscuros e textos proibidos, buscando desvendar os segredos de como aproveitar a energia bruta gerada pela dor e pela tragédia. À medida que ele se aprofundava em sua investigação, a bússola moral de Sanjay começou a ficar confusa e sua obsessão pelo poder o consumiu. Ele ficou obcecado com a ideia de manipular a própria essência do sofrimento, aproveitando sua energia para alimentar suas próprias habilidades misteriosas. A cada experiência, ele se distanciava mais da situação dos outros, vendo a dor deles apenas como uma fonte para seu próprio avanço. Agora, ele vagueia pela terra como uma figura temida e fascinante, movido por sua busca incansável por conhecimento proibido e por seu desejo insidioso de dominar as artes sombrias de extrair poder arcano dos cantos mais sombrios do sofrimento humano. Natureza:gentil=2,severo=8,honesto=2,astúcia=8,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能萨加 impulsionado por sua busca incansável por conhecimento proibido e seu desejo insidioso de dominar as artes sombrias de extrair poder arcano dos cantos mais sombrios do sofrimento humano. Natureza:gentil=2,severo=8,honesto=2,astúcia=8,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能萨加 impulsionado por sua busca incansável por conhecimento proibido e seu desejo insidioso de dominar as artes sombrias de extrair poder arcano dos cantos mais sombrios do sofrimento humano. Natureza:gentil=2,severo=8,honesto=2,astúcia=8,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能萨加</t>
+  </si>
+  <si>
+    <t>Like:历史|故事 Desc:Zafeera sempre carrega consigo escamas de prata em suas andanças sem rumo. Orgulha-se da sua natureza pacífica. Ela não é uma maga que mata, mas ainda é um pesadelo para os moradores próximos. Se Zafeera vir alguém com uma calça enrolada em uma perna, ela enrolará o outro lado. Se você vir alguém com metade do cabelo faltando, você irá raspá-lo de graça. Se você vir alguém sem um braço, Zafeera cortará o outro braço. Seu comportamento errático não se baseia em seu humor no momento ou em qualquer outra circunstância, mas sim na busca por sua ideia de “equilíbrio”. Seu compromisso com o equilíbrio é extremo e ele nunca para de buscá-lo. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=9,raiva=1,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能韦利纳</t>
+  </si>
+  <si>
+    <t>Tipo:音乐|浪漫|忧伤 Desc:Ela costuma dançar à beira do rio, seu reflexo na água é seu único público. Desde criança, Umara sonhava em se tornar uma verdadeira dançarina. Quando o velho rei foi deposto, os Nasirs ocuparam a cidade de Jamal, a antiga capital. À medida que a guerra continuava e os combates continuavam, a cidade de Jamal permaneceu em alerta constante. Umara nem sabia como era Jamal City, nem tinha os documentos necessários para ir até lá. Mesmo assim, Umara pratica todos os dias para se juntar ao grupo de artistas mais famoso da cidade e se tornar uma dançarina profissional. Quando ela estiver no maior palco do mundo, o público sob seus pés conhecerá a maior felicidade. Natureza:gentil=7,severo=3,honesto=8,astúcia=2,calma=5,raiva=5,forte=7,fraco=3 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳,</t>
+  </si>
+  <si>
+    <t>Como:文学|音乐 Desc:Tiqin nasceu como membro de uma nobre casa Nasir. Ele poderia ter levado uma vida refinada e pacífica, mas ao saber das más ações dos Nasir através de seu grande amor pela história, decidiu deixar sua casa e escolher a paz em vez da guerra. Usando o conhecimento de alquimia que lhe foi transmitido durante a juventude, ela se tornou uma alquimista viajante. Natureza:gentil=7,severo=3,honesto=3,astúcia=7,calma=6,raiva=4,forte=8,fraco=2 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能提可沁</t>
+  </si>
+  <si>
+    <t>Tipo:绘画|故事 Desc:Ele já foi um cidadão comum de uma cidade comum. Quando ele tinha 12 anos, bandidos saquearam e assassinaram a população de sua cidade. Testemunhar o massacre de seus companheiros liberou as habilidades mágicas latentes de Assel. Uma magia poderosa foi desencadeada na cidade. Assel expulsou os bandidos, mas também feriu muitos moradores locais. A vida nunca mais foi a mesma para Assel. Embora ninguém expressasse isso abertamente, Assel podia sentir que as pessoas já não o viam da mesma maneira. Assel tomou a decisão de deixar sozinho sua cidade natal e viajar pelo mundo. Ele espera um dia ter controle suficiente sobre seu poder para proteger os inocentes como um mago poderoso. Natureza: gentil=6,severo=4,honesto=8,astúcia=2,calma=3,raiva=7,forte=2,fraco=8 habilidades de luta:踩脚趾|直拳|飞腿|冲刺重拳fight_dgskill:刺拳,1 AssSkill:统率技能阿塞尔</t>
+  </si>
+  <si>
+    <t>Como:神秘|特殊装备 WildMonsterKiller:1 Robber:100 Desc:Basit já foi o melhor carrasco do antigo império. Ele separou inúmeras cabeças de seus corpos. Aplicou rigorosamente todas as leis e agiu como um símbolo da lei e da ordem no Antigo Império. Quando a cidade de Jamal caiu, o carrasco tornou-se um pária odiado. As famílias daqueles que ele matou se uniram para prendê-lo e jogar fora a chave, pensando que Basit morreria de fome ou se tornaria alimento para roedores. Basit comeu ratos para sobreviver, no entanto, um dos ratos que comeu foi amaldiçoado. A maldição foi transferida para ele. Agora Basit era imortal... mas estava condenado a sempre conhecer o sofrimento. A forma de Basit se contorceu em sua prisão infernal. A cauda de um rato cresceu e exalou gases nocivos. Basit procurou nas ruínas da cidade de Jamal até encontrar sua antiga espada de carrasco. Assim que o segurou nas mãos, ele só tinha um desejo: punir todos os pecadores do mundo. Natureza:gentil=1,severo=9,honesto=1,astúcia=9,calma=4,raiva=6,forte=9,fraco=1 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能卜烈</t>
+  </si>
+  <si>
+    <t>Like:神秘|珠宝 Robber:100 Desc:No leste há um rio longo e sinuoso. Onde há rios, há pessoas. Emin é um salvador que vive e trabalha no rio. Por Utar suficiente, Emin resgatará qualquer coisa que esteja no fundo do rio para qualquer pessoa, seja bens, cadáveres ou tesouros. Ele não se importa se o tesouro que recupera vale mais do que o preço que recebe para resgatá-lo, ou se o cadáver no leito do rio tem alguma história trágica por trás dele. O rio lava sua alma e tira essas emoções desnecessárias e inúteis. Natureza:gentil=5,severo=5,honesto=5,astúcia=5,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能罗夫</t>
+  </si>
+  <si>
+    <t>Como:工艺|神秘 Desc:Shahid nasceu em uma pequena vila árida no Vale Twinluna. Quase todos os homens nascidos lá se juntaram aos Dakn Night Rangers para ganhar a vida, e Shahid não foi exceção. Os Night Rangers foram responsáveis ​​por perigosas missões de reconhecimento em cavernas cheias de monstros. A maioria dos Night Rangers veio de origens humildes e teve treinamento limitado. Poucos retornaram de suas missões subterrâneas. Shahid usou sua agilidade e reflexos excepcionais para sobreviver a vários ataques aos covis escuros, ganhando a atenção de seu comandante. O comandante tomou Shahid como aprendiz e o promoveu a Capitão dos Night Rangers. Um homem comum aproveitaria esta posição para escapar desta vida de escuridão e morte mas Shahid entendeu que seu comandante seu mestre Foi ele quem formou os Night Rangers. Isso fez dele o homem responsável pelas mortes de seu pai e tio. Agora Shahid deve escolher entre a vingança e a vida. Natureza:tipo=3,severo=7,honesto=0,astúcia=10,calma=9,raiva=1,forte=6,fraco=4 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgshabilidade:刺拳, 1 AssSkill:统率技能邵影</t>
+  </si>
+  <si>
+    <t>Tipo:乐器|忧伤|浪漫|女神 Desc:Takiyah perdeu uma perna durante os tempos turbulentos de sua juventude. Embora seu corpo estivesse fraco, seu coração estava forte. Um dia, ele resgatou um viajante ferido que desabou nos portões de sua aldeia. Quando o viajante acordou, não disse nada e saiu pelas portas. Na manhã seguinte, todas as pessoas da aldeia de Takiyah perderam a perna esquerda. Takiyah não percebeu que sua gentileza traria tamanho desastre para a aldeia. Sua culpa a levou a deixar sua cidade natal... Natureza: gentil = 10, severo = 0, honesto = 9, astúcia = 1, calma = 5, raiva = 5, forte = 4, fraco = 6 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能耶雅莉瓦</t>
+  </si>
+  <si>
+    <t>Tipo:文学|工艺 Ladrão:100 Desc:O avô de Infan era um técnico muito famoso em sua época. No entanto, seu avô foi acusado de ser leal ao Antigo Império e foi preso. Uma geração de artesãos lendários morreu com ele. Infan era originalmente um fazendeiro comum. Ao arrumar os pertences do avô, ele acidentalmente encontrou o manual do técnico deixado pelo avô. No início ele estava apenas curioso, mas rapidamente ficou obcecado. Ele não pôde deixar de aprimorar suas habilidades mecânicas, trabalhando dia e noite, esquecendo de comer e dormir. Eventualmente, ele dominou completamente as habilidades de seu avô e até começou a incorporar suas próprias ideias. Nasceu um mestre da maquinaria. Natureza:gentil=7,severo=3,honesto=5,astúcia=5,calma=6,raiva=4,forte=8,fraco=2 habilidades de luta:踩脚趾|冲刺重拳|绝技裂地|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能封大木</t>
+  </si>
+  <si>
+    <t>Como:特殊装备|装饰 WildMonsterKiller:1 Desc:Zina nasceu em uma pequena tribo. Seu pai era um lutador habilidoso e um famoso líder militar dentro da tribo. Cada um dos cinco irmãos de Zina era um guerreiro da tribo. Zina era a querida de seu pai e amada por sua família. Mas ela não queria viver uma vida protegida, então fugiu. Zina planejou encontrar o famoso Mestre Espadachim nas Montanhas Zagros. A lenda diz que este mestre poderia derrubar cem inimigos com um único golpe. Natureza:gentil=6,severo=4,honesto=5,astúcia=5,calma=5,raiva=5,forte=8,fraco=2 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能日娜</t>
+  </si>
+  <si>
+    <t>Tipo:乐器|神秘|忧伤 Desc:Hina parece ser de outro mundo. Ninguém sabe de onde ele vem ou quais são seus planos. Ele é gentil e elegante, embora seus cabelos brancos e olhos prateados contrastem com seu rosto jovem. Hina costuma sentar-se à beira do rio com uma aparência perdida, sua saia iridescente como uma concha refletindo um arco-íris. É pálido e precioso, como uma pérola levada à praia. Natureza:gentil=6,severo=4,honesto=5,astúcia=5,calma=8,raiva=2,forte=4,fraco=6 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能韩瑶</t>
+  </si>
+  <si>
+    <t>Tipo:乐器|格斗|浪漫 WildMonsterKiller:1 Robber:100 Desc:Toya já foi um assassino impenitente. Ele tem o sangue de inúmeras almas em suas mãos. Ao contrário de um caçador de recompensas, Toya matou sem se preocupar com o lucro e se tornou o criminoso mais procurado do antigo império. Ele cumpriu sua pena na prisão de Jamal City. Quando o Nefrit caiu, Toya estava livre novamente. Sua alma cantava nesta terra em guerra, cheia de batalhas e monstros. Toya gosta do novo mundo e do sofrimento sem fim que ele causa aos outros. Natureza:tipo=1,severo=9,honesto=0,astúcia=10,calma=5,raiva=5,forte=5,fraco=5 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能托亚</t>
+  </si>
+  <si>
+    <t>Tipo:神秘|格斗 Ladrão:100 Desc:Yaya teve uma infância infeliz. Ela foi abandonada por ser tão feia. Não conhecendo o amor, Yaya tornou-se cruel e implacável. Ele rejeitou tudo no mundo humano. Só para experimentar um pouco de sopa, a vovó concordou em se tornar objeto de experimentos de uma feiticeira aos dezesseis anos. Centenas de pessoas morreram nessas experiências cruéis, mas Yaya sobreviveu. Ela se tornou parte mulher, parte monstro! Seu novo poder monstruoso combinava bem com seu egoísmo e crueldade. Caminhe pelo mundo como um pesadelo. Agora o nome Yaya é sinônimo de morte. Natureza:gentil=5,severo=5,honesto=7,astúcia=3,calma=3,raiva=7,forte=9,fraco=1 habilidades de luta:踩脚趾|直拳|飞腿|饮酒 luta_dgskill:刺拳, 1 AssSkill:统率技能耶牙</t>
+  </si>
+  <si>
+    <t>Like:工艺 WildMonsterKiller:1 Desc:O implacável Galo Zahra, com um coração de aço. Ela já foi uma jovem nobre de Nefrit e herdeira da Casa Zahra. Foi abandonado quando a aliança sitiou a cidade de Jamal. Com apenas seis anos de idade, ela sofreu abusos inimagináveis ​​nas mãos de seus captores. Seu corpo foi destruído e ele perdeu o braço e a perna esquerdos. Um guerreiro com uma armadura móvel rudimentar a salvou de seus cruéis captores e a ajudou a escapar da cidade de Jamal. O guerreiro perguntou se ele queria viver, mas Gallus não conseguiu emitir nenhum som. Ele lutou com todas as suas forças e acenou com a cabeça. Desde aquele dia, um guerreiro meio mecânico ronda os Penhascos Umbra. Ele carrega consigo um legado de dor e resistência. As terras dos Penhascos Umbra se tornaram seu lar, onde ele persegue como uma sombra em busca de justiça. Seu rosto, que esconde uma doçura perdida entre as adversidades, contrasta com a intensidade de seus olhos azuis profundos que brilham com uma luz inabalável na escuridão da noite. Natureza:gentil=7,severo=3,honesto=7,astúcia=3,calma=5,raiva=5,forte=10,fraco=0 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 fight_dgskill:刺拳,1 AssSkill:统率技能西河伽罗</t>
+  </si>
+  <si>
+    <t>Como:乐器|音乐 Desc:Aganazzar, conhecido como a Estrela da Harmonia, é um artista talentoso cujo instrumento é a própria magia. Sua voz celestial e habilidades mágicas têm o poder de curar não apenas feridas físicas, mas também almas aflitas. Criada pela avó feiticeira, Aganazzar aprendeu a canalizar sua energia mágica através da música, transformando cada música em um feitiço de cura que toca o coração de quem a ouve. Rejeitando ofertas dos poderosos nobres que desejavam possuí-la, Aganazzar parte numa viagem errante, levando a sua música e magia a quem mais precisa, deixando um rasto de cura e esperança no seu rasto. Aganazzar tornou-se uma lenda no reino, conhecido pela sua capacidade de trazer harmonia e alívio através da sua música. Seu espírito livre e rebelde a leva a viajar por terras distantes, evitando sempre ser capturada por quem a considera uma possessão. Em cada apresentação, ele demonstra sua habilidade musical e profundo conhecimento de magia, criando um vínculo mágico com seu público e despertando emoções profundas. Natureza:gentil=6,severo=4,honesto=3,astúcia=7,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能安古欢</t>
+  </si>
+  <si>
+    <t>Tipo:音乐|乐器 DescEmbora pareça ter dez anos, ela tem a sabedoria e a seriedade de uma mulher de oitenta anos. Muitos ficam surpresos ao ver uma garota bruxa. Seu dom inato para a profecia lhe rendeu muitos seguidores, mas ela se recusa a exercer autoridade sobre eles. Najima frequentemente olha para um ponto no céu com uma expressão vazia. Ninguém sabe de onde veio e ninguém sabe para onde irá. Natureza:gentil=5,severo=5,honesto=10,astúcia=0,calma=7,raiva=3,forte=5,fraco=5 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能天星</t>
+  </si>
+  <si>
+    <t>Like:装饰|可爱 Desc:Em um mundo cheio de caos e violência, Batu surge como um enigma singular. A sua figura imponente, adornada com músculos poderosos, contrasta com o seu apreço pela paz e a sua aversão ao conflito. Porém, quando a injustiça se manifesta na forma de briga, Batu não resiste a agir. Nesses momentos, sua força imponente é liberada e seus punhos tornam-se instrumentos para acabar com a violência, sempre com o intuito de restaurar a harmonia e a tranquilidade. Apesar de sua aparência imponente, Batu tem um coração bondoso e gentil. Na maioria dos dias, ela busca serenidade em suas atividades diárias e encontrou um hobby incomum na costura. Com uma destreza inesperada, ele usa agulha e linha para reparar os rasgos que muitas vezes ocorrem em suas roupas durante seus momentos de ação. Este contraste único entre a sua natureza imponente e a sua habilidade no bordado mostra a diversidade de facetas que compõem Batu, um protetor comprometido com a paz e dedicado a encontrar a beleza nas habilidades mais inesperadas. Natureza: gentil=9,severo=1,honesto=9,astúcia=1,calma=9,raiva=1,forte=1,fraco=9 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳fight_dgskill:刺拳,1 AssSkill:统率技能巴图</t>
+  </si>
+  <si>
+    <t>Como:浪漫|工艺 WildMonsterKiller:1 Robber:100 Desc:O Sol Negro despertou um gênio antigo e maligno. Este gênio perverso há muito perdeu seu lar original. Um desequilíbrio nas forças universais prendeu-o numa espada... uma espada que pertencia a Rwal. O gênio nunca para de tentar assumir o controle do corpo de Rwal, enquanto Rwal é forçado a resistir constantemente. Rwal está ficando mais fraco a cada dia. Não demorará muito para que esta terra tenha outro espadachim possuído por um gênio. Natureza: gentil=6,severo=4,honesto=3,astúcia=7,calma=4,raiva=6,forte=4,fraco=6 habilidades de luta:踩脚趾|冲刺重拳|飞腿|吼叫fight_dgskill:刺拳,1 AssSkill:统率技能墨敕</t>
+  </si>
+  <si>
+    <t>Tipo:装饰|玩具|可爱 Desc:Wakata morava com seu pai em uma terra distante ao leste, coberta de neve. Apesar da neve, naquela terra distante existem muitas fontes termais onde florescem lindas flores de pêssego rosa. A vida tranquila de Wakata chegou ao fim abruptamente quando seu pai desapareceu. Ele começou uma jornada para o oeste para encontrar seu pai. O que ele não sabia era que a magia de cura que aprendeu com seu pai tornaria sua jornada para o oeste incrivelmente perigosa. Natureza:gentil=8,severo=2,honesto=5,astúcia=5,calma=5,raiva=5,forte=8,fraco=2 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒 luta_dgskill:刺拳,1 AssSkill:统率技能若桃</t>
+  </si>
+  <si>
+    <t>Like:历史|特殊装备|音乐 Desc:A magia não pode simplesmente ser lançada do nada. Alguns tipos de magia requerem componentes ou ferramentas arcanas, enquanto outros consomem o poder espiritual do conjurador. Um artífice que usa magia para forjar uma arma mágica criará uma reação mágica oposta cada vez que criar a referida arma. Esse tipo de negação mágica duradoura é um preço que todo artesão deve pagar. Quanto mais poderosa for a arma, maior será o preço e maior será a resistência. Eventualmente, um artífice não pode usar uma arma criada por seu próprio povo, muito menos sua própria arma encantada. Esta é a oficina mais solitária do planeta. Eles forjaram armas durante toda a vida, mas agora devem dizer adeus ao trabalho de sua vida. Natureza: gentil = 5, severo = 5, honesto = 6, astúcia = 4, calmo = 7, raiva = 3, forte = 5, fraco = 5 habilidades de luta:</t>
+  </si>
+  <si>
+    <t>Como:浪漫|地理 WildMonsterKiller:1 Desc:Nura é uma guerreira de origens misteriosas. Ela é tão habilidosa quanto bonita e tem uma vontade forte. Ela é versada em todos os tipos de armas e seu combate desarmado também é excelente. Durante uma missão secreta, ele descobriu o salitre. Desde então, ele vem fazendo experiências com pólvora. Ele viajou milhões de côvados até esta terra devastada pela guerra para encontrar um lugar adequado para testar a força de sua pólvora. Natureza: gentil=6,severo=4,honesto=5,astúcia=5,calma=4,raiva=6,forte=8,fraco=2 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳fight_dgskill:刺拳,1 AssSkill:统率技能薇卡</t>
+  </si>
+  <si>
+    <t>Como:忧伤|特殊装备 Ladrão:100 Desc:A escuridão sustenta o pecado e o desejo, assim como Raheel por dez longos anos. Depois que o sol negro nasceu no céu, o povo de Raheel acreditou que o sol trazia maldições e cataclismos, então eles construíram uma cidade subterrânea e começaram uma vida longe do sol. Esta cidade subterrânea permaneceu estável durante dez anos, mas esta estabilidade foi rapidamente minada no meio de uma grande fome... Raheel emergiu como o único vencedor desta batalha sangrenta pela sobrevivência. Ele deixou a escuridão e saiu da masmorra. Natureza:gentil=1,severo=9,honesto=1,astúcia=9,calma=7,raiva=3,forte=10,fraco=0 habilidades de luta:踩脚趾|冲刺重拳|飞腿|饮酒|绝技组合拳fight_dgskill:刺拳,1 AssSkill:统率技能桑开</t>
+  </si>
+  <si>
+    <t>Desc: Agura já foi um guerreiro da tribo Wild Horse. Quando ele era jovem, ele morou com seus pais e sua irmã mais nova perto da cidade deserta de Kuquan. Durante uma guerra, a cidade de Kuquan foi atacada por um grupo inimigo, enquanto Agula lutava com outras tropas inimigas na linha de frente. Quando Agula voltou para casa, descobriu que apenas sua irmã havia sobrevivido. Em sua dor, Agula abandonou seu juramento ao Rei Cavalo Selvagem e levou sua irmã para a Cidade das Flores porque ela gostava de flores. Na Cidade das Flores, Agula descobriu que não tinha outras habilidades além da luta, mas não queria ingressar no exército e ficar longe da família. Eventualmente, Agula encontrou seu lugar no torneio local de artes marciais. Ele pensou que a vida iria melhorar a partir de então, mas logo depois, A irmã de Agura ficou gravemente doente e morreu. Devastado, Agula encontrou uma fuga no campo de batalha e se dedicou a buscar o combate definitivo. Tipo: História | Brinquedo.</t>
+  </si>
+  <si>
+    <t>Desc: Khrasisson afirma vir do outro extremo das montanhas, onde uma densa floresta pode ser vista após cruzar perigosas cadeias de montanhas. Depois de caminhar vários dias para o leste, um grande rio pode ser avistado e, do outro lado do rio, fica a vila onde Khrasisson nasceu. Depois de cruzar as montanhas, Khrasisson chegou pela primeira vez à cidade de Spring Valley, onde repeliu mais de vinte bandidos sozinho. Ele então passou por Weeping Spring Town, North Wilderness Village e pelo oásis Wo Lake, e finalmente chegou ao Camel Bell Market. Cada vez que chegava a um novo lugar, Khrasisson deixava sua própria história. No início, os moradores locais não conseguiam se comunicar com Khrasisson devido à barreira do idioma, e muitos pensavam que ele era uma pessoa quieta. Mas agora, nas tabernas do Camel Bell Market, sempre há animação quando Khrasisson está presente. Gosto: Artesanato | História.</t>
+  </si>
+  <si>
+    <t>Desc: Jamilla vem da antiga aristocracia da tribo do Escorpião. Ela e sua irmã, Shariya, receberam desde cedo uma educação de elite dentro da tribo e visitavam frequentemente a tenda do chefe. Seu mentor costumava dizer: "Jamilla é talentosa e inteligente, enquanto Shariya é meticulosa. Quando os dois estão juntos, eles podem exercer sua força máxima". No entanto, as duas irmãs tornaram-se hostis uma com a outra porque ambas se apaixonaram pelo mesmo homem, que mais tarde se tornou o chefe da tribo do Escorpião, Garra Longa. Incapaz de suportar ver o relacionamento de sua irmã com Garra Longa florescer, Jamila finalmente completou uma poção altamente tóxica sob a instigação de Amantha. Qualquer um que tomar esta poção se tornará uma pessoa inútil. O resto da história é bem conhecido. Tipo: misterioso</t>
+  </si>
+  <si>
+    <t>Desc: Jaina era originalmente da Família Dourada, um clã famoso no deserto, mas foi banida porque não herdou o poder mágico para controlar o ouro. Quando era jovem, Jaina aprendeu artes marciais sob a orientação de seu pai. Devido à morte precoce de seus pais, Jaina começou a viver sozinha ainda jovem, praticando habilidades de combate em tavernas e nas ruas. Ela combinou essas habilidades com as artes marciais de seu pai para desenvolver seu próprio estilo e se tornou uma lutadora conhecida. Ela acredita que um dia retornará à Família Dourada para provar sua força. Tipo: Lutando</t>
+  </si>
+  <si>
+    <t>Desc: Outrora uma poderosa feiticeira do StarClan, Zann foi responsável por registrar e testemunhar tudo neste deserto. Ele integrou-se na civilização do deserto, vivenciando inúmeras estações e testemunhando a ascensão e queda de um regime após o outro. Com o passar dos anos, ela ficou muito imersa nos papéis que desempenhava: guerreira, aventureira, curandeira... Quando finalmente recobrou o juízo, descobriu que seus companheiros de clã haviam desaparecido há muito tempo. Tipo: História</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4181,74 +3023,79 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Incorrecto" xfId="1" builtinId="27"/>
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="6" xr:uid="{46E4D6C0-98B6-47F0-ACF7-56160F36CD80}"/>
     <cellStyle name="普通" xfId="2" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="普通 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="普通 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
@@ -4618,11 +3465,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="5" max="5" width="55.375" customWidth="1"/>
     <col min="7" max="7" width="138.125" customWidth="1"/>
@@ -4670,8 +3517,8 @@
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>365</v>
+      <c r="G2" s="14" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="409.5">
@@ -4688,13 +3535,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>367</v>
+      <c r="G3" s="14" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="409.5">
@@ -4711,13 +3558,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>369</v>
+      <c r="G4" s="14" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="409.5">
@@ -4734,13 +3581,13 @@
         <v>24</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>371</v>
+      <c r="G5" s="14" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5">
@@ -4757,13 +3604,13 @@
         <v>29</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>373</v>
+      <c r="G6" s="14" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="409.5">
@@ -4780,13 +3627,13 @@
         <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>375</v>
+      <c r="G7" s="14" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="409.5">
@@ -4803,13 +3650,13 @@
         <v>37</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>377</v>
+      <c r="G8" s="14" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="409.5">
@@ -4826,13 +3673,13 @@
         <v>41</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>379</v>
+      <c r="G9" s="14" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="409.5">
@@ -4849,13 +3696,13 @@
         <v>45</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>381</v>
+      <c r="G10" s="14" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="409.5">
@@ -4872,13 +3719,13 @@
         <v>50</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>382</v>
+      <c r="G11" s="14" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="409.5">
@@ -4895,13 +3742,13 @@
         <v>55</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>385</v>
+      <c r="G12" s="14" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="409.5">
@@ -4918,13 +3765,13 @@
         <v>59</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>387</v>
+      <c r="G13" s="14" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="409.5">
@@ -4941,13 +3788,13 @@
         <v>63</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>389</v>
+      <c r="G14" s="14" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="409.5">
@@ -4964,13 +3811,13 @@
         <v>68</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>391</v>
+      <c r="G15" s="14" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="409.5">
@@ -4987,13 +3834,13 @@
         <v>72</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>392</v>
+        <v>378</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>393</v>
+      <c r="G16" s="14" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="409.5">
@@ -5010,13 +3857,13 @@
         <v>77</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>395</v>
+      <c r="G17" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="409.5">
@@ -5033,13 +3880,13 @@
         <v>82</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>397</v>
+      <c r="G18" s="14" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="409.5">
@@ -5056,13 +3903,13 @@
         <v>86</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>399</v>
+      <c r="G19" s="14" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="409.5">
@@ -5079,13 +3926,13 @@
         <v>90</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>401</v>
+      <c r="G20" s="14" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="409.5">
@@ -5102,13 +3949,13 @@
         <v>94</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="12" t="s">
-        <v>403</v>
+      <c r="G21" s="14" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="409.5">
@@ -5125,13 +3972,13 @@
         <v>99</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>404</v>
+      <c r="G22" s="14" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="409.5">
@@ -5148,13 +3995,13 @@
         <v>103</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>407</v>
+      <c r="G23" s="14" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="409.5">
@@ -5171,13 +4018,13 @@
         <v>107</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G24" s="12" t="s">
-        <v>408</v>
+      <c r="G24" s="14" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="409.5">
@@ -5194,13 +4041,13 @@
         <v>111</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="12" t="s">
-        <v>411</v>
+      <c r="G25" s="14" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="409.5">
@@ -5217,13 +4064,13 @@
         <v>115</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G26" s="12" t="s">
-        <v>413</v>
+      <c r="G26" s="14" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="409.5">
@@ -5240,13 +4087,13 @@
         <v>119</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>415</v>
+      <c r="G27" s="14" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="409.5">
@@ -5263,13 +4110,13 @@
         <v>123</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>531</v>
+        <v>390</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G28" s="12" t="s">
-        <v>416</v>
+      <c r="G28" s="14" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="409.5">
@@ -5286,13 +4133,13 @@
         <v>127</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>417</v>
+        <v>391</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>418</v>
+      <c r="G29" s="14" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="409.5">
@@ -5309,13 +4156,13 @@
         <v>131</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="G30" s="12" t="s">
-        <v>420</v>
+      <c r="G30" s="14" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="409.5">
@@ -5332,13 +4179,13 @@
         <v>135</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>421</v>
+        <v>393</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="G31" s="12" t="s">
-        <v>422</v>
+      <c r="G31" s="14" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="409.5">
@@ -5355,13 +4202,13 @@
         <v>139</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>423</v>
+        <v>394</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G32" s="12" t="s">
-        <v>424</v>
+      <c r="G32" s="14" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="409.5">
@@ -5378,13 +4225,13 @@
         <v>143</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>425</v>
+        <v>395</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>426</v>
+      <c r="G33" s="14" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="409.5">
@@ -5401,13 +4248,13 @@
         <v>147</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="G34" s="12" t="s">
-        <v>428</v>
+      <c r="G34" s="14" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="409.5">
@@ -5424,13 +4271,13 @@
         <v>151</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>429</v>
+        <v>397</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G35" s="12" t="s">
-        <v>430</v>
+      <c r="G35" s="14" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="409.5">
@@ -5447,13 +4294,13 @@
         <v>155</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>432</v>
+      <c r="G36" s="14" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="409.5">
@@ -5470,13 +4317,13 @@
         <v>159</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>433</v>
+        <v>399</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>434</v>
+      <c r="G37" s="14" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="409.5">
@@ -5493,13 +4340,13 @@
         <v>163</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>435</v>
+        <v>400</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="G38" s="12" t="s">
-        <v>436</v>
+      <c r="G38" s="14" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="409.5">
@@ -5516,13 +4363,13 @@
         <v>167</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>437</v>
+        <v>401</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G39" s="12" t="s">
-        <v>438</v>
+      <c r="G39" s="14" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="409.5">
@@ -5539,13 +4386,13 @@
         <v>171</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>439</v>
+        <v>402</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="G40" s="12" t="s">
-        <v>440</v>
+      <c r="G40" s="14" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="409.5">
@@ -5562,13 +4409,13 @@
         <v>176</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>441</v>
+        <v>403</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G41" s="12" t="s">
-        <v>442</v>
+      <c r="G41" s="14" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="409.5">
@@ -5585,13 +4432,13 @@
         <v>180</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>443</v>
+        <v>404</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="G42" s="12" t="s">
-        <v>444</v>
+      <c r="G42" s="14" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="409.5">
@@ -5608,13 +4455,13 @@
         <v>184</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G43" s="12" t="s">
-        <v>446</v>
+      <c r="G43" s="14" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="409.5">
@@ -5631,13 +4478,13 @@
         <v>188</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>447</v>
+        <v>406</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="G44" s="12" t="s">
-        <v>448</v>
+      <c r="G44" s="14" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="409.5">
@@ -5654,13 +4501,13 @@
         <v>192</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>449</v>
+        <v>407</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="G45" s="12" t="s">
-        <v>450</v>
+      <c r="G45" s="14" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="409.5">
@@ -5677,13 +4524,13 @@
         <v>196</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>534</v>
+        <v>408</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="G46" s="12" t="s">
-        <v>535</v>
+      <c r="G46" s="14" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="409.5">
@@ -5700,13 +4547,13 @@
         <v>200</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>451</v>
+        <v>409</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="G47" s="12" t="s">
-        <v>452</v>
+      <c r="G47" s="14" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="409.5">
@@ -5723,13 +4570,13 @@
         <v>204</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>454</v>
+        <v>410</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G48" s="12" t="s">
-        <v>453</v>
+      <c r="G48" s="14" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="409.5">
@@ -5746,13 +4593,13 @@
         <v>208</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="G49" s="12" t="s">
-        <v>460</v>
+      <c r="G49" s="14" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="409.5">
@@ -5769,13 +4616,13 @@
         <v>212</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>456</v>
+        <v>412</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="G50" s="12" t="s">
-        <v>457</v>
+      <c r="G50" s="14" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="409.5">
@@ -5792,13 +4639,13 @@
         <v>216</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>458</v>
+        <v>413</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="G51" s="12" t="s">
-        <v>459</v>
+      <c r="G51" s="14" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="409.5">
@@ -5815,13 +4662,13 @@
         <v>220</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>461</v>
+        <v>414</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="G52" s="12" t="s">
-        <v>462</v>
+      <c r="G52" s="14" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="409.5">
@@ -5838,13 +4685,13 @@
         <v>224</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>463</v>
+        <v>415</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="G53" s="12" t="s">
-        <v>464</v>
+      <c r="G53" s="14" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="409.5">
@@ -5861,13 +4708,13 @@
         <v>228</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>465</v>
+        <v>416</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="G54" s="12" t="s">
-        <v>466</v>
+      <c r="G54" s="14" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="409.5">
@@ -5884,13 +4731,13 @@
         <v>232</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="G55" s="12" t="s">
-        <v>468</v>
+      <c r="G55" s="14" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="409.5">
@@ -5907,13 +4754,13 @@
         <v>237</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>469</v>
+        <v>418</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G56" s="12" t="s">
-        <v>470</v>
+      <c r="G56" s="14" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="409.5">
@@ -5930,13 +4777,13 @@
         <v>241</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>471</v>
+        <v>419</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="G57" s="12" t="s">
-        <v>472</v>
+      <c r="G57" s="14" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="409.5">
@@ -5953,13 +4800,13 @@
         <v>245</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>473</v>
+        <v>420</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="G58" s="12" t="s">
-        <v>474</v>
+      <c r="G58" s="14" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="409.5">
@@ -5976,13 +4823,13 @@
         <v>249</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>475</v>
+        <v>421</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="G59" s="12" t="s">
-        <v>476</v>
+      <c r="G59" s="14" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="409.5">
@@ -5999,13 +4846,13 @@
         <v>253</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>477</v>
+        <v>422</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G60" s="12" t="s">
-        <v>478</v>
+      <c r="G60" s="14" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="409.5">
@@ -6022,13 +4869,13 @@
         <v>257</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>479</v>
+        <v>423</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="G61" s="12" t="s">
-        <v>480</v>
+      <c r="G61" s="14" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="409.5">
@@ -6045,13 +4892,13 @@
         <v>262</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>481</v>
+        <v>424</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G62" s="12" t="s">
-        <v>482</v>
+      <c r="G62" s="14" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="409.5">
@@ -6068,13 +4915,13 @@
         <v>266</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>483</v>
+        <v>425</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="G63" s="12" t="s">
-        <v>484</v>
+      <c r="G63" s="14" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="409.5">
@@ -6091,13 +4938,13 @@
         <v>270</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>485</v>
+        <v>426</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G64" s="12" t="s">
-        <v>486</v>
+      <c r="G64" s="14" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="409.5">
@@ -6114,13 +4961,13 @@
         <v>274</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>487</v>
+        <v>427</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="G65" s="12" t="s">
-        <v>488</v>
+      <c r="G65" s="14" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="409.5">
@@ -6137,13 +4984,13 @@
         <v>278</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>489</v>
+        <v>428</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G66" s="12" t="s">
-        <v>490</v>
+      <c r="G66" s="14" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="409.5">
@@ -6160,13 +5007,13 @@
         <v>282</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>491</v>
+        <v>429</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="G67" s="12" t="s">
-        <v>492</v>
+      <c r="G67" s="14" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="409.5">
@@ -6183,13 +5030,13 @@
         <v>286</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>493</v>
+        <v>430</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="G68" s="12" t="s">
-        <v>494</v>
+      <c r="G68" s="14" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="409.5">
@@ -6206,13 +5053,13 @@
         <v>290</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>495</v>
+        <v>431</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="G69" s="12" t="s">
-        <v>496</v>
+      <c r="G69" s="14" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="409.5">
@@ -6229,13 +5076,13 @@
         <v>294</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>497</v>
+        <v>432</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="G70" s="12" t="s">
-        <v>498</v>
+      <c r="G70" s="14" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="409.5">
@@ -6252,13 +5099,13 @@
         <v>298</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>499</v>
+        <v>433</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="G71" s="12" t="s">
-        <v>500</v>
+      <c r="G71" s="14" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="409.5">
@@ -6275,13 +5122,13 @@
         <v>302</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>501</v>
+        <v>434</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="G72" s="12" t="s">
-        <v>502</v>
+      <c r="G72" s="14" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="409.5">
@@ -6298,13 +5145,13 @@
         <v>306</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>503</v>
+        <v>435</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="G73" s="12" t="s">
-        <v>504</v>
+      <c r="G73" s="14" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="409.5">
@@ -6321,13 +5168,13 @@
         <v>310</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>505</v>
+        <v>436</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="G74" s="12" t="s">
-        <v>506</v>
+      <c r="G74" s="14" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="409.5">
@@ -6344,13 +5191,13 @@
         <v>314</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>507</v>
+        <v>437</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="G75" s="12" t="s">
-        <v>508</v>
+      <c r="G75" s="14" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="409.5">
@@ -6367,13 +5214,13 @@
         <v>318</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>509</v>
+        <v>438</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="G76" s="12" t="s">
-        <v>510</v>
+      <c r="G76" s="14" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="409.5">
@@ -6390,13 +5237,13 @@
         <v>322</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>532</v>
+        <v>439</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="G77" s="12" t="s">
-        <v>533</v>
+      <c r="G77" s="14" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="409.5">
@@ -6413,13 +5260,13 @@
         <v>326</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>511</v>
+        <v>440</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="G78" s="12" t="s">
-        <v>512</v>
+      <c r="G78" s="14" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="409.5">
@@ -6436,13 +5283,13 @@
         <v>330</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>513</v>
+        <v>441</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="G79" s="12" t="s">
-        <v>514</v>
+      <c r="G79" s="14" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="409.5">
@@ -6459,13 +5306,13 @@
         <v>334</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>515</v>
+        <v>442</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="G80" s="12" t="s">
-        <v>516</v>
+      <c r="G80" s="14" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="409.5">
@@ -6482,13 +5329,13 @@
         <v>338</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>517</v>
+        <v>443</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="G81" s="12" t="s">
-        <v>518</v>
+      <c r="G81" s="14" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="409.5">
@@ -6505,13 +5352,13 @@
         <v>342</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>519</v>
+        <v>444</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="G82" s="12" t="s">
-        <v>520</v>
+      <c r="G82" s="14" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="409.5">
@@ -6528,13 +5375,13 @@
         <v>346</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>521</v>
+        <v>445</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="G83" s="12" t="s">
-        <v>522</v>
+      <c r="G83" s="14" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="409.5">
@@ -6551,13 +5398,13 @@
         <v>350</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>523</v>
+        <v>446</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="G84" s="12" t="s">
-        <v>524</v>
+      <c r="G84" s="14" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="409.5">
@@ -6574,13 +5421,13 @@
         <v>354</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>525</v>
+        <v>447</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="G85" s="12" t="s">
-        <v>526</v>
+      <c r="G85" s="14" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="409.5">
@@ -6597,13 +5444,13 @@
         <v>358</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>527</v>
+        <v>448</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="G86" s="12" t="s">
-        <v>528</v>
+      <c r="G86" s="14" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="409.5">
@@ -6620,13 +5467,13 @@
         <v>362</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>529</v>
+        <v>449</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="G87" s="12" t="s">
-        <v>530</v>
+      <c r="G87" s="14" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>